<commit_message>
Day 19 | Day_2
</commit_message>
<xml_diff>
--- a/Batch/19/Day_1.xlsx
+++ b/Batch/19/Day_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29307"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\statistics\Batch\19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C79F646-618C-4C74-A106-6F86D5519415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C2C88E-D1B3-4284-A53B-B242FA5B7F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,10 +359,11 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,7 +418,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,8 +600,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>98599</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -620,7 +620,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -665,8 +665,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>143558</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Ink 9">
@@ -685,7 +685,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Ink 9">
@@ -730,8 +730,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19759</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="17" name="Ink 16">
@@ -750,7 +750,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="17" name="Ink 16">
@@ -795,8 +795,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>27278</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="19" name="Ink 18">
@@ -815,7 +815,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="19" name="Ink 18">
@@ -860,8 +860,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="43" name="Ink 42">
@@ -880,7 +880,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="43" name="Ink 42">
@@ -925,8 +925,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>45278</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="44" name="Ink 43">
@@ -945,7 +945,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="44" name="Ink 43">
@@ -990,8 +990,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Ink 47">
@@ -1010,7 +1010,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Ink 47">
@@ -1055,8 +1055,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>49238</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="49" name="Ink 48">
@@ -1075,7 +1075,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="49" name="Ink 48">
@@ -1120,8 +1120,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>86318</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Ink 61">
@@ -1140,7 +1140,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Ink 61">
@@ -1185,8 +1185,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>68678</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="74" name="Ink 73">
@@ -1205,7 +1205,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="74" name="Ink 73">
@@ -1250,8 +1250,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72319</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="76" name="Ink 75">
@@ -1270,7 +1270,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="76" name="Ink 75">
@@ -1315,8 +1315,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>132194</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Ink 87">
@@ -1335,7 +1335,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Ink 87">
@@ -1380,8 +1380,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>69349</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="115" name="Ink 114">
@@ -1400,7 +1400,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="115" name="Ink 114">
@@ -1445,8 +1445,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>26632</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="143" name="Ink 142">
@@ -1465,7 +1465,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="143" name="Ink 142">
@@ -1510,8 +1510,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133871</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="145" name="Ink 144">
@@ -1530,7 +1530,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="145" name="Ink 144">
@@ -1575,8 +1575,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>68948</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="154" name="Ink 153">
@@ -1595,7 +1595,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="154" name="Ink 153">
@@ -1640,8 +1640,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>6995</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="162" name="Ink 161">
@@ -1660,7 +1660,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="162" name="Ink 161">
@@ -1705,8 +1705,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>29839</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="174" name="Ink 173">
@@ -1725,7 +1725,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="174" name="Ink 173">
@@ -1770,8 +1770,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>155233</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="175" name="Ink 174">
@@ -1790,7 +1790,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="175" name="Ink 174">
@@ -1835,8 +1835,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>156633</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="176" name="Ink 175">
@@ -1855,7 +1855,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="176" name="Ink 175">
@@ -1900,8 +1900,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>133707</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="183" name="Ink 182">
@@ -1920,7 +1920,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="183" name="Ink 182">
@@ -1965,8 +1965,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>125468</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="184" name="Ink 183">
@@ -1985,7 +1985,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="184" name="Ink 183">
@@ -2030,8 +2030,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161272</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="185" name="Ink 184">
@@ -2050,7 +2050,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="185" name="Ink 184">
@@ -2095,8 +2095,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>6995</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="194" name="Ink 193">
@@ -2115,7 +2115,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="194" name="Ink 193">
@@ -2160,8 +2160,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>134435</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="205" name="Ink 204">
@@ -2180,7 +2180,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="205" name="Ink 204">
@@ -2225,8 +2225,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>87472</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="230" name="Ink 229">
@@ -2245,7 +2245,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="230" name="Ink 229">
@@ -2290,8 +2290,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>19874</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="237" name="Ink 236">
@@ -2310,7 +2310,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="237" name="Ink 236">
@@ -2355,8 +2355,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>134476</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="240" name="Ink 239">
@@ -2375,7 +2375,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="240" name="Ink 239">
@@ -2420,8 +2420,8 @@
       <xdr:row>16</xdr:row>
       <xdr:rowOff>176555</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId57">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="245" name="Ink 244">
@@ -2440,7 +2440,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="245" name="Ink 244">
@@ -2485,8 +2485,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>129191</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="246" name="Ink 245">
@@ -2505,7 +2505,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="246" name="Ink 245">
@@ -2550,8 +2550,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>17231</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="270" name="Ink 269">
@@ -2570,7 +2570,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="270" name="Ink 269">
@@ -2615,8 +2615,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>48911</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="271" name="Ink 270">
@@ -2635,7 +2635,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="271" name="Ink 270">
@@ -2680,8 +2680,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>179992</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId65">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="276" name="Ink 275">
@@ -2700,7 +2700,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="276" name="Ink 275">
@@ -2745,8 +2745,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>24309</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId67">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="293" name="Ink 292">
@@ -2765,7 +2765,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="293" name="Ink 292">
@@ -2810,8 +2810,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>179878</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId69">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="298" name="Ink 297">
@@ -2830,7 +2830,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="298" name="Ink 297">
@@ -2875,8 +2875,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>64997</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId71">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="309" name="Ink 308">
@@ -2895,7 +2895,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="309" name="Ink 308">
@@ -2940,8 +2940,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>85877</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId73">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="312" name="Ink 311">
@@ -2960,7 +2960,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="312" name="Ink 311">
@@ -3005,8 +3005,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>26992</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId75">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="318" name="Ink 317">
@@ -3025,7 +3025,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="318" name="Ink 317">
@@ -3070,8 +3070,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>161550</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId77">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="331" name="Ink 330">
@@ -3090,7 +3090,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="331" name="Ink 330">
@@ -3135,8 +3135,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>152632</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId79">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="332" name="Ink 331">
@@ -3155,7 +3155,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="332" name="Ink 331">
@@ -3200,8 +3200,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>753</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId81">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="334" name="Ink 333">
@@ -3220,7 +3220,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="334" name="Ink 333">
@@ -3265,8 +3265,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>154072</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId83">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="335" name="Ink 334">
@@ -3285,7 +3285,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="335" name="Ink 334">
@@ -3330,8 +3330,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>13034</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId85">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="339" name="Ink 338">
@@ -3350,7 +3350,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="339" name="Ink 338">
@@ -3395,8 +3395,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>158073</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId87">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="340" name="Ink 339">
@@ -3415,7 +3415,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="340" name="Ink 339">
@@ -3460,8 +3460,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>168112</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId89">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="341" name="Ink 340">
@@ -3480,7 +3480,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="341" name="Ink 340">
@@ -3525,8 +3525,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>159513</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId91">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="344" name="Ink 343">
@@ -3545,7 +3545,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="344" name="Ink 343">
@@ -3590,8 +3590,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>128512</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId93">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="345" name="Ink 344">
@@ -3610,7 +3610,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="345" name="Ink 344">
@@ -3655,8 +3655,8 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>81671</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId95">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="346" name="Ink 345">
@@ -3675,7 +3675,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="346" name="Ink 345">
@@ -3720,8 +3720,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>146790</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId97">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="347" name="Ink 346">
@@ -3740,7 +3740,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="347" name="Ink 346">
@@ -3785,8 +3785,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>47111</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId99">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="348" name="Ink 347">
@@ -3805,7 +3805,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="348" name="Ink 347">
@@ -3850,8 +3850,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>150873</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId101">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="349" name="Ink 348">
@@ -3870,7 +3870,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="349" name="Ink 348">
@@ -3915,8 +3915,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>11872</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId103">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="350" name="Ink 349">
@@ -3935,7 +3935,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="350" name="Ink 349">
@@ -3980,8 +3980,8 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>13312</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId105">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="351" name="Ink 350">
@@ -4000,7 +4000,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="351" name="Ink 350">
@@ -4045,8 +4045,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>124797</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId107">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="364" name="Ink 363">
@@ -4065,7 +4065,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="364" name="Ink 363">
@@ -4110,8 +4110,8 @@
       <xdr:row>38</xdr:row>
       <xdr:rowOff>29037</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId109">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="365" name="Ink 364">
@@ -4130,7 +4130,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="365" name="Ink 364">
@@ -4175,8 +4175,8 @@
       <xdr:row>42</xdr:row>
       <xdr:rowOff>163874</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId111">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="373" name="Ink 372">
@@ -4195,7 +4195,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="373" name="Ink 372">
@@ -4240,8 +4240,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>143035</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId113">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="374" name="Ink 373">
@@ -4260,7 +4260,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="374" name="Ink 373">
@@ -4305,8 +4305,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>178716</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId115">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="375" name="Ink 374">
@@ -4325,7 +4325,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="375" name="Ink 374">
@@ -4370,8 +4370,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>36679</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId117">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="384" name="Ink 383">
@@ -4390,7 +4390,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="384" name="Ink 383">
@@ -4435,8 +4435,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>57477</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId119">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="397" name="Ink 396">
@@ -4455,7 +4455,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="397" name="Ink 396">
@@ -4500,8 +4500,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>80599</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId121">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="407" name="Ink 406">
@@ -4520,7 +4520,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="407" name="Ink 406">
@@ -4565,8 +4565,8 @@
       <xdr:row>45</xdr:row>
       <xdr:rowOff>75117</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId123">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="417" name="Ink 416">
@@ -4585,7 +4585,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="417" name="Ink 416">
@@ -4630,8 +4630,8 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>97273</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId125">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="418" name="Ink 417">
@@ -4650,7 +4650,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="418" name="Ink 417">
@@ -4695,8 +4695,8 @@
       <xdr:row>51</xdr:row>
       <xdr:rowOff>434</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId127">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="430" name="Ink 429">
@@ -4715,7 +4715,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="430" name="Ink 429">
@@ -4760,8 +4760,8 @@
       <xdr:row>50</xdr:row>
       <xdr:rowOff>173275</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId129">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="431" name="Ink 430">
@@ -4780,7 +4780,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="431" name="Ink 430">
@@ -4825,8 +4825,8 @@
       <xdr:row>50</xdr:row>
       <xdr:rowOff>46195</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId131">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="445" name="Ink 444">
@@ -4845,7 +4845,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="445" name="Ink 444">
@@ -4890,8 +4890,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>113678</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId133">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="461" name="Ink 460">
@@ -4910,7 +4910,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="461" name="Ink 460">
@@ -4955,8 +4955,8 @@
       <xdr:row>59</xdr:row>
       <xdr:rowOff>51594</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId135">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="465" name="Ink 464">
@@ -4975,7 +4975,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="465" name="Ink 464">
@@ -5020,8 +5020,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>70077</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId137">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="466" name="Ink 465">
@@ -5040,7 +5040,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="466" name="Ink 465">
@@ -5085,8 +5085,8 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>86195</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId139">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="471" name="Ink 470">
@@ -5105,7 +5105,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="471" name="Ink 470">
@@ -5150,8 +5150,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>86236</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId141">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="472" name="Ink 471">
@@ -5170,7 +5170,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="472" name="Ink 471">
@@ -5215,8 +5215,8 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>9237</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId143">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="486" name="Ink 485">
@@ -5235,7 +5235,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="486" name="Ink 485">
@@ -5280,8 +5280,8 @@
       <xdr:row>54</xdr:row>
       <xdr:rowOff>62959</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId145">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="487" name="Ink 486">
@@ -5300,7 +5300,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="487" name="Ink 486">
@@ -5345,8 +5345,8 @@
       <xdr:row>63</xdr:row>
       <xdr:rowOff>170951</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId147">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="497" name="Ink 496">
@@ -5365,7 +5365,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="497" name="Ink 496">
@@ -5410,8 +5410,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>120952</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId149">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="503" name="Ink 502">
@@ -5430,7 +5430,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="503" name="Ink 502">
@@ -5475,8 +5475,8 @@
       <xdr:row>59</xdr:row>
       <xdr:rowOff>152034</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId151">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="515" name="Ink 514">
@@ -5495,7 +5495,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="515" name="Ink 514">
@@ -5540,8 +5540,8 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId153">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="518" name="Ink 517">
@@ -5560,7 +5560,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="518" name="Ink 517">
@@ -5605,8 +5605,8 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId155">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="523" name="Ink 522">
@@ -5625,7 +5625,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="523" name="Ink 522">
@@ -5670,8 +5670,8 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>142118</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId157">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="541" name="Ink 540">
@@ -5690,7 +5690,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="541" name="Ink 540">
@@ -5735,8 +5735,8 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>153998</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId159">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="542" name="Ink 541">
@@ -5755,7 +5755,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="542" name="Ink 541">
@@ -5800,8 +5800,8 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>152558</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId161">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="547" name="Ink 546">
@@ -5820,7 +5820,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="547" name="Ink 546">
@@ -5865,8 +5865,8 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>6995</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId163">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="552" name="Ink 551">
@@ -5885,7 +5885,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="552" name="Ink 551">
@@ -5930,8 +5930,8 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>181194</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId165">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="563" name="Ink 562">
@@ -5950,7 +5950,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="563" name="Ink 562">
@@ -5995,8 +5995,8 @@
       <xdr:row>71</xdr:row>
       <xdr:rowOff>19194</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId167">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="564" name="Ink 563">
@@ -6015,7 +6015,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="564" name="Ink 563">
@@ -6060,8 +6060,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>107959</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId169">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="573" name="Ink 572">
@@ -6080,7 +6080,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="573" name="Ink 572">
@@ -6125,8 +6125,8 @@
       <xdr:row>66</xdr:row>
       <xdr:rowOff>9679</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId171">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="577" name="Ink 576">
@@ -6145,7 +6145,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="577" name="Ink 576">
@@ -6190,8 +6190,8 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>56953</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId173">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="591" name="Ink 590">
@@ -6210,7 +6210,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="591" name="Ink 590">
@@ -6255,8 +6255,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>52151</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId175">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="602" name="Ink 601">
@@ -6275,7 +6275,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="602" name="Ink 601">
@@ -6320,8 +6320,8 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>38471</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId177">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="616" name="Ink 615">
@@ -6340,7 +6340,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="616" name="Ink 615">
@@ -6385,8 +6385,8 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>105668</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId179">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="652" name="Ink 651">
@@ -6405,7 +6405,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="652" name="Ink 651">
@@ -6450,8 +6450,8 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>75706</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId181">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="668" name="Ink 667">
@@ -6470,7 +6470,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="668" name="Ink 667">
@@ -6515,8 +6515,8 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>9826</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId183">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="669" name="Ink 668">
@@ -6535,7 +6535,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="669" name="Ink 668">
@@ -6580,8 +6580,8 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>148549</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId185">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="681" name="Ink 680">
@@ -6600,7 +6600,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="681" name="Ink 680">
@@ -6645,8 +6645,8 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>133347</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId187">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="682" name="Ink 681">
@@ -6665,7 +6665,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="682" name="Ink 681">
@@ -6710,8 +6710,8 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>136309</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId189">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="683" name="Ink 682">
@@ -6730,7 +6730,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="683" name="Ink 682">
@@ -6775,8 +6775,8 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>93747</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId191">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="703" name="Ink 702">
@@ -6795,7 +6795,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="703" name="Ink 702">
@@ -6883,7 +6883,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 119 15639,'0'0'7742,"26"0"-6149,291 12-80,-342-27-1476,11 4-116,0 1 1,-1 1-1,0 0 0,0 1 1,-1 1-1,0 0 0,-19-5 1,45 27-287,12 5 388,3-8 22,0-2-1,0 0 1,41 9 0,-38-11-37,-27-7-14,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 2 0,-5 5 5,0 0-1,-1 0 1,1-1 0,-2 0 0,1-1-1,-1 1 1,0-1 0,0-1-1,-1 0 1,-16 8 0,4-1-260,-19 12-955,-21 13-5673,35-22-536</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2178.29">884 197 18296,'0'0'8631,"-2"-3"-8346,2 2-283,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0 0 0,-1-1 1,1 1-1,0-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1 0 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 1,-1 1-1,-7 22-86,7-21 84,-10 26 14,1 1 0,2 0 0,1 0 0,0 1 0,-3 57-1,6-87 54,-1-1-1,1 1 0,-1-1 0,0 1 0,1-1 1,-8-3-1,6 1-179,-38-19-1352,42 20 1064,0 1-1,0-1 0,1 0 1,-1 0-1,0 1 1,1-1-1,0 0 0,-1 0 1,1 0-1,0-1 0,-1-2 1,-3-18-5121</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2334.76">933 16 15335,'0'0'8052,"39"-16"-8356,-21 30-993,-4 5-2033,0-1-2624</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2334.75">933 16 15335,'0'0'8052,"39"-16"-8356,-21 30-993,-4 5-2033,0-1-2624</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2725.74">1245 133 16424,'0'0'7760,"-12"-1"-7562,5 0-182,1 1 0,-1-1 0,1 2-1,-1-1 1,1 1 0,-1 0 0,1 0 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 1-1,0 0 1,1 0 0,-1 0 0,1 1 0,-1 0 0,1 0 0,0 0 0,1 1 0,-1-1 0,1 1-1,-6 8 1,8-9-16,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,2 7 0,0-7-8,0-1-1,0 0 1,0 1-1,0-1 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1 0,1-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,5 1-1,-45 1 881,6-4-4265,29-11-8925</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3054.75">1372 224 16151,'0'0'5032,"-8"12"-4621,-25 37-235,32-48-172,0-1-1,1 1 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1 0-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 1-1,0 0 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,2 0 1,5 1 1,1 0 1,-1 0 0,0-1-1,16-2 1,-19 1 12,-1 1 40,0 0 0,1 0-1,-1-1 1,0 1 0,0-1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0-1 0,0 0-1,-1 0 1,1 0 0,-1-1 0,0 1-1,0-1 1,1 0 0,-2 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,0-1 0,-1-3-1,1 6-26,-1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,-2-1 1,-1 1-138,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 1,0 1-1,-6 1 0,7-1-68,4 0 160,-3-1-438,1 1 1,-1 0-1,0 0 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 1-1,1 0 1,-1 0 0,-2 1-1,-3 6-5064</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3458.23">1661 174 12534,'0'0'10533,"-6"11"-9989,-55 89 149,61-100-688,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 1,0 1-1,24-11 39,24-16-116,-22 13-64,-18 10 51,0-1 0,0-1-1,-1 1 1,0-1-1,0 0 1,10-10 0,-16 15 224,-1 2-112,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,2 3 0,1-2 35,-1 0 1,0-1-1,1 1 1,-1-1-1,1 1 0,0-2 1,-1 1-1,1 0 1,5-1-1,5 0-671,0 0-1,0-2 1,0 0 0,29-7-1,-7-3-5189</inkml:trace>
@@ -6986,7 +6986,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">153 5 12054,'0'0'6773,"0"-4"-6023,0 6-595,-57 264 2707,51-229-2604,1-10 207,-1 52 2654,28-79-3066,4 0-26,354 14-54,-355-10 102,-25-4-51,0-4-46,-1-1 0,1 1 0,-1-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 1 0,0-1 0,-4-4 0,-40-44-97,22 26 31,24 26 84,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,0 0 0,0 0 0,0 0 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 1 1,-1 13-91,11 21 0,-2-27 87,1 0 0,0-1-1,1 0 1,-1 0 0,1-1 0,1 0 0,-1-1 0,1 0 0,0-1 0,0 0 0,0 0 0,16 2-1,-12-2 31,-14-4-22,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,-1 1 0,0 0 0,-19 27 69,19-27-59,-25 32-141,-66 88 365,35-39-3117,35-47-2974,0-8-5005</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2301.26">1057 216 8196,'0'0'11624,"1"-5"-10117,1-26 2068,-6 32-3557,0-1 0,0 2-1,0-1 1,1 0 0,-1 1-1,0 0 1,0-1 0,1 1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 1-1,0 0 1,1 0 0,-1 0 0,-3 6-1,-5 6 1,1-1 0,-13 30 1,14-25 8,0 1 0,-8 32 0,15-44-31,0 0-1,1 0 0,0 0 0,0 0 1,1 0-1,0 0 0,0 1 1,1-1-1,2 15 0,-1-20 5,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,0-2-1,0 1 0,1 0 1,-1 0-1,0-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0 0 1,5-5-1,5-5-1,-1 0 1,-1-1 0,0 0-1,0-1 1,-1 0-1,8-16 1,-15 23-39,1 0 0,-1 0 1,0 0-1,-1 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0-1 1,-1 1-1,0-1 0,0 0 0,0 1 1,-1-1-1,0 0 0,-3-7 0,3 11 22,0 0-1,-1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,-1 0 0,0 0 0,0 1 1,1-1-1,-1 1 0,-1-1 0,1 1 1,-6-3-1,2 2-8,0 0 0,0 1-1,-1-1 1,1 2 0,-1-1 0,1 1-1,-1 0 1,-9 0 0,5 1 11,0 0 0,0 1 1,-1 1-1,1 0 0,0 0 0,0 1 1,1 1-1,-1 0 0,1 0 1,-17 10-1,25-13-5,0 1 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,1 1 1,-1 5-1,1-6-26,1 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,1 0 1,-1 1-1,1-1 1,-1-1-1,1 1 1,0 0 0,0 0-1,0-1 1,0 1-1,1-1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,0-1 1,5 3 0,33 16-53,-24-12 85,-1 1 0,1 0 1,25 19-1,-38-24 19,1 1-1,-1-1 1,0 1 0,0-1 0,0 1-1,0 1 1,-1-1 0,0 0 0,0 1-1,0-1 1,-1 1 0,0 0 0,0 0-1,-1 0 1,2 8 0,0 20-226,-2 59-1,-1-49-7074,0-32-1956</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2301.25">1057 216 8196,'0'0'11624,"1"-5"-10117,1-26 2068,-6 32-3557,0-1 0,0 2-1,0-1 1,1 0 0,-1 1-1,0 0 1,0-1 0,1 1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 1-1,0 0 1,1 0 0,-1 0 0,-3 6-1,-5 6 1,1-1 0,-13 30 1,14-25 8,0 1 0,-8 32 0,15-44-31,0 0-1,1 0 0,0 0 0,0 0 1,1 0-1,0 0 0,0 1 1,1-1-1,2 15 0,-1-20 5,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,0-2-1,0 1 0,1 0 1,-1 0-1,0-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0 0 1,5-5-1,5-5-1,-1 0 1,-1-1 0,0 0-1,0-1 1,-1 0-1,8-16 1,-15 23-39,1 0 0,-1 0 1,0 0-1,-1 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0-1 1,-1 1-1,0-1 0,0 0 0,0 1 1,-1-1-1,0 0 0,-3-7 0,3 11 22,0 0-1,-1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,-1 0 0,0 0 0,0 1 1,1-1-1,-1 1 0,-1-1 0,1 1 1,-6-3-1,2 2-8,0 0 0,0 1-1,-1-1 1,1 2 0,-1-1 0,1 1-1,-1 0 1,-9 0 0,5 1 11,0 0 0,0 1 1,-1 1-1,1 0 0,0 0 0,0 1 1,1 1-1,-1 0 0,1 0 1,-17 10-1,25-13-5,0 1 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 0,1 1 1,-1 5-1,1-6-26,1 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,1 0 1,-1 1-1,1-1 1,-1-1-1,1 1 1,0 0 0,0 0-1,0-1 1,0 1-1,1-1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,0-1 1,5 3 0,33 16-53,-24-12 85,-1 1 0,1 0 1,25 19-1,-38-24 19,1 1-1,-1-1 1,0 1 0,0-1 0,0 1-1,0 1 1,-1-1 0,0 0 0,0 1-1,0-1 1,-1 1 0,0 0 0,0 0-1,-1 0 1,2 8 0,0 20-226,-2 59-1,-1-49-7074,0-32-1956</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2692.1">1226 496 5106,'0'0'17128,"3"5"-17323,-2 6 172,14 57 84,-15-65-58,1 0 0,0 1 1,0-2-1,0 1 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0-1 1,0 0-1,1 1 0,-1-1 0,0 0 0,1 0 1,0 0-1,3 1 0,-4-2 37,0-1-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0-1 1,0 1-1,-1-1 1,1 0 0,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,0 1-1,0-1 1,1 1-1,0-2 1,29-52 1041,-23 40-941,2-18 879,-7 22-2281,6 25-14846</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3570.65">1528 530 10453,'0'0'12128,"-2"-12"-11176,-9-38-375,11 49-569,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1-1,0-1 1,1 1 0,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,-1 1 0,-23 15-170,21-10 166,1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,2 1 0,-1-1 0,0 1-1,1 0 1,1-1 0,-1 1 0,1 10 0,0-16-20,1-1-1,-1 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,1-1-1,16-8-72,-12 4 134,1 0 1,-1 0-1,-1 0 0,1 0 1,-1-1-1,0 0 0,0 0 1,-1 0-1,0 0 0,4-9 1,-7 15-5,0 21-847,0-18 811,1 0 1,-1 0-1,1 1 1,0-1 0,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0 0,0 0-1,-1-1 1,1 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,1-1-1,-1 0 1,0 1-1,0-1 1,0-1 0,1 1-1,-1 0 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,-1 0 1,1 1-1,3-4 1,1-2-64,0-1 0,0 0 0,-1-1 0,0 1 0,-1-1 1,0 0-1,0-1 0,-1 1 0,0-1 0,-1 0 0,0 0 0,2-14 1,0-10-503,-2 0 1,-1-49-1,-6 66 917,-4 18-105,6 1-265,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1 3-1,-2 18 115,0 1 0,0 29 0,3-44-90,1 0-1,1 0 1,-1 0 0,1 0 0,1 0 0,-1 0 0,2 0-1,5 16 1,-7-23-11,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 1,1 1-1,-1-1 1,0 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,-1 1 1,1 0-1,0-1 1,0 0-1,0 1 1,-1-1-1,3 0 1,0 0 22,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,4-4 0,0 0 45,-1 0 0,0 0 0,-1-1 0,0 1 0,0-1-1,0 0 1,-1 0 0,0-1 0,0 0 0,4-12 0,-8 33 272,-1-1-270,1 0 1,0-1-1,1 1 0,1 0 0,3 16 0,-4-26-61,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,2-1 0,22-10-1673,-10-7-3610,-15 6-679</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3757.79">1908 209 17528,'0'0'4082,"-4"6"-7444,4 3-1776</inkml:trace>
@@ -7039,28 +7039,28 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 785 12998,'0'0'8692,"67"-4"-5459,4 4-2658,278 12 56,-277-10-335,-71-2-229,24 0 181,-11-2-245,0-2 0,0 1 0,0-2 0,-1 0 0,0 0 0,0-1 0,17-11 0,-6 5-3,42-25 33,70-51 1,-84 52-1,2 2 0,83-39 0,-137 73-33,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1-1 0,-1 1 1,0-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1-2 1,-15-6-32,-3-1 44,-7-8 31,21 13-40,-1 0-1,0 0 1,0 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 1-1,-7-2 1,12 4-23,6 0-207,0 0 197,0 1 0,0 0 0,-1-1 1,1 2-1,-1-1 0,1 0 0,-1 1 0,1 0 0,5 3 1,12 4 38,-4-4 4,33 12 33,-49-16-52,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,0-1 0,1 1-1,-1 4 1,0-2 2,0 1 0,0-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-3 4 0,-4 2-81,1-1 0,-2 1 0,-12 9 0,9-8-392,-13 12-1478,10-5-2676,12-11-1552</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="711.95">1616 229 7251,'0'0'12073,"-8"1"-11847,4-1-192,0 1 0,1 0 1,-1-1-1,0 1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,1-1 0,-1 0 1,1 1-1,-2 4 0,-1 1 229,1 1 0,-1 0 0,2 0 0,-1 0 0,0 15 0,3-24-246,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,1-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,0 0 0,0-1 0,-1 1 0,1-1-1,0 0 1,0 1 0,1-1 0,-1 0 0,0 1 0,0-1-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 1 0,-1-2 0,3 1-1,5 0 96,0 0 0,-1-1 0,1-1 0,0 1 0,0-1-1,-1-1 1,1 1 0,-1-2 0,0 1 0,0-1 0,0 0-1,-1-1 1,1 1 0,-1-2 0,0 1 0,0-1 0,-1 0-1,8-9 1,-9 9-70,0 0 1,-1 0-1,1 0 0,-1 0 0,-1-1 0,1 0 0,-1 1 1,0-1-1,-1 0 0,0-1 0,0 1 0,0 0 0,-1-1 1,0 1-1,0-1 0,-1 1 0,0-1 0,-1 1 0,1-1 1,-1 1-1,-1-1 0,-2-9 0,2 13-39,-1 0 0,1-1 0,0 1-1,-1 0 1,0 1 0,0-1 0,0 0 0,-1 1 0,1 0-1,-1-1 1,0 2 0,1-1 0,-2 0 0,1 1 0,0-1-1,0 1 1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1 0-1,0 0 1,1 0 0,-1 1 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 1 0,-6 1 0,3-1-12,1 0 0,0 0 0,0 1 0,0 0 0,0 0 0,0 1 0,0 0 0,1 0 1,-1 0-1,1 1 0,0 0 0,0 1 0,0-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,-5 9 0,9-12 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0 0 0,1 0 0,0 0 0,-1-1-1,1 1 1,0 0 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,1-1 0,1 2 0,4 3-6,1-1 0,-1 1-1,1-1 1,17 7 0,15 11 107,-33-17-76,0 0 0,0 1 0,-1 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,-1 0 0,1 1 0,-1 0 0,-1-1 0,0 1 0,2 10 0,-1-2-81,-1 0 1,-1 1-1,0-1 0,-2 1 0,0 0 0,-3 20 0,0-25-1264,1-5-1031,1-1-3499</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1073.34">1853 293 7924,'0'0'12715,"0"49"-11309,0 45-742,0-93-631,1-1 0,-1 1-1,1-1 1,-1 1 0,0-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,0 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0-2-1,28-13 946,-24 8-948,0 1 0,0 0 0,-1-1 0,0 0 0,0 0 0,-1-1 0,0 1-1,0 0 1,0-1 0,-1 0 0,0 0 0,-1 0 0,1-9 0,-2 15-428,12 3-10900,1 2 4524</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1073.33">1853 293 7924,'0'0'12715,"0"49"-11309,0 45-742,0-93-631,1-1 0,-1 1-1,1-1 1,-1 1 0,0-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,0 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,0-2-1,28-13 946,-24 8-948,0 1 0,0 0 0,-1-1 0,0 0 0,0 0 0,-1-1 0,0 1-1,0 0 1,0-1 0,-1 0 0,0 0 0,-1 0 0,1-9 0,-2 15-428,12 3-10900,1 2 4524</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2479.5">2138 284 6675,'0'0'12422,"-2"-9"-11003,-7-28-568,8 37-833,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-2 1 0,-21 18 282,14-9-161,0 0 1,1 0 0,-11 20 0,16-26-112,1-1 0,0 1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,1 9 0,0-12-28,0 0 0,-1-1 0,1 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,1 0-1,-1-1 0,0 1 0,0 0 0,1-1 0,33-7-23,-30 5-16,0 0-1,-1 0 0,1-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,-1-1-1,1 1 1,5-10-1,-8 13 243,-1 42-411,-1-39 221,1 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,1 1 0,0-1 1,-1 1-1,1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,0-1-1,1 1 0,-1 0 0,1-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,1-1-1,4-1 12,-1 1 0,0-1 0,0 0 1,0-1-1,0 0 0,0 0 0,-1 0 0,1 0 0,8-8 1,-5 2-54,-1 1 0,0-2 1,0 1-1,-1-1 0,0 0 0,-1-1 1,0 0-1,0 0 0,-2 0 1,7-20-1,-5 8-152,-1 0-1,-2 0 1,0-1 0,-1-37 0,-2 61 185,1 0 1,-1 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,-1 0-1,-11 9 90,-9 19-50,14-11 32,0 0 0,1 0 0,1 1 1,0 0-1,2 0 0,0 0 0,1 0 0,0 1 0,3 31 0,-1-47-74,0-1 1,1 1-1,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,1-1 1,-1 0-1,0 0 0,1 0 0,-1 1 1,1-1-1,-1-1 0,1 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1-1-1,1 0 0,-1 0 0,1 0 1,0 0-1,3 0 0,0 0 17,0-1 0,0 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,0-1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 0 1,0-1-1,8-6 0,-9 6 6,-2 2 5,1-1 0,0 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,2-6 0,-3 8-20,0 37-331,0-34 327,-1-1 0,1 0 0,0 1 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,3 0 1,-1 0-1,0 0 1,0 0-1,1-1 1,-1 0-1,0 0 0,7-1 1,-4 1 24,-1-1-29,0-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,0-1 0,0 0 0,0 0 1,0-1-1,-1 1 0,0-1 0,0 0 1,0-1-1,0 1 0,0-1 0,-1 0 1,0 0-1,0 0 0,0-1 0,4-10 0,2-3-18,0 0-1,-2 0 0,-1-1 0,0 0 1,5-24-1,-9 24-149,-1 0-1,1-38 1,-20 97 77,11-21 170,1 0 1,1 0 0,1 0-1,1 1 1,0-1 0,1 1 0,2 22-1,0-38-79,-1-1-1,0 1 1,1-1-1,-1 1 1,1-1-1,0 1 0,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,3 1-1,-1-1-3,0-1 0,0 1 0,0-1-1,0 1 1,1-1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,1 0 0,7-1 0,-7 1-2,1-1 1,0 0 0,0 0 0,0 0-1,-1-1 1,1 0 0,-1 0 0,1 0 0,-1-1-1,0 1 1,0-1 0,0-1 0,0 1-1,0-1 1,-1 0 0,0 0 0,0 0-1,0 0 1,4-6 0,-5 2 48,0-1 0,-1 1 0,1-1 1,-2 0-1,1 0 0,-1 0 0,0 0 0,-1 0 0,-1-11 1,1 7 267,-2 35-235,2-19-91,-1 1 0,1 0 0,0 0-1,0 0 1,0 0 0,1 0 0,1 6-1,-2-8-5,1-1-1,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 1,0-1-1,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 1 1,3-1-1,-2 0-19,1 1-1,0-1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,-1-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0-1,1 0 1,-1-1 0,0 1 0,0 0 0,1-1 0,-1 0-1,0 1 1,2-4 0,-1 1 101,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0-1-1,0 1 1,-1 0 0,0-1-1,0-7 1,-1 22-123,0 0 1,-1 0-1,0 0 1,-6 14-1,-5 25 112,9-9-13,2 0-1,4 60 1,0-56 7,-6 76 0,4-117-44,-1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-5-1 0,1 2-60,1-1-1,-1-1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,0 0-1,1-1 0,0 0 1,-1 0-1,1 0 1,-9-7-1,-10-16-2905,3-7-1836</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2633.73">2744 116 17032,'0'0'1248,"78"-10"-1728,-57 8-3698</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2806.73">2661 0 16680,'0'0'3025,"-53"55"-13574</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3917.15">591 790 8516,'0'0'12342,"4"27"-10763,5-11-1387,0-1 1,0 0-1,1-1 1,1 0-1,1-1 1,0 0-1,0-1 1,15 12-1,14 14 48,32 33-63,105 77 0,-177-147-174,1 0 1,-1 0-1,1 0 0,0 1 0,0-1 0,0-1 0,-1 1 1,1 0-1,0 0 0,0-1 0,0 1 0,2-1 0,-3 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,0-1-1,0-2 7,1-1-1,-1 1 1,0-1-1,0 0 1,0 0-1,-1 0 1,0 0-1,0-6 0,0-4 2,0-28 63,0 41-69,0 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 1,-1 0-1,-2-3 0,4 5-1,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 2 0,0 28-49,0-25 65,0 0-24,1 1-1,0-1 1,-1 0-1,2 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,2 1 1,3 4-1,18 29-26,-25-37 28,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,0 0 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1 0,0 1-1,0-1 1,0 1 0,-1 0-1,-36 18-423,25-13-255,-18 7-2145,-1-2-2081</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5060.62">1528 1103 13574,'0'0'9493,"0"-6"-8829,-3-20-144,3 20 128,-4 24-279,-2 20 148,-6 35 54,-5 127 0,16-188-1148,0 28 504,5-23-3285,5-9-4898,1-7-2085</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5542.66">1538 1120 15575,'0'0'8356,"12"-6"-8295,-1 0-61,1 1-1,-1 0 0,1 1 0,0 0 1,24-3-1,-34 6-2,0 1-1,0-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 1 1,0-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,1 0 1,-1 0 0,0 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 1-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 1-1,-1-1 1,1 0-1,-1 0 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,-1-1 0,1 0-1,-1 3 1,0-1 86,0 0 1,0 0 0,0 0-1,-1-1 1,1 1-1,-1 0 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 0-1,-1 0 1,0 0-1,1 0 1,-5 3-1,-58 41 682,21-16-692,37-26-67,4-4-14,0 1-1,1 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1-1,0 1 1,0 2 0,2-4-144,18-1-1163,4 0 1225,-14-1 26,-1 1 1,1 0-1,-1 0 1,1 1-1,0 0 1,13 4-1,-18-4 41,-1 0-1,0 1 0,1-1 1,-1 1-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 1 0,0-1 1,-1 0-1,1 0 0,-1 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,-1 0 0,1 3 1,0-2 31,0-1 1,-1 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,-1-1 0,0 1-1,0-1 1,-4 6-1,2-5 85,-1 0 0,0-1 0,1 0 0,-1 1 0,0-2-1,-1 1 1,1-1 0,0 1 0,-1-1 0,0-1-1,1 1 1,-12 1 0,14-3-257,-30 5 808,32-5-776,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,-1-2 0,2-14-5287</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6491.47">1789 1361 15367,'0'0'3500,"16"-3"-2683,52-10-438,-65 12-350,1 1 1,0-1 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,0-1 0,0 0-1,6-5 1,-7 6-7,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-2-2 0,1 3-12,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,-1 0 0,-28-3 536,25 3-487,0 0-1,0 1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,-6 4 1,7-2-30,0-1 0,1 1 0,-1 1 0,1-1 0,-1 0 0,2 1 0,-1 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1-1,1-1 1,1 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,2 10 0,-2-13-26,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,3 1 0,47 2 100,-40-4-64,-1 1-37,0-1 1,0 0-1,0 0 0,0-1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 1,-1-1-1,1-1 0,-1 1 0,0-1 0,0 0 0,-1-1 0,0 0 0,0 0 1,0-1-1,-1 0 0,6-9 0,-3 2 5,0 0 0,-1-1-1,-1 0 1,-1-1 0,0 1 0,-1-1 0,0 0 0,-2-1-1,0 1 1,-1-1 0,0-22 0,-3 54-41,-1 0 1,0-1-1,-1 1 1,-8 23-1,6-24 69,1 1 0,1 0 0,0 0-1,-2 27 1,5-26 34,-1-12-73,1 0-1,0 1 1,0-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,1 6 0,-1-8 1,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,1-2 0,15-5 68,0-1 0,22-14 1,-25 14 50,0 0 0,0 0 0,29-9 0,-42 17-62,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 2 1,6 31-23,-4-21 185,-1-7-218,0-1 0,0 0 0,0 0 0,0-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,0 0 0,5 5 0,-4-6-223,1 0 1,0 0-1,0 0 0,0-1 1,0 0-1,1 0 0,-1 0 1,0-1-1,0 1 1,0-1-1,7-1 0,-6 1-337,0-1 0,0 0 0,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,1-1 0,-2 0 0,1 1 0,0-2-1,-1 1 1,5-5 0,-5 4 239,-1 1 0,1-1 0,-1-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,0-1 0,3-10 0,-4 11 787,-1 1 1,1-1-1,-1 1 1,0-1 0,0 0-1,0 1 1,-1-1 0,-1-5-1,2 9-318,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-2 0-1,-21 11 654,18-7-697,0 1 1,0 0-1,0 0 1,1 0 0,0 0-1,0 1 1,0 0-1,1-1 1,0 1 0,0 0-1,1 1 1,0-1-1,0 0 1,0 14-1,2-20-92,1-1-1,0 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,1 0 0,13-1 1937,-1 34-1802,-13-29-252,-1 0 0,1-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,1 1 0,-1 0-1,1-1 1,0 1 0,2 2-1,-2-4-418,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,2 0 0,7 0-6345</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6491.46">1789 1361 15367,'0'0'3500,"16"-3"-2683,52-10-438,-65 12-350,1 1 1,0-1 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,0-1 0,0 0-1,6-5 1,-7 6-7,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-2-2 0,1 3-12,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,-1 0 0,-28-3 536,25 3-487,0 0-1,0 1 1,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,0 0-1,-6 4 1,7-2-30,0-1 0,1 1 0,-1 1 0,1-1 0,-1 0 0,2 1 0,-1 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1-1,1-1 1,1 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,2 10 0,-2-13-26,1-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 0,3 1 0,47 2 100,-40-4-64,-1 1-37,0-1 1,0 0-1,0 0 0,0-1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 1,-1-1-1,1-1 0,-1 1 0,0-1 0,0 0 0,-1-1 0,0 0 0,0 0 1,0-1-1,-1 0 0,6-9 0,-3 2 5,0 0 0,-1-1-1,-1 0 1,-1-1 0,0 1 0,-1-1 0,0 0 0,-2-1-1,0 1 1,-1-1 0,0-22 0,-3 54-41,-1 0 1,0-1-1,-1 1 1,-8 23-1,6-24 69,1 1 0,1 0 0,0 0-1,-2 27 1,5-26 34,-1-12-73,1 0-1,0 1 1,0-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,1 6 0,-1-8 1,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,1-2 0,15-5 68,0-1 0,22-14 1,-25 14 50,0 0 0,0 0 0,29-9 0,-42 17-62,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 2 1,6 31-23,-4-21 185,-1-7-218,0-1 0,0 0 0,0 0 0,0-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,0 0 0,5 5 0,-4-6-223,1 0 1,0 0-1,0 0 0,0-1 1,0 0-1,1 0 0,-1 0 1,0-1-1,0 1 1,0-1-1,7-1 0,-6 1-337,0-1 0,0 0 0,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,1-1 0,-2 0 0,1 1 0,0-2-1,-1 1 1,5-5 0,-5 4 239,-1 1 0,1-1 0,-1-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,0-1 0,3-10 0,-4 11 787,-1 1 1,1-1-1,-1 1 1,0-1 0,0 0-1,0 1 1,-1-1 0,-1-5-1,2 9-318,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-2 0-1,-21 11 654,18-7-697,0 1 1,0 0-1,0 0 1,1 0 0,0 0-1,0 1 1,0 0-1,1-1 1,0 1 0,0 0-1,1 1 1,0-1-1,0 0 1,0 14-1,2-20-92,1-1-1,0 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,1 0 0,13-1 1937,-1 34-1802,-13-29-252,-1 0 0,1-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,1 1 0,-1 0-1,1-1 1,0 1 0,2 2-1,-2-4-418,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,2 0 0,7 0-6345</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6667.48">2584 1323 14006,'0'0'6403,"18"51"-6243,-7-39-64,-1-4-96,5-4-848,6-4-1441,-3 0 128,3-2-2753,-3-12-433</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6855.23">2765 1304 5507,'0'0'16887,"-25"-9"-16567,4 28 225,0 3-257,3 2-144,4 1-128,0-1 0,7-2-32,0-2-304,7-7-1649,0-5-1633</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7042.89">2850 1295 16696,'0'0'6387,"-7"68"-6195,7-51-80,0-3-112,0-4 0,0-2-497</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7300.91">3009 1168 17624,'0'0'6707,"-8"13"-6043,6-8-618,-5 7 131,1 0 0,0 1 0,1-1 0,0 1 0,1 0 0,1 0 0,0 0 0,-2 22 0,5-24-236,1 5-1257,8-13-8736</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7862.78">3088 1200 6723,'0'0'18315,"-3"-6"-18003,1 3-291,-9-16-10,4 21-40,1 14 26,0 5 35,3-16-14,1 1 0,0 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,1 1 1,-1-1-1,3 10 0,-2-15-24,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 1 0,1-2 0,0 1-1,-1 0 1,1 0 0,0 0 0,0-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0-1,0-1 1,3 0 0,-2 0 21,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,-1 0 1,1-1-1,-1 1 0,4-5 1,-4 3 1,1-1 1,-1-1 0,0 1-1,-1 0 1,1 0 0,-1-1-1,0 1 1,0-1 0,-1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,-1-1 0,0 1 0,0-1-1,-1 1 1,-2-7 0,3 9-19,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 1 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0 1-1,0-1 1,0 0 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-4 2-1,4-2-143,0 0-1,0 1 1,1 0-1,-1-1 1,0 1-1,1 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 1 1,0-1-1,-3 6 1,-7 23-5794,11-14-16</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8186.48">3320 1193 13366,'0'0'9903,"8"12"-9310,-6-8-568,3 4 66,0 1-1,0 0 0,-1 0 1,0 1-1,3 14 1,-6-22-73,0 1 1,-1 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,-1 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,0 0-1,0 0 1,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-5 2 1,0 0 81,-1-1 0,0 0 0,1 0 0,-1-1 1,0 0-1,0 0 0,-1-1 0,1 0 0,0 0 0,-10-1 1,17-1-79,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 1,0-1-1,0 1 0,1 0 1,-1-2-1,5-46-49,2 34 10,1 0 0,1 0 1,0 1-1,1 1 0,0 0 1,1 0-1,20-19 0,-10 10-242,7-5-578,13-14-1455,-24 13-3521,-16 19 15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8364.46">2946 1034 17224,'0'0'3009</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8364.45">2946 1034 17224,'0'0'3009</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9832.63">543 874 10261,'0'0'8518,"0"56"-4855,0 288-1336,3-318-2278,0-1-1,1 0 1,2 1 0,1-2 0,0 1 0,2-1 0,1 0 0,25 44-1,-13-32-6,2-1-1,0-2 0,3 0 0,54 52 0,-70-76-35,0-1 0,0 0 0,1 0 0,0-2-1,0 1 1,0-1 0,1-1 0,0 0 0,0-1-1,22 4 1,3-2 40,0-2-1,60-1 0,-97-5-36,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-4 0,1 3-42,0-1 12,0 1 0,0-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-2-5 0,2 9 23,0-1-1,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 1 0,-1-1 0,1 1 0,-1-1 1,0 1-1,1 0 0,-3 0 0,4 44-185,1-41 182,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,3 2 0,15 21 35,-19-23-29,-1-1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,-1-1 0,1 0 1,0 0-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,0 0 0,-2 0 0,-41 25-255,22-14-1578,9-2-2272,1-4-2011</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10802.05">1658 1729 13558,'0'0'7462,"-1"-8"-5038,1 7-2410,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,-21 29 306,2 1 1,2 0 0,0 2 0,-13 36-1,21-38-130,9-26-15,5-17-97,8-22-278,1 0-1,2 1 0,2 0 1,0 1-1,40-50 1,-58 83 193,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 1,0 0-1,1 0 0,-1 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,1 0 0,-1 0 0,0 1 1,0-1-1,0 0 0,-1 1 0,6 13-42,1 22 268,-1 1 1,0 60-1,-4-23-4266,-1-57 1927</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10979.49">1594 1804 13622,'0'0'7956,"57"-24"-8036,-29 24-1153,8-5-2464,-8 1-4211</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11601.54">1786 1867 14311,'0'0'7184,"7"-2"-6269,-1 1-851,1-1-1,0 0 0,-1-1 0,0 1 0,1-1 1,-1 0-1,0-1 0,-1 1 0,1-1 1,-1-1-1,0 1 0,1-1 0,-2 0 1,1 0-1,-1 0 0,0 0 0,0-1 1,0 0-1,-1 0 0,1 0 0,-2 0 1,1 0-1,-1-1 0,0 1 0,0-1 0,1-8 1,7-53 154,-10 67-244,0 41-524,0-27 576,0 0 0,1 0-1,0 0 1,1 0 0,0 0 0,6 17-1,-7-27-21,0 0-1,1 0 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,1-1 1,-1 1 0,1 0-1,0-1 1,-1 0-1,1 0 1,0 1 0,0-1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 0-1,0 1 1,0-1 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,3-1 1,-1 0-2,0 0 0,0 0-1,0 0 1,0-1 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0-1,0-1 1,0 0 0,3-5 0,-2 1-131,1 1 0,-2-1 0,1 0 0,-1-1 0,0 1 0,-1 0 0,0-1 0,1-18 1,-4 36 115,0 0 1,-1-1 0,0 1 0,0 0 0,-5 10 0,-6 27 311,9 22-38,4-38-8304</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11789.34">1914 1775 13078,'0'0'6339,"50"-2"-6339,-11 2 224,4 0-224,-1 0-912,-3 0-1089,-10 0-1617,-12 0-2465</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12197.92">2229 1769 12134,'0'0'5493,"12"12"-4597,40 35 49,-49-43-803,1-1 0,-1 1 1,1 0-1,-1 0 0,0 1 1,4 8-1,-7-12-68,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,0 1 0,-1 0 54,0-1-1,0 1 1,0 0 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1-1 0,0 1 0,1 0-1,-1-1 1,0 0 0,1 1-1,-1-1 1,0 0 0,-3-1 0,6 1-128,-1 0 1,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,1 0 0,10-25-1279,-3 19 403,-1-1 1,1 1-1,0 0 1,0 1-1,17-11 1,-20 15 825,-1 0 1,0 0 0,1 0-1,-1 1 1,1-1-1,0 1 1,-1 0 0,1 1-1,6-1 983,-11 63 2947,0 1-5668</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12337.86">2496 1717 10293,'0'0'2177</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12337.85">2496 1717 10293,'0'0'2177</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13551.44">2496 1704 5122,'56'-15'10560,"-56"14"-10446,1 1 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 0,0 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 1,0-1-1,0 1 0,0 0 1,-1 15-465,1-15 749,-5 35 1143,-14 57-1,1-7-942,18-89 82,0-3-582,0 0 0,0 0 0,1 0-1,0 1 1,0-1 0,2-7 0,-2 11-109,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,3 1 0,-5-1 7,1 1-1,-1 0 0,0 0 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,1 0 0,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 1,-1 0-1,1-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 2 0,-2-2 8,1 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,-1-1 0,1 1 0,0 0 0,0 0 0,-1-1 0,1 1-1,-1 0 1,-2 0 0,-21 5 83,20-5-83,0 0 0,0 0 1,1 1-1,-1-1 0,0 1 1,1 0-1,-1 0 0,-5 4 0,9-5-15,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,20 0-145,-18 0 121,15 1-146,0-2 0,0 0 0,-1-1 0,1-1 0,-1-1 0,1 0 0,18-8 0,-30 10 225,-1 0 0,0-1-1,0 0 1,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 1-1,0-2 1,-1 1 0,1 0 0,-1-1 0,0 1 0,0-1-1,0 0 1,-1 0 0,0 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,0 1 0,0-1 0,-1 1 0,0-10 0,0 15 110,-4 38 68,2-28-123,0 0 0,0 0 0,1 0 0,1 0 0,-1 1 0,3 18 0,-1-28-101,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0-1-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,32-11 96,-26 6-37,0 0 0,-1-1 0,1 0 0,8-12 0,-13 16-49,0-1 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,0 1 0,1-8-1,-2 12-45,7 39-70,-7-38 114,1 1 0,-1-1-1,1 1 1,-1 0 0,1-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,2-1 0,3-2 7,1 1 1,-1-1-1,0-1 1,0 1-1,-1-1 1,1 0-1,-1 0 1,8-11-1,-7 5-31,-1 0 0,0 1 0,0-2 0,-1 1 0,-1 0 0,0-1-1,-1 0 1,0 1 0,1-15 0,2-8-428,-23 98 332,14-51 147,0 0 1,0 0-1,1 1 1,1-1-1,0 1 1,1 0-1,1 20 1,0-33-35,0 1-1,1-1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1 0 0,1-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,2 0 0,39 2-14,-31-2 22,1-1 13,-1 0 0,1-1 0,-1 0 1,0-1-1,0 0 0,0 0 0,0-1 0,-1-1 0,0 0 1,1 0-1,-2-1 0,10-7 0,-13 9-27,0-1 0,0 1 0,0-1-1,-1-1 1,0 1 0,0-1 0,-1 1 0,1-2 0,-1 1 0,0 0-1,-1-1 1,0 1 0,0-1 0,0 0 0,-1 0 0,0 0-1,0-1 1,-1 1 0,1-11 0,-2 18 11,-1-1-1,1 1 1,0 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 1 1,0-1 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 1-1,-17 8 43,11-3-38,0 1 0,0 0 0,1 1 0,0-1 0,0 1 1,0 0-1,1 0 0,0 1 0,1 0 0,0 0 0,0 0 0,1 0 1,0 0-1,1 1 0,0 0 0,0-1 0,1 1 0,1 0 1,-1 0-1,3 16 0,-2-25-29,1 1 0,-1 0 1,1-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,1 0-1,-1 0 0,1 0 0,-1 1 1,1-1-1,-1-1 0,1 1 1,0 0-1,-1 0 0,1-1 0,0 1 1,-1-1-1,1 1 0,3 0 1,-2-1-347,-1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,2-1-1,8-16-7021</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13708.2">3031 1748 6835,'0'0'12678,"35"12"-12950,12-12-449,-5 0-1375,-7 0-4483</inkml:trace>
 </inkml:ink>
@@ -7158,7 +7158,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="488.13">242 157 2161,'0'0'5066,"0"-14"-1453,0-48-893,0 37 4612,-3 77-5786,-9 52-1,5-51-1860,0 53-1,7-105 116,1-1 0,-1 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1-1,18-10-6181,-5-4-477</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="818.03">288 254 5074,'0'0'10627,"1"-11"-9523,6-32-304,6 165 2794,-12-120-3587,-1 1 0,0-1 0,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,3 2 0,-3-4 3,0 1-1,0 0 1,0-1 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1-1-1,0 1 1,1 0 0,2-1 0,-1-1 26,1 1 1,0-1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0-1,1-1 1,-1 1 0,0 0 0,0-1 0,0 1 0,2-5 0,-1-5 61,1 1 1,-2-1-1,1 0 0,-2 0 0,0 0 1,-1-22-1,0 34-118,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,-1 1-1,1-1 1,0 1-1,0-1 1,-1 0 0,1 1-1,-1-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,-1 1 1,1-1-1,-1 1 1,0-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 1-1,-1-1 1,0 0-1,1 0 1,-1 1 0,-1 0-1,-1 0-805,0 0-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1-1,-1 0 1,1 0 0,0 1-1,-3 1 1,1 3-6169</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2354.61">452 220 9861,'0'0'7998,"3"3"-7758,0-1-116,0 1 1,0 0-1,-1 0 0,0 0 1,1 0-1,-1 1 0,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,-1 0 0,2 6 1,1 67 1749,-4-55-1579,1-22-36,0-11 160,1 0-441,0 0 0,0 1 0,1-1 1,0 1-1,1-1 0,0 1 0,0 0 1,2 0-1,-1 1 0,1-1 0,8-11 0,-13 20 14,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 0,11 26-75,-10-24 103,4 10 226,-1 0 0,0 0 0,-1 0 0,2 25 875,10-91-585,4 19-577,-18 32 30,0 0-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,0 0 0,1 0 1,-1-1-1,0 1 1,1 0-1,0 0 0,-1 0 1,1 1-1,0-1 0,-1 0 1,1 1-1,3-2 1,-3 4 4,0 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 1,-1 1-1,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 5 1,2 3 0,3 8 12,-5-11 3,2 0-1,-1 0 0,1-1 1,0 1-1,1-1 0,0 0 0,6 9 1,-8-14-5,-1-1-1,1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,1-1 1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1-1,1 1 1,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,3-1 0,-1 1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,3-8 1,-3 0-22,0 0 0,0 0 0,-1 0 0,0 0 0,-1-13 1,0 23 9,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 1-1,-1-1 1,1 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 0 0,0 1 0,1-1-1,-1 1 1,0-1 0,1 0 0,-1 1-1,0-1 1,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,-2 0 0,2 0-8,-1 0 1,0 1 0,1-1-1,0 0 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,1 0-1,-1 1 1,0-1-1,0 2 1,-2 7 29,0 0 0,1 1 0,0-1 1,1 1-1,0-1 0,0 1 1,1-1-1,1 1 0,1 12 0,-1-22-9,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,1-1-1,-1 1 1,0-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 1,0 0-1,1 0 0,-1 0 1,0-1-1,0 1 1,1 0-1,-1 0 0,0-1 1,0 1-1,3-2 1,39-16 126,-40 15-125,0 1 1,0-1 0,0 1-1,0-1 1,-1 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0-1-1,1-7 1,-1 1-7,-1 0 0,0 0 0,0-20 0,-1 19-26,0 11 20,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 0,1 1 0,-10 11-114,7-10 113,1 1-1,0-1 1,0 1 0,1-1 0,-1 1 0,0-1 0,1 1-1,0 0 1,0-1 0,-1 1 0,1 0 0,1 0 0,-1-1 0,1 5-1,0-5 5,0-1-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,1 1 0,-1 0 1,0 0-1,1-1 0,-1 1 1,1-1-1,-1 1 0,0-1 0,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 1,1-1-1,2 1-3,-1 0 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0-1-1,0 1 1,0-1 0,-1 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0-1 0,0 1 0,3-6 0,8-8-7,-14 16-4,-3 95-309,3-94 324,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 0 0,1 1 0,-1-1 1,0 0-1,1 1 0,-1-1 1,1 0-1,-1 0 0,1 1 0,-1-1 1,2 0-1,21-1-2,-19 0 3,1-1 0,-1 0 0,1 1 0,-1-1-1,0-1 1,0 1 0,8-6 0,-9 6-57,-1-1 1,1 0-1,0 0 1,-1 1-1,0-1 0,0-1 1,0 1-1,0 0 0,0-1 1,-1 1-1,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 1,0-5-1,-1 9 56,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0-1 0,0 1 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 1 0,-9 9-25,5-2 49,1 1 1,0-1-1,0 1 0,1 0 0,1 0 0,-1 0 1,1 1-1,1-1 0,0 0 0,1 10 0,-1-7-11,0-11-8,-1-1 0,2 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 1,0 0-1,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,-1 1 0,2-1 0,29 0-526,-22-2-557,-1 0 1,0 0-1,0-1 1,-1-1-1,11-5 1,11-11-7252</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2484.7">1287 148 12902,'0'0'12021,"-7"-34"-12053,4 34-112,3 6-1424,-4 8-833,4 4-1953,0-2-2770</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2484.69">1287 148 12902,'0'0'12021,"-7"-34"-12053,4 34-112,3 6-1424,-4 8-833,4 4-1953,0-2-2770</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2752.13">1386 234 13766,'0'0'6353,"-15"11"-5940,-49 39 219,61-47-526,-1 0 0,1 1-1,0 0 1,-1 0 0,2 0 0,-1 0-1,0 0 1,1 1 0,0-1-1,0 1 1,0 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,1 0-1,1 7 1,-1-3-15,1-8-79,-1 1 0,0 0 0,0 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0-1,1 0 1,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,3 0 0,8 2 21,-1-1 0,1-1 0,20-1 0,-21 0-4,4 0 16,1-1 0,-1-1 0,24-7 0,5-8-1708,-11-8-4687,-25 12-1139</inkml:trace>
 </inkml:ink>
 </file>
@@ -7478,14 +7478,14 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="375.54">439 233 6835,'0'0'10717,"-7"-9"-9903,5 10-811,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,-1 3 0,-1 0-17,1-1 1,0 1 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 5-1,2-9 9,1 0-1,-1-1 0,0 1 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,1 0 1,0-1-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,1-1-1,-1 1 57,0 0 0,1 0-1,-1 0 1,0-1 0,0 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,1 0-1,-1 0 1,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1-1 0,-1 1 0,0 0 0,1-3-1,-1 2 108,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,-3-2 1,3 2-449,-1 1 0,1-1 0,-1 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,0-1-1,0 1 1,0 0 0,-3 0 0,5 6-5663,1 0-1050</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="509.35">426 220 12294</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="730.23">426 233 12294,'74'-36'1085,"-59"29"1010,-15 38-1925,-3-9 186,2-18-317,0 0 1,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,1 6 0,-1-9-25,0 0 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,0-1 0,1 1 1,-1 0-1,1-2 0,28-13 390,-28 13-264,0 0-1,0 0 1,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0-5 0,-8 8-9412,2 0 2468</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1274.86">674 239 10901,'0'0'5221,"-1"10"-4976,-5 62 1,32-73-323,-13-3 118,1-1 0,-1-1 0,0 0 0,-1-1 0,15-10 1,-1 1-20,-24 14-27,-2 2-179,4 11-76,-4-9 275,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,2 2 0,1-3 20,1 0-1,-1 0 1,0-1-1,1 0 1,-1 1 0,0-1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 0 0,0 0-1,0-1 1,-1 1-1,1 0 1,-1-1-1,4-7 1,4-4 11,-2-1 1,0 1 0,-1-1-1,10-33 1,-11-6 319,-5 39 3696,-11 47-4202,3-8 36,0 0 0,2 1-1,0 0 1,1 0 0,0 26 0,4-49-32,0 0 1,0 0 0,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 0 0,0 1-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 1 1,0-1 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 1-1,-1-1 1,1 0 0,0 0-1,0-1 1,0 1-1,1 0 1,18 0-5382</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1274.85">674 239 10901,'0'0'5221,"-1"10"-4976,-5 62 1,32-73-323,-13-3 118,1-1 0,-1-1 0,0 0 0,-1-1 0,15-10 1,-1 1-20,-24 14-27,-2 2-179,4 11-76,-4-9 275,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,2 2 0,1-3 20,1 0-1,-1 0 1,0-1-1,1 0 1,-1 1 0,0-1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 0 0,0 0-1,0-1 1,-1 1-1,1 0 1,-1-1-1,4-7 1,4-4 11,-2-1 1,0 1 0,-1-1-1,10-33 1,-11-6 319,-5 39 3696,-11 47-4202,3-8 36,0 0 0,2 1-1,0 0 1,1 0 0,0 26 0,4-49-32,0 0 1,0 0 0,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,-1-1 1,1 0 0,0 1-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 1 1,0-1 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 1-1,-1-1 1,1 0 0,0 0-1,0-1 1,0 1-1,1 0 1,18 0-5382</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1498.12">851 199 5410,'0'0'14359,"31"-20"-14359,8 10 64,7-2-64,1 0-880,-1 0-529,-7-1 32,-7 5-1504,-8 4-4178</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2110.53">1447 37 16135,'0'0'6884,"-1"1"-6861,0-1 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,1 0 1,-1-1-1,0 1 0,1 0 0,-1 0 1,-1 1-1,-16 21 148,-28 48 0,41-62-150,0 1 1,1-1 0,1 1-1,-1-1 1,1 1-1,1 0 1,0 0-1,1 0 1,-1 14-1,2-22-121,0 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0-1-1,0 0 1,1 1-1,-1-1 1,0 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0 0,1-1-1,0 1 1,2 0 0,7 1-1999,-1 0 0,0-1 0,1 0 0,12-1 0,-21 0 1614,22 0-7239</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3278.47">1602 105 6755,'0'0'9394,"-4"-6"-9114,-21-30 72,20 35-209,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1 0,0 1-1,-7 0 1,1 0 197,7-1-289,0 1 0,0 1 0,0-1 0,1 0 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 1 1,-5 4 0,-33 33 584,31-29-473,0 1 0,0 0 0,-13 24 0,21-33-160,0 0 1,0 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,1 1-1,-1-1 1,1 0 0,0 0-1,-1 1 1,1-1-1,1 0 1,-1 1-1,0-1 1,1 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,3 5 1,-2-6 4,1 0-1,-1-1 1,0 1 0,0-1 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1-1-1,1 1 1,0-1 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,-1-1-1,1 0 1,4-1 0,1 0 38,0-1-1,0 0 1,-1-1 0,1 1-1,-1-1 1,0-1 0,8-5 0,-9 5-85,-1-1 0,1 0 1,-1 0-1,0-1 1,0 0-1,-1 1 0,0-1 1,0-1-1,0 1 1,-1-1-1,-1 1 0,1-1 1,-1 0-1,0 0 1,-1 0-1,0 0 0,0 0 1,-1-16-1,0 22 53,0 1 0,0-1 0,-1 0 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 1 0,-3 0 0,0 0 9,1-1 1,-1 1-1,0 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 1 0,0 0 0,0 0 1,0 0-1,-5 5 0,7-5-33,1-1 1,-1 0-1,0 0 0,1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,0 0 1,0-1-1,1 1 0,-1 0 0,1 4 0,0-5 10,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,1-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,3-1 0,8 0 10,-1 0 0,1-1 0,-1-1 0,0 0 0,0-1 0,0 0 0,0-1 0,-1 0 0,0-1 0,0 0 0,0 0 0,-1-1 0,1-1 0,-2 0 0,1 0 0,-1-1 0,-1 0 0,0-1-1,0 0 1,-1 0 0,0-1 0,0 1 0,-1-2 0,6-15 0,-51 172 882,23-105-829,2 1 0,2 1 0,1 0-1,3 1 1,1 0 0,-2 59 0,9-101-62,0-1 0,0 1 1,0-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,0-1 0,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,1 0-1,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,0 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 0,-1 0 1,1-1-1,-1 1 1,1 0-1,-1-1 1,0 1-1,1-1 0,2-1 21,0 1-1,-1-1 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,2-2 1,-2 1-46,0-1 1,0 1 0,-1 0 0,0-1-1,0 0 1,0 1 0,0-1 0,-1 1 0,1-1-1,-1 0 1,0 1 0,-1-1 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1-1,-1-1 1,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0 0,0 0-1,0 1 1,-7-6 0,-1 0 44,-1 0 0,0 2 0,-1-1 0,0 2 0,0-1 0,0 2 0,-1 0 0,-14-3 0,52 0-634,22 0-58,118-28-8514,-107 19 3055</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3554.3">2130 38 10085,'0'0'9265,"-2"6"-8841,-27 78 10,14-46 271,2 0-1,-12 58 1,23-61-509,2-35-200,0 1 0,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,1-1 0,-1 1 1,0 0-1,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,1 0-1,7 0-510,0 0 0,-1 0 0,1-1 0,0-1 0,14-3 0,-20 4-43,0 0 0,0-1 0,0 1 0,0-1-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1-1-1,-1 1 1,4-5 0,0-5-3770</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3787.26">2027 199 9380,'0'0'7252,"46"-2"-7012,-17 2-64,3 0-96,-4-2-80,-3-4-256,-8 0-1137,-6-2-2048,-7 0-1938</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3958.33">2106 84 1585,'0'0'19048,"-3"-63"-19032,17 55-16,4 2-80,3 2-448,4 2-736,-4 2-753,4 0-625,-4 2-4721</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4920.43">2353 139 13382,'0'0'3821,"-1"14"-2199,1-4-1394,0 0 76,0 1 1,-1-1 0,0 0-1,0 0 1,-1 0 0,-1-1 0,0 1-1,0 0 1,0-1 0,-1 0-1,-8 14 1,31-40-979,1 1 0,32-19 0,-49 35 692,-2 13 255,-2-12-251,1 1-1,0-1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 1 0,0 0 0,6-3 5,0-1-1,-1-1 1,1 1-1,-1-1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,0-1 0,8-7 1,-12 12 88,31 8 185,-26-8-274,-1 0 0,0 0 1,1-1-1,-1 0 0,1 1 0,-1-2 0,0 1 0,0-1 0,0 1 0,1-1 1,-2-1-1,1 1 0,0-1 0,0 0 0,-1 0 0,0 0 0,1-1 0,-1 1 1,-1-1-1,1 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,3-8 1,5-11 216,-1 0 1,-1 0-1,-1-1 1,6-29 0,-18 86 270,-9 33-634,-90 245 318,100-301 134,5-20-166,8-21-76,-3 17-43,78-134 64,-75 134-124,1 1 1,0 0-1,1 1 1,0 0-1,1 1 1,0 0-1,24-15 1,-32 24-20,0 1 0,0-1 0,0 1 0,0 0 0,0 1 1,1-1-1,8 0 0,-13 1 27,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0 0-1,0-1 1,0 1 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 2 0,0 0 11,0 1-1,0-1 1,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1-1,-5 2 1,-18 8 64,-1-1 1,0-1-1,-36 7 0,-1-5-3208,39-9-2314</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4920.42">2353 139 13382,'0'0'3821,"-1"14"-2199,1-4-1394,0 0 76,0 1 1,-1-1 0,0 0-1,0 0 1,-1 0 0,-1-1 0,0 1-1,0 0 1,0-1 0,-1 0-1,-8 14 1,31-40-979,1 1 0,32-19 0,-49 35 692,-2 13 255,-2-12-251,1 1-1,0-1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 1 0,0 0 0,6-3 5,0-1-1,-1-1 1,1 1-1,-1-1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,0-1 0,8-7 1,-12 12 88,31 8 185,-26-8-274,-1 0 0,0 0 1,1-1-1,-1 0 0,1 1 0,-1-2 0,0 1 0,0-1 0,0 1 0,1-1 1,-2-1-1,1 1 0,0-1 0,0 0 0,-1 0 0,0 0 0,1-1 0,-1 1 1,-1-1-1,1 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,3-8 1,5-11 216,-1 0 1,-1 0-1,-1-1 1,6-29 0,-18 86 270,-9 33-634,-90 245 318,100-301 134,5-20-166,8-21-76,-3 17-43,78-134 64,-75 134-124,1 1 1,0 0-1,1 1 1,0 0-1,1 1 1,0 0-1,24-15 1,-32 24-20,0 1 0,0-1 0,0 1 0,0 0 0,0 1 1,1-1-1,8 0 0,-13 1 27,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0 0-1,0-1 1,0 1 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 2 0,0 0 11,0 1-1,0-1 1,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1-1,1 1 1,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1-1,-5 2 1,-18 8 64,-1-1 1,0-1-1,-36 7 0,-1-5-3208,39-9-2314</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7662.64">224 662 8660,'0'0'7865,"5"-7"-6931,14-23 261,-14 23 744,-23 7-1525,0 0-1,1 2 0,-24 5 0,36-6-421,1 0 1,-1 0 0,1 0-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 1-1,1-1 1,-1 1-1,0 0 1,1 1-1,-1-1 1,1 0-1,0 1 1,-4 6-1,6-7-22,-1-1-1,1 0 0,1 1 0,-1-1 1,0 0-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 1,1-1-1,0 1 0,-1-1 0,1 0 1,2 5-1,1 0-4,1 0-1,0 0 1,1 0 0,11 10-1,-13-13 35,-1-1-1,1 0 0,0 1 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,-1-1 0,0 1 0,1-1 1,-2 1-1,1 0 0,-1 0 0,2 7 0,-4-10 7,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,-1 0 0,-47 9 119,46-8-126,-1 0 15,0-1 0,0 1 0,-1 0 0,1-1 0,-1 0 0,1-1 0,0 1 0,-9-3 0,12 2-36,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1-2 0,-1 2 13,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0-1,1 0 1,0 0-4,1 0 0,-1 1 0,0-1 1,0 1-1,0-1 0,1 1 0,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,3 2 0,9 2-36,0 0-1,-1 2 0,20 9 0,-16-7 1,-10-5 64,1 0 0,0 0 1,0-1-1,0 0 1,0-1-1,0 0 0,1-1 1,12 0-1,-18 0-9,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1-1,1-1 1,-1 1 0,0-1 0,0 0 0,0 0 0,3-6 0,0-5-210,0 4 1786,-4 30-810,-1-19-774,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,1 0 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,-1 0 1,1 1-1,0-1 0,0 0 0,0 1 0,2-1-12,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0-1 0,4 0 1,-3 0-29,0 0 0,1 0 1,-1-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,1-1 0,0 1 1,-1-1-1,0 0 0,1 0 0,4-6 1,0-15 228,-7 20 263,-2 17-401,-2 6-115,2-15 63,0 1-1,0 0 0,1 0 0,0 0 0,0 0 1,0 0-1,1 7 0,0-10-10,-1-1 0,1 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-2 1,0 1-1,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,2 0 0,2 0-58,1 0-1,0 0 1,0 0 0,0-1-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 0-1,-1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,-1 0 1,9-9 0,-6 9 910,-7 10-545,-9 23-389,4-16 329,4-12-115,3-2-207,131-55-1831,-134 56 1925,1 1 0,0-1 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 2 0,1 23 347,0-23-317,65 31 932,-54-30-2418,1 0 0,-1-1 1,1 0-1,20 0 0,2-2-4188</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8460.23">1272 710 13222,'0'0'9623,"-5"1"-9578,2 0-38,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1-1,1 0 1,-1-1 0,0 1 0,1 0-1,0 0 1,-1 0 0,1 1-1,0-1 1,0 0 0,0 1-1,-2 4 1,1-1-19,1-1 0,0 1 0,0 0 0,0 0 0,1 0 0,0 0 0,0 0 0,1 0 0,0 8-1,1-13-5,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,0-1 1,1 2 3,-1-1 0,0 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1-1 0,0 0 0,1 1 0,-1-1 0,3-2 1,-4 2 32,0 1 0,-1-1 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,0 0 0,0-1 1,-1 0 13,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-6-1 1,5 2-22,-1-1 0,1 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 1 1,-8 1-1,10-1-23,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 1 0,1 1 0,1-2-55,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,3-1 0,40-1-12,-43 2 68,7-1 32,0-1-1,0 0 0,0 0 0,-1 0 0,1-1 1,0 0-1,-1-1 0,0 0 0,0 0 0,0 0 1,9-9-1,5-5 233,-2-2-1,19-22 1,-27 30-37,-43 88 95,-50 122-63,73-170-245,1 0-1,1 1 0,2-1 1,0 1-1,0 40 1,20-82-327,-12 7 211,0-1 1,0 1 0,0-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0 0-1,-1 0 1,0 0 0,0 0 0,0-1-1,-1 1 1,0 0 0,0 0 0,-1 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,-1 0 1,-1 1 0,0 0 0,1 0-1,-2 0 1,1 0 0,-1 1 0,0 0-1,0 0 1,0 0 0,-10-6 0,11 8 326,-1 1 0,1 0 0,-1-1 1,0 2-1,1-1 0,-1 1 0,0-1 0,-9 0 1,12 2 464,5 0-549,62 0-203,1-3 0,103-18 0,-167 21-154,13-7-113,-13-1-3592</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9057.44">2039 690 6739,'0'0'15567,"-8"10"-14633,2 2-892,1 0 0,0 0 0,1 1 0,0 0-1,1 0 1,0 0 0,1 0 0,1 0 0,0 23 0,1-35-62,1 1 1,0-1 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0-1,0-1 1,1 1-1,-1-1 1,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,4-1 1,-1 1-802,1 0-1,0 0 1,0 0 0,-1-1 0,1 0 0,0 0-1,-1 0 1,9-3 0,-5-8-4560,-7 0-2175</inkml:trace>
@@ -8068,7 +8068,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">374 613 11237,'0'0'3925,"-12"13"-3819,-142 181 809,153-193-578,2-7-233,0-1 0,0 0 0,1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,0 0 0,0 0 1,1 1-1,7-10 0,52-57-996,-55 64 807,2-4-53,-8 8 131,1 1 0,-1 0 1,0 0-1,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,1 0-1,-1 0 0,6-3 0,-7 9 14,-1-1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,0-1 0,0 0-1,0 0 1,0 1 0,-1 3 0,1-1 96,0 32 404,-10 73 0,-5-49-3984,13-60 1428</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="266.97">264 748 10789,'0'0'7745,"0"0"-7742,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,100 0 47,-100 5-1568,-1 0 865,0-1-1,0 1 1,-1 0 0,0-1-1,1 1 1,-2 0 0,1-1-1,0 1 1,-1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,-2 4-1,-16 19-6110</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="266.96">264 748 10789,'0'0'7745,"0"0"-7742,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,100 0 47,-100 5-1568,-1 0 865,0-1-1,0 1 1,-1 0 0,0-1-1,1 1 1,-2 0 0,1-1-1,0 1 1,-1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,-2 4-1,-16 19-6110</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="955.27">149 1106 13638,'0'0'6534,"0"5"-6059,-1 9-403,-1-1 0,0 1 0,0-1 0,-2 0 0,0 0 0,0 0 0,-12 22 0,30-117-1286,-3 48 1237,-7 20 12,1 1 0,0-1 1,0 1-1,1 0 0,9-13 1,-13 22-30,1 1 1,0 0 0,0-1 0,0 1 0,0 0-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 1-1,0 0 1,0 0 0,0 1 0,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,0 1 0,1-1 0,5 1-1,-9 0-6,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 2 0,-8 20 12,-27 18 81,-18 4 84,36-32-176,0 2 1,2 0 0,-20 22 0,34-36-55,1 1-1,-1 0 0,1 0 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1-1 0,1 1 1,0 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,1 1 1,45 22 223,-21-11-243,-25-12 79,0 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1 0,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1 0 1,0-1 0,1 1-1,-1-1 1,0 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1-1 0,1 1-1,0-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,0-1 1,-1 1-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,1 1 0,-2-1-1,-48 14 727,44-13-773,-14 3-301,-43 11 959,29 3-6044,27-12-1270</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9423.9">317 305 8148,'0'0'5842,"0"-4"-5543,0-11-149,0 11 239,13 16 569,7 92 367,-8-28-553,-12-76-744,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0-1 1,1 1-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1-1 1,10-11 639,16-32-662,-16 25 150,11-12-132,1 2 0,1 0 0,44-38 0,95-69-2645,-74 64-1943,-47 36-3047</inkml:trace>
 </inkml:ink>
@@ -8474,9 +8474,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">272 180 12422,'0'0'3356,"-13"-6"-2161,-59-30 659,70 35-1810,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,0-1 1,-2 4-1,-48 52-134,46-50 160,-3 5-60,0 0 0,0 0 0,1 1 0,1 1 0,1-1 0,-9 23 0,13-31-7,0 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 0 1,0 1-1,-1-1 0,2 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0-1 0,1 1 0,3 5 0,-3-8-40,0 1 1,1-1 0,-1 0-1,1 1 1,0-2-1,0 1 1,0 0-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1-1-1,-1 1 1,1-1 0,0 0-1,0-1 1,0 1-1,-1-1 1,1 0 0,0 0-1,0 0 1,0-1-1,0 1 1,6-3-1,6 0-357,-1-1-1,-1-1 0,1 0 0,-1-1 1,0-1-1,15-9 0,-15 7-500,1-1 1,-2-1-1,0 0 0,0-1 1,-1 0-1,0-2 0,-1 1 1,-1-1-1,0-1 0,8-16 1,10-20-2518</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1220.14">516 24 5843,'0'0'7902,"0"-6"-7670,-3-12-264,-5 23-40,-15 39 6,10-18 201,9-17-84,-19 33 401,-19 53-1,37-82-412,1 0 0,0 0 0,1 0 0,0 0 1,1 0-1,1 0 0,0 1 0,1-1 0,1 18 0,0-31-43,-1 1 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,0 0 0,0 1 0,28-2-4,-22-1-21,0 0 0,0 0-1,-1 0 1,1-1 0,11-7-1,-11 5-45,-1 0-1,0 0 1,-1 0-1,1-1 0,-1 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,0-1-1,-1 0 0,0-1 1,5-13-1,-1-34 2015,-9 55-1912,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-3 1 0,-2 4-23,0 0 0,0 0-1,1 0 1,0 1 0,0 0 0,1 0-1,-1 0 1,1 0 0,1 1-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 9 1,27-46 156,23-49-464,-51 131-366,3-47 688,-1 1 0,1-1-1,0 1 1,0 0-1,1 0 1,0 0 0,0-1-1,1 1 1,1 8 0,-1-14-20,0-1 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0 0,0-1-1,2 0 1,23-8 138,-21 5-133,1 0 0,-1-1 1,0 1-1,0-1 0,-1 0 1,1-1-1,-1 1 0,0-1 0,-1 1 1,1-1-1,-1 0 0,-1-1 0,1 1 1,-1 0-1,0-1 0,0 0 0,-1 1 1,0-1-1,1-8 0,9 57-505,-11 0 453,0-15 42,0-28 14,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,28-46-838,-23 40 920,-1 1 0,0-1 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,0-1 1,0 0-1,1-12 1054,-3 24-1163,-1 0 1,1 0-1,-1 0 0,2 0 0,-1 0 1,0 0-1,1 0 0,0 0 0,3 9 1,0-6 32,0 0 0,0 0 0,1-1 1,9 12-1,14 24 46,-29-42-32,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 1,0-1-1,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-3 0 0,-43 4 787,58-21-5649,13-4-5113</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1220.13">516 24 5843,'0'0'7902,"0"-6"-7670,-3-12-264,-5 23-40,-15 39 6,10-18 201,9-17-84,-19 33 401,-19 53-1,37-82-412,1 0 0,0 0 0,1 0 0,0 0 1,1 0-1,1 0 0,0 1 0,1-1 0,1 18 0,0-31-43,-1 1 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,0 0 0,0 1 0,28-2-4,-22-1-21,0 0 0,0 0-1,-1 0 1,1-1 0,11-7-1,-11 5-45,-1 0-1,0 0 1,-1 0-1,1-1 0,-1 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,0-1-1,-1 0 0,0-1 1,5-13-1,-1-34 2015,-9 55-1912,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-3 1 0,-2 4-23,0 0 0,0 0-1,1 0 1,0 1 0,0 0 0,1 0-1,-1 0 1,1 0 0,1 1-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 9 1,27-46 156,23-49-464,-51 131-366,3-47 688,-1 1 0,1-1-1,0 1 1,0 0-1,1 0 1,0 0 0,0-1-1,1 1 1,1 8 0,-1-14-20,0-1 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0 0,0-1-1,2 0 1,23-8 138,-21 5-133,1 0 0,-1-1 1,0 1-1,0-1 0,-1 0 1,1-1-1,-1 1 0,0-1 0,-1 1 1,1-1-1,-1 0 0,-1-1 0,1 1 1,-1 0-1,0-1 0,0 0 0,-1 1 1,0-1-1,1-8 0,9 57-505,-11 0 453,0-15 42,0-28 14,0 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,28-46-838,-23 40 920,-1 1 0,0-1 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,0-1 1,0 0-1,1-12 1054,-3 24-1163,-1 0 1,1 0-1,-1 0 0,2 0 0,-1 0 1,0 0-1,1 0 0,0 0 0,3 9 1,0-6 32,0 0 0,0 0 0,1-1 1,9 12-1,14 24 46,-29-42-32,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 1,0-1-1,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-3 0 0,-43 4 787,58-21-5649,13-4-5113</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1433.07">1030 256 13926,'0'0'4931,"25"0"-4819,3 0-16,8 0-32,6-8-64,-3 0-544,0 1-1313,-3 1-224,-12 0-2577,-9 2-1537</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1609.18">1145 243 6163,'0'0'9108,"-29"12"-9156,29-10 32,14 0 16,11-2 0,4 0-688,3 0-1842,-4-4-1968,0-8-1648</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1609.17">1145 243 6163,'0'0'9108,"-29"12"-9156,29-10 32,14 0 16,11-2 0,4 0-688,3 0-1842,-4-4-1968,0-8-1648</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1838.26">1272 130 4098,'0'0'11360,"-6"-4"-10611,-13-6-1012,23 17 208,40 35 264,-7-8-78,-30-27-111,0 1 0,0 0 0,-1 0 0,0 1-1,-1 0 1,0 0 0,0 0 0,4 15 0,-7-20-9,-1-1-1,0 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,-1 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 1,0-1 0,0 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,-5 4 1,-11 8-128,-1-1 1,-1-1-1,-39 19 1,5-11-5290,33-15-2566</inkml:trace>
 </inkml:ink>
 </file>
@@ -8598,7 +8598,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1871.85">764 383 11461,'0'0'6393,"-3"-8"-5713,0 0-521,3 5-106,-1 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 1,-1 0-1,0 0 0,1-1 1,-1 1-1,-3-2 0,4 3-3,-1 0-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,0 0 0,-4 1 1,2-1-49,1 1-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,-2 3 0,-26 53 288,29-55-282,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 3 0,-2-6-1,1 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1-1 1,0 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1-1,0-2 1,28-18 375,-24 14-345,0 0 0,-1 0 0,0 0 0,-1-1 0,1 1 0,-1-1 0,-1 0 0,1 0-1,-1 0 1,2-14 0,-4 20-3,0 42-709,0-38 690,0 4 12,0 1 1,0 0 0,1 0-1,0 0 1,0-1 0,1 1-1,2 8 1,-3-14-14,0 0 1,1 1 0,-1-1-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 0-1,0 1 1,1-1-1,-1-1 1,1 1 0,0 0-1,-1-1 1,1 1-1,0-1 1,-1 0 0,6 0-1,-4 1 5,1-1-1,-1-1 1,0 1-1,1 0 1,-1-1 0,0 0-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,-1-1 1,4-3-1,0 0-10,0-1-1,-1 1 0,0-2 0,-1 1 0,1-1 0,-2 0 1,7-11-1,-3-1-58,0 0 1,-1 0-1,-1-1 1,-1 0-1,-1 0 0,2-24 1,-6 45 49,2-15 35,-1 1 0,-1-1 0,0 0 0,-1 0 0,-4-20 0,5 34-26,0 1 0,0-1 0,0 1-1,0 0 1,-1-1 0,1 1 0,0-1-1,0 1 1,0-1 0,0 1-1,-1 0 1,1-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1-1,1 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,-14 12-47,-7 25 27,15-14 112,1 1 0,1-1 1,1 1-1,1 0 0,-1 34 0,4-47-80,0 1 0,1-1 0,0 0-1,1 1 1,0-1 0,7 21-1,-8-29-30,0-1-1,1 1 0,-1 0 1,1-1-1,0 1 0,-1-1 0,1 1 1,1-1-1,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1-1 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0-1 1,6 0-1,-4-1-48,1 1 1,-1-1-1,0 0 0,0-1 0,0 0 1,0 1-1,0-2 0,-1 1 1,1 0-1,-1-1 0,0 0 1,0 0-1,5-6 0,0-1-1,-1 0 0,0 0 0,0-1 0,8-17 0,11-59-284,-33 133 636,1-18 34,-1 47 1,6-71-294,0 2 15,0 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,0 0 1,2 5-1,-2-9-40,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 0-1,2 0 1,0-1-43,0 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,-1-1 1,0 1-1,1-1 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1 0 1,3-5-1,-3 4-607,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-10 0,-1-12-3576</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2060.31">1192 113 1585,'0'0'17112,"-7"2"-20058,7 12-767,0 4-3251</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2556.23">1193 508 9124,'0'0'7753,"11"3"-6891,37 11-137,-45-14-679,0 1-1,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 1,0-1-1,0 0 1,0 1-1,3-4 1,2-3-1,-1 0 0,0 0 0,0 0 0,5-12 0,-9 17-28,12-27-438,-2-1 1,0-1-1,-2 0 0,-2 0 1,7-54-1,-11 23 3503,-4 76-3592,-11 138 1016,1 0-190,8-129-365,0-3-3114</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4664.44">1352 362 12166,'0'0'6923,"22"-11"-6523,101-7-106,-64 10-1205,77-19-1,-153 27 4392,-18 10-3814,27-7 350,1 1 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 1 0,0-1 1,1 1-1,-1 0 0,1 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,1 0 0,-1 1 1,1-1-1,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,0 0 0,0 9 1,1-17-19,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,20-2 120,16-14 209,-25 7-304,-1-1 0,-1 0 0,0-1 0,0 0 0,-1 0 0,0-1 0,-1 0 0,-1 0 0,8-16 0,-17 160 673,2-131-691,0 0-1,0-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,-1 1-1,1 0 1,1-2-1,3 0 38,0 0 1,0 0-1,0-1 0,0 0 0,0 0 1,5-4-1,7-11-85,-1-1 0,-1 0 0,0-1 0,-2 0 0,0-1 0,-2-1 0,0 0 0,15-46 0,-23 56-14,-1-1-1,0 1 1,-1-1 0,-1-22-1,0 29 73,0 5-12,-1 27-689,-3 22 805,-9 159 779,13-203-888,0-1 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,0-1 1,0 1-1,0-1 0,1 0 0,-1 1 0,0-1 1,1 0-1,0 0 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,6 0 0,-4 0 2,1-1-1,-1 1 1,1-1-1,-1 0 0,1-1 1,-1 0-1,1 1 1,-1-2-1,1 1 1,-1-1-1,0 1 1,0-2-1,0 1 1,0 0-1,0-1 1,0 0-1,0 0 1,6-6-1,-5 2-22,0 1 0,-1-1-1,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,-1-1 0,0 1-1,-1-1 1,0 0-1,0-12 1,-1 20-21,0 30-662,0 93 961,0-121-267,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 1,0 1 0,0 0-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 1,1-1 0,2 0 33,-1 0 1,1-1-1,0 1 1,-1-1-1,1 0 1,-1 0 0,0 0-1,0-1 1,4-2-1,2-6-101,0-1-1,0 0 1,-1 0-1,-1 0 1,0-1-1,-1-1 1,0 1-1,-1-1 1,7-25-1,-9 192 522,-3-153-444,0 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1-1 0,22 0 223,-19-1-214,-1 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,3-5 0,31-49 0,-13 18-60,-15 28 25,-7 9 10,1-1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,0 1 1,1-5-1,-2 8 16,0 26-498,-3 57 856,3-82-363,1-1 1,-1 1-1,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,1-1 0,35-10 166,-28 5-141,1-1 1,-1 1 0,0-2 0,-1 1 0,14-16 0,-19 19-34,0 0 0,0-1 0,0 0 0,0 1 0,-1-1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 1,0-1-1,0 1 0,0-11 0,-3 16-3,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,-3 1 0,-1 2-1,0 0 0,0 1-1,0-1 1,1 1 0,-1 1-1,1-1 1,1 1 0,-1-1-1,1 1 1,-5 9 0,6-11-7,1 1 0,-1 0-1,1-1 1,0 1 0,0 0 0,1 0 0,0 0 0,-1 0-1,2 0 1,-1 0 0,0 1 0,1-1 0,0 0 0,0 0 0,2 8-1,-1-12 7,0 0-1,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,0 0 0,1 0 1,2 0-1,43 0-491,-33 0 110,-6 0-9,1-1-1,0 1 1,0-2-1,-1 1 1,1-1-1,-1 0 1,13-6-1,28-20-6227,-28 11-1017</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4664.43">1352 362 12166,'0'0'6923,"22"-11"-6523,101-7-106,-64 10-1205,77-19-1,-153 27 4392,-18 10-3814,27-7 350,1 1 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 1 0,0-1 1,1 1-1,-1 0 0,1 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,1 0 0,-1 1 1,1-1-1,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,0 0 0,0 9 1,1-17-19,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,20-2 120,16-14 209,-25 7-304,-1-1 0,-1 0 0,0-1 0,0 0 0,-1 0 0,0-1 0,-1 0 0,-1 0 0,8-16 0,-17 160 673,2-131-691,0 0-1,0-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,0 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,-1 1-1,1 0 1,1-2-1,3 0 38,0 0 1,0 0-1,0-1 0,0 0 0,0 0 1,5-4-1,7-11-85,-1-1 0,-1 0 0,0-1 0,-2 0 0,0-1 0,-2-1 0,0 0 0,15-46 0,-23 56-14,-1-1-1,0 1 1,-1-1 0,-1-22-1,0 29 73,0 5-12,-1 27-689,-3 22 805,-9 159 779,13-203-888,0-1 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,0-1 1,0 1-1,0-1 0,1 0 0,-1 1 0,0-1 1,1 0-1,0 0 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,6 0 0,-4 0 2,1-1-1,-1 1 1,1-1-1,-1 0 0,1-1 1,-1 0-1,1 1 1,-1-2-1,1 1 1,-1-1-1,0 1 1,0-2-1,0 1 1,0 0-1,0-1 1,0 0-1,0 0 1,6-6-1,-5 2-22,0 1 0,-1-1-1,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,-1-1 0,0 1-1,-1-1 1,0 0-1,0-12 1,-1 20-21,0 30-662,0 93 961,0-121-267,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 1,0 1 0,0 0-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 1,1-1 0,2 0 33,-1 0 1,1-1-1,0 1 1,-1-1-1,1 0 1,-1 0 0,0 0-1,0-1 1,4-2-1,2-6-101,0-1-1,0 0 1,-1 0-1,-1 0 1,0-1-1,-1-1 1,0 1-1,-1-1 1,7-25-1,-9 192 522,-3-153-444,0 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1-1 0,22 0 223,-19-1-214,-1 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,3-5 0,31-49 0,-13 18-60,-15 28 25,-7 9 10,1-1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,0 1 1,1-5-1,-2 8 16,0 26-498,-3 57 856,3-82-363,1-1 1,-1 1-1,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,1-1 0,35-10 166,-28 5-141,1-1 1,-1 1 0,0-2 0,-1 1 0,14-16 0,-19 19-34,0 0 0,0-1 0,0 0 0,0 1 0,-1-1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 1,0-1-1,0 1 0,0-11 0,-3 16-3,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,-3 1 0,-1 2-1,0 0 0,0 1-1,0-1 1,1 1 0,-1 1-1,1-1 1,1 1 0,-1-1-1,1 1 1,-5 9 0,6-11-7,1 1 0,-1 0-1,1-1 1,0 1 0,0 0 0,1 0 0,0 0 0,-1 0-1,2 0 1,-1 0 0,0 1 0,1-1 0,0 0 0,0 0 0,2 8-1,-1-12 7,0 0-1,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,1 1 1,-1-1-1,0 0 0,1 0 1,2 0-1,43 0-491,-33 0 110,-6 0-9,1-1-1,0 1 1,0-2-1,-1 1 1,1-1-1,-1 0 1,13-6-1,28-20-6227,-28 11-1017</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5140.53">1741 245 1697,'0'0'13510,"-14"6"-13158,21-2-192,11-4 80,7 2 609,10-2 63,8 0-496,-1 0-416,8-8-2049,-8 0-4033</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5317.82">2138 219 10869,'0'0'7876,"29"-4"-9349</inkml:trace>
 </inkml:ink>
@@ -8628,9 +8628,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">852 124 13654,'0'0'6710,"26"45"-6064,40 86 87,-72-129-650,0 0-1,0 0 1,-1-1 0,1 0-1,0 0 1,0 0-1,-9-1 1,10 0-29,-84 11-47,81-9-24,0 0 0,1 0-1,-1 0 1,1 1 0,-1 0 0,1 0-1,0 1 1,0 0 0,-6 5 0,13-9-96,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,12 0-6415</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="496.48">1214 127 11605,'0'0'7214,"0"5"-6637,0 5-508,-1 0 147,1 0 0,1-1 0,0 1 0,4 17 0,-5-25-176,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 0 0,3 0 0,-3 0 6,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 1,1-1-1,14-40 401,-13 39-393,0-8 18,0 0 0,0 0 0,-1 0 1,-1-19-1,0 22 77,0 9-172,0-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,-9 6-2575,2 5-1333,3 0-3769</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="496.47">1214 127 11605,'0'0'7214,"0"5"-6637,0 5-508,-1 0 147,1 0 0,1-1 0,0 1 0,4 17 0,-5-25-176,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1 0,0 0 0,3 0 0,-3 0 6,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 1,1-1-1,14-40 401,-13 39-393,0-8 18,0 0 0,0 0 0,-1 0 1,-1-19-1,0 22 77,0 9-172,0-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 1,-9 6-2575,2 5-1333,3 0-3769</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1436.88">1399 132 7796,'0'0'12848,"1"4"-12562,2 85 2168,-3-88-2443,0-1 1,0 0-1,1 0 0,-1 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,1 1-1,-1-1 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,1-1 0,13-9 111,72-65-472,-85 77 345,0 0 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 4 0,2 40 308,0-46-300,0 1 1,-1 0-1,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,1-2 0,29-18 27,-27 16-40,0 0-1,-1 0 0,1 0 0,-1-1 0,1 1 1,-2-1-1,1 0 0,0 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,-1-1 0,0 1 0,0-1 0,0 1 1,-1-1-1,1 1 0,-2-9 0,1 14 9,4 37-855,20 11 918,1 0 48,-24-45-103,0 0-1,0-1 0,0 1 1,0 0-1,-1 0 0,0-1 1,1 1-1,-1 0 1,0 0-1,0 0 0,0-1 1,-1 1-1,1 0 1,-2 5-1,1-7 14,-1 1-1,1 0 1,0-1-1,-1 1 1,0-1-1,1 0 1,-1 1-1,1-1 1,-1 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 1-1,-4-2 1,12-18-414,5 3-289,1 0 0,0 1-1,1 1 1,25-21 0,-18 16-557,32-36 1,-47 49 1045,0-1 1,-1 0-1,1 0 1,-2 0-1,1-1 1,-1 1 0,0-1-1,0 0 1,-1 0-1,2-9 1,-10 67 8024,-9 162-7147,15-209-1438,0 19 75,1-14-8239</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1608.17">1802 178 14006,'0'0'9285,"21"-33"-9958,8 27 561,6 2-192,1 0-1233,-4 4-431,-4 0-482,-14 0-4673</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1608.16">1802 178 14006,'0'0'9285,"21"-33"-9958,8 27 561,6 2-192,1 0-1233,-4 4-431,-4 0-482,-14 0-4673</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2725.3">1959 140 10373,'0'0'6984,"0"11"-6221,1-1-426,0-1 0,0 1-1,1 0 1,0-1 0,0 1-1,1-1 1,1 1 0,-1-1-1,10 16 1,-10-21-161,-1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,0 1 0,0 0 0,1 7-1,-2-11-114,0 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0 0,0 0-1,0-1 1,-1 1-1,0 0 1,1-3-35,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,2-5 1,1 2-140,1 0 0,-1 0 1,1 1-1,0 0 0,0 0 1,0 0-1,1 0 0,0 0 1,0 1-1,0 0 0,0 0 0,8-3 1,73-38-1804,-86 44 1907,1 1-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-1,-1 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 1,1 1-1,-1 0 0,8 30 179,-6-21-119,-1-7-52,1 0-1,-1 0 1,1-1 0,0 1-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0-1-1,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,4-1 1,-1 0-144,1-1 0,-1 1 1,0-1-1,0-1 0,0 1 0,0-1 0,0 0 1,-1 0-1,0-1 0,0 1 0,0-1 1,0 0-1,-1-1 0,0 1 0,7-11 0,-31 70 3287,18-50-3124,1 1 1,0-1-1,0 1 0,0-1 1,0 0-1,1 1 0,0-1 0,0 1 1,0 0-1,1-1 0,1 9 1,3-12-52,1 0-1,-1 0 1,1 0 0,-1-1 0,1 0 0,0 0-1,-1 0 1,8-2 0,-10 2-58,10-2-309,0 0 0,0 0 0,-1-1 0,18-7 0,-24 8 124,-1 0-1,0 0 1,0-1 0,1 0 0,-1 0 0,-1 0 0,1 0-1,0-1 1,-1 0 0,0 0 0,0 0 0,5-6 0,-4-7 1292,-5 13 1065,-6 11-1342,-6 13-183,8-17-462,1 1 0,1-1 0,-1 1 0,0 0 0,1 0 0,0 0 1,0 0-1,0 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,0 1 1,1-1-1,-1 1 0,1 0 0,0-1 0,0 1 0,2 6 0,-2-11-89,1 1 0,0 0-1,0-1 1,-1 1 0,1 0 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,2 0-1,25-2 69,-17 0-85,-1-1 0,0 0 0,0 0 0,0-1 0,-1 0 0,1-1 0,-1 0 0,0-1 0,0 0 0,11-10 0,-7 5-515,-1 0 1,0-2-1,-1 1 1,0-1-1,17-27 0,-22 27 88,0 1-1,0-1 0,-1 0 1,-1-1-1,5-25 0,-2-32 4158,-9 82-3508,1 0 1,-1 0-1,-1-1 1,0 1-1,-9 19 1,-8 33 897,17-45-1021,0 0 0,1 0 0,1 1 1,1-1-1,3 34 0,-2-50-186,0 0 1,-1 0-1,1 0 0,0 1 0,1-1 1,-1 0-1,0-1 0,0 1 0,1 0 1,-1 0-1,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1-1 0,4 1 0,-4 0-286,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,2-2 0,5-11-6529</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3150.37">2778 262 6723,'0'0'11077,"-13"-2"-10402,-39-6-392,39 6-299,43-5-678,16-5 600,-30 7 151,-1 1 1,1 0 0,-1 1 0,23-1 0,-37 7 98,0-1 0,0 1 1,0 0-1,0-1 0,-1 1 0,1 0 0,-1 0 1,0-1-1,0 1 0,0 0 0,-1 5 0,1-5 27,0 3-42,0 1 1,0 0-1,1-1 1,0 1-1,0 0 0,4 10 1,-4-16-130,-1 0 0,1 0-1,-1 0 1,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 1,1 0 1,0-1 0,0 1-1,-1 0 1,1-1 0,0 1 0,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,3-3-1,7-5 34,1-1 0,-1-1 1,11-14-1,-19 21-86,0 0 0,0-1 1,0 1-1,0-1 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1 0 1,0-1-1,0 1 0,0 0 1,0-7-1,-3 12-469,1 0 1,-1 0-1,0 0 0,0 0 1,0 1-1,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,0 1 1,-2 1-1,-6 6-5455</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3456.97">3082 267 15015,'0'0'2756,"10"12"-1977,31 40-24,-40-50-677,1-1-1,-1 1 1,0 0 0,1-1 0,-1 1 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 4 0,0-5 9,0 0 1,0 0-1,0-1 1,1 1-1,-1-1 1,0 1-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 0-58,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,2-2 0,-2-1-244,1 0-1,0 0 1,0 1-1,0-1 0,1 0 1,0 1-1,2-6 1,31-27-4743,-7 19-1459,-13 13-185</inkml:trace>
@@ -8640,7 +8640,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6148.2">1143 1063 13238</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7389.64">1143 1063 13238,'45'37'1331,"-43"-36"-1135,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,0 0 0,-1 0 0,4-3 0,-3 2-73,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,-1-5-1,1-4 428,0 12-522,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0-1,-11 5 222,-10 13-352,18-13 114,-1 1 0,2 0-1,-1 0 1,0 0 0,1 1-1,0-1 1,1 1 0,-1-1-1,1 1 1,1 0 0,-1 0-1,1 0 1,0 0 0,1 1-1,0 12 1,1-18-12,0 0 1,0-1-1,0 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,1-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 1 1,0-1-1,-1 1 0,1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,3 0-1,55-2-23,-52-1-195,-1 0 0,1 0 1,-1-1-1,0 1 0,0-2 1,-1 1-1,1-1 0,-1 0 0,0 0 1,0-1-1,0 0 0,-1 0 0,0 0 1,5-9-1,8-8 264,-13 95 1433,-5-72-1472,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 1,10-11 109,18-26-469,-18 22 167,-4 6 9,-6 8 144,0-1-1,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 1,1 1-1,0-1 1,-1 1-1,1 0 0,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0 0-1,4-1 1,-5 5 45,0 0 0,0-1 0,0 1 1,-1 0-1,1 0 0,-1-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 3 0,1-4 29,0 93 2017,2-101-2024,0-1 0,0 1 0,1 0 0,0-1-1,0 1 1,0 1 0,7-10 0,-2 3-160,28-33-506,-34 42 590,1 1 0,-1-1-1,1 1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,4-1-1,-6 2-68,-1 25-123,1-19 249,0 1 59,0-1-1,0 0 1,0 0 0,0 0 0,1 0 0,5 10 0,-7-15-61,0-1 1,1 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,-1 1-1,2-1 1,0 0 0,0-1 1,0 1-1,0 0 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,4-2-1,51-41 80,-56 98-32,1-33 345,-1-15-313,3 28 211,-2-33-303,-1 0 0,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1-1,0 0 1,-1 1-1,1-1 1,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,-1-1-1,1 1 1,0-1 0,-1 1-1,1 0 1,0-1-1,-1 1 1,1-1-1,0 0 1,6-4-22,-1 0 0,1 0 0,-1-1 1,0 0-1,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 1,-1-1-1,0 1 0,-1 0 0,0-1 0,0 0 0,0 0 1,-1 0-1,0 0 0,1-16 0,-3 23-14,0 19-325,-4 81 282,4-98-29,0-1 1,0 0-1,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,1 0 1,-1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,7-7-4354</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7560.3">1959 928 14583,'0'0'10757,"-7"-10"-10757,4 10-3698,-4 0-672,0 6-6787</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8209.46">2076 1115 9861,'0'0'14550,"-14"8"-14022,14-6-400,0 2-128,7 1 0,4-1 0,7-4 0,10 0-16,0 0-400,8 0-2465,-1 0-1521,-10-4-6675</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8209.45">2076 1115 9861,'0'0'14550,"-14"8"-14022,14-6-400,0 2-128,7 1 0,4-1 0,7-4 0,10 0-16,0 0-400,8 0-2465,-1 0-1521,-10-4-6675</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8758.53">2487 1099 8980,'0'0'12699,"3"-10"-11842,1 3-585,-3 4-151,1-1-1,0 1 1,-1-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0 0,-1-7-1,-3 10-63,0 0 0,0 0-1,-1 0 1,1 0 0,0 1-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-6 2 0,6-1-63,1 1 1,-1-1 0,1 0 0,-1 1 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,1 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0 0 1,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,1 0-1,-1-1 1,1 1 0,0 0 0,0-1 0,0 1 0,0 0-1,1-1 1,-1 0 0,1 1 0,0-1 0,0 0 0,4 5-1,38 28 0,-35-29-14,1 0-1,-2 0 0,1 1 1,12 14-1,-21-22 14,0 0 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 0,0 1 1,1-1-1,-1 1 0,0-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,-1 1 0,1 0 0,-19 6 0,-33-6 201,43-1-183,8 0-30,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-2-1 0,3 1-158,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 1-1,0-1 1,-1 0-1,2-1 1,15-14-4744,9-4-3870</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9021.57">2717 927 6371,'0'0'15644,"0"4"-15580,-3 44 1331,-10 59 0,2-25-1479,6 0-5746</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9188.72">2656 1121 13062,'0'0'10709,"8"-29"-11125,13 23-17,7 0-175,4 0-1473,0 2-288,-4 0-2641,-6 2-4466</inkml:trace>
@@ -8717,7 +8717,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">207 0 9428,'0'0'10285,"-26"5"-9274,13 3-987,0 1 0,0 1 0,1 0 0,0 0 0,0 1 0,1 1 0,1 0 0,0 0 0,1 1 0,0 0 0,1 1 0,0 0 0,1 0 0,1 1 0,0-1 0,1 2 0,1-1 0,0 0 0,1 1 0,1 0 0,0-1 0,1 1 0,1 0 0,2 25 0,-1-38-194,-1 0-1,1 0 1,0 0-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 0,1 0 1,4 2-1,-2-1-615,1-1 0,-1 1-1,1-1 1,0 0 0,-1-1 0,1 0-1,0 1 1,10-1 0,19 0-6412</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="731.12">464 164 6451,'0'0'8983,"-10"-11"-8282,3 11-594,0 0 0,0 0 0,0 0 0,1 1 1,-1 0-1,0 0 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,1 1 0,0 0 0,0-1 0,1 2 0,-1-1 0,1 0 0,0 1 0,-5 11 0,6-9 26,0 0 1,1 0-1,0 0 1,0 0-1,1 1 0,0-1 1,1 0-1,0 1 1,0-1-1,0 1 0,4 13 1,-4-21-122,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,3 1 1,37 2-4187,-28-4-685,-8 1-807</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2170.28">551 313 5891,'0'0'7528,"3"-4"-6660,0 2-413,8-10-316,-7 0 3554,-5 11-3614,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,-1 1 0,-29-1-462,26 0 467,2 0-94,1 0-1,0 0 1,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,1 0 1,0 0-1,-2 2 1,1 1-63,-1-1 0,1 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 9-1,5-13-36,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-2 0,0 1 0,4-1 0,-1-1-15,-1-1 1,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,-1-1 0,0 1 0,5-7-1,-13 20 350,1 1-1,1-1 1,-1 1-1,1 0 0,1 0 1,0 0-1,0 0 1,1 13-1,2-22-173,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,2-1-1,6-3 0,0-1 0,-1 0 1,0-1-1,-1 0 0,1 0 0,-2-1 0,1 0 1,-1 0-1,0-1 0,0 0 0,-1 0 0,0 0 0,6-15 1,-5 9-111,-1-1 1,0 0 0,-1 0 0,0 0 0,-1-1 0,-1 0 0,-1 1 0,0-20 0,-2 35-91,-5 8-87,1 1 205,0 0 1,0-1-1,0 2 0,1-1 0,0 0 0,1 1 0,0-1 1,-1 11-1,-2 1 105,0-1 145,1 1 0,1-1 0,1 1 0,1 0 0,0-1 0,4 30 0,-3-48-203,1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,2-1 0,51-7 376,-46 5-357,-1-1 1,0 0 0,0 0 0,0-1 0,0 0-1,-1 0 1,0-1 0,8-8 0,-11 10-111,-1 0 0,0 0 0,1 0 0,-2 0 0,1 0 0,0-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-9 0,-3 14 44,1 0 1,0 0-1,-1 1 1,1-1-1,-1 0 0,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,-1 1 1,-1 2-1,0 1 5,0 0 0,0 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 1-1,1-1 1,0 0 0,0 1 0,1-1 0,1 8 0,-1-12-50,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,0 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 0 0,1 1-1,-1-1 1,2 0 0,30 0-4449,-19-4-77</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2170.27">551 313 5891,'0'0'7528,"3"-4"-6660,0 2-413,8-10-316,-7 0 3554,-5 11-3614,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,-1 1 0,-29-1-462,26 0 467,2 0-94,1 0-1,0 0 1,-1 1-1,1-1 1,-1 1 0,1 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,1 0 1,0 0-1,-2 2 1,1 1-63,-1-1 0,1 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 9-1,5-13-36,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-2 0,0 1 0,4-1 0,-1-1-15,-1-1 1,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,-1-1 0,0 1 0,5-7-1,-13 20 350,1 1-1,1-1 1,-1 1-1,1 0 0,1 0 1,0 0-1,0 0 1,1 13-1,2-22-173,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,2-1-1,6-3 0,0-1 0,-1 0 1,0-1-1,-1 0 0,1 0 0,-2-1 0,1 0 1,-1 0-1,0-1 0,0 0 0,-1 0 0,0 0 0,6-15 1,-5 9-111,-1-1 1,0 0 0,-1 0 0,0 0 0,-1-1 0,-1 0 0,-1 1 0,0-20 0,-2 35-91,-5 8-87,1 1 205,0 0 1,0-1-1,0 2 0,1-1 0,0 0 0,1 1 0,0-1 1,-1 11-1,-2 1 105,0-1 145,1 1 0,1-1 0,1 1 0,1 0 0,0-1 0,4 30 0,-3-48-203,1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,2-1 0,51-7 376,-46 5-357,-1-1 1,0 0 0,0 0 0,0-1 0,0 0-1,-1 0 1,0-1 0,8-8 0,-11 10-111,-1 0 0,0 0 0,1 0 0,-2 0 0,1 0 0,0-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-9 0,-3 14 44,1 0 1,0 0-1,-1 1 1,1-1-1,-1 0 0,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,-1 1 1,-1 2-1,0 1 5,0 0 0,0 1 0,1-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 1-1,1-1 1,0 0 0,0 1 0,1-1 0,1 8 0,-1-12-50,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,1 0-1,-1-1 1,0 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 0 0,1 1-1,-1-1 1,2 0 0,30 0-4449,-19-4-77</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2429.43">560 209 12774,'0'0'4530,"110"0"-4530,-71 0-320,-4 0-1233,-3 0-2273,0 0-4017</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3356.72">1117 284 9076,'0'0'9367,"-4"-7"-8158,4 6-1207,-1-1 25,0 0 0,1 0-1,-1 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 1 1,-1 0 0,1 0-1,0-1 1,-1 2 0,1-1-1,-4 0 1,4 0-52,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,-1 2 1,2-4-22,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,2-1 0,0 1 81,0 0 0,0-1 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,-1 0 1,3-3-1,4 148 717,-6-109-584,0-11-165,0 1 0,-2 0 0,-6 44 1,6-64 44,-1 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,-1 0 0,0-1-1,0 1 1,-1-1 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,0 0-1,-1-1 1,1 0 0,-10 3-1,13-4-9,-1 0-1,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0-1 0,0-4-276,0 1-1,1 0 1,0 0-1,0 0 1,0 0-1,1 0 1,0 0-1,0 1 1,0-1-1,1 0 1,0 1-1,6-10 1,7-1-1407,1 0 0,0 2 0,1 0-1,34-20 1,-25 16-1575,41-32-1,-30 8 3645,-33 35 498,-1 0 0,1 0-1,-1-1 1,4-13 0,-6 5 7040,-12 23-6434,-12 24-1870,20-28 356,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 1-1,1-1 1,0 0 0,0 1 0,0-1-1,1 0 1,-1 0 0,1 1 0,0 2-1,0-4-2,0 0 0,0-1-1,0 0 1,0 1-1,0-1 1,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1-1,1 1 1,0-1 0,0 0-1,0 0 1,-1 0 0,4 0-1,-2-1 37,0 1 1,0 0-1,0 0 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 1,-1 0-1,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 1,-1 0-1,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,-1-4-1,0 5-43,1 0 1,0 0-1,-1 0 1,0 1-1,1-1 0,-1 1 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,-4 0 1,-14 5-6877</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3793.99">1352 281 5282,'0'0'9365,"13"5"-8597,42 17-42,-53-21-684,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 3 0,-2 36 825,0-27-247,1-13-548,0 0 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 0,-1-1 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,-1 0 1,-1 1-1,2-2 449,9-9 231,31-32-1070,2 2-1,62-46 1,-101 93 561,0-1 0,-1 0 0,0 0 1,0 1-1,0 7 0,-1 12-75,0 13 75,0-14-4015</inkml:trace>
@@ -8753,9 +8753,9 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">294 9 16968,'0'0'1763,"-13"-2"-664,3 0-898,5 1-146,1 0-1,-1 0 0,0 0 1,1 1-1,-1 0 0,0 0 1,1 0-1,-1 0 0,0 1 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 1-1,1 0 0,0 0 0,-1 0 1,-3 3-1,-10 8 121,1 0 1,1 1-1,0 1 0,1 1 1,1 0-1,-21 31 0,28-37-143,1 1 0,0 0 0,1 0 0,0 0 0,1 1 0,0 0 0,1 0 0,0 0 0,1 0 0,0 0 0,1 0 0,1 1 0,0 15 0,1-22-99,0-1 0,0 0 0,1 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,1-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,1 0 0,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0 0,1-1 0,0 0 0,0 0-1,8 3 1,7 0-1504,0 0 0,1 0 0,0-2 0,41 1 0,-4-3-6748</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="324.3">525 161 14231,'0'0'7205,"-10"41"-6892,-24 101 452,17-62-1869,16-76 17,-1 5 371,2-6-2892</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="563.42">489 168 6723,'0'0'10269,"1"0"-10254,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,1 1 1,-1-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,1 0-1,-1 0 1,1 1 0,1 4 149,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 0-1,1 10 1,4 12 274,-2-13-824,0 3 743,1 0 0,1 0 0,1-1 0,10 19 0,-14-31-668,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,1 1 0,8 5 0,-8-6-515,-1-1 1,1-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,-1 0 0,1 0-1,0-1 1,0 1 0,7-1-1,-4 0-6303</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="563.41">489 168 6723,'0'0'10269,"1"0"-10254,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,1 1 1,-1-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,1 0-1,-1 0 1,1 1 0,1 4 149,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 0-1,1 10 1,4 12 274,-2-13-824,0 3 743,1 0 0,1 0 0,1-1 0,10 19 0,-14-31-668,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,1 1 0,8 5 0,-8-6-515,-1-1 1,1-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,-1 0 0,1 0-1,0-1 1,0 1 0,7-1-1,-4 0-6303</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="805.29">695 114 13382,'0'0'4213,"-6"16"-3394,-6 22-252,1 1 1,2 0 0,1 1 0,-3 70-1,11-102 312,2 12-4683,-1-20 3489,-1 1 0,1-1-1,-1 0 1,1 1 0,0-1-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,2-1 0,12-4-4797</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1121.65">744 282 6755,'0'0'10010,"0"-10"-9805,-7 59 728,4-41-666,1 1 0,0-1 0,1 1 1,0 0-1,0 0 0,1-1 0,0 1 0,1 0 1,2 16-1,-2-24-245,0 1 0,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,1-1 0,-1 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,1-1 0,1 0 0,1-1 64,0 0 0,1 0 0,-1 0-1,0-1 1,0 0 0,-1 1 0,1-1 0,0-1-1,5-5 1,-4 1-12,0 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,-2 0 1,1 0-1,2-17 1,-2-17-3133,-10 40-3597,0 3-1115</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1121.64">744 282 6755,'0'0'10010,"0"-10"-9805,-7 59 728,4-41-666,1 1 0,0-1 0,1 1 1,0 0-1,0 0 0,1-1 0,0 1 0,1 0 1,2 16-1,-2-24-245,0 1 0,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,1-1 0,-1 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,1-1 0,1 0 0,1-1 64,0 0 0,1 0 0,-1 0-1,0-1 1,0 0 0,-1 1 0,1-1 0,0-1-1,5-5 1,-4 1-12,0 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,-2 0 1,1 0-1,2-17 1,-2-17-3133,-10 40-3597,0 3-1115</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2572.15">929 274 1153,'0'0'14035,"0"11"-13336,0 8-174,-1 0 0,-1 0-1,0-1 1,-2 1 0,-8 27-1,6-28 157,9-18 11,15-26 203,-5 6-1183,-5 11 214,0-3-184,1 0-1,1 1 1,0 0-1,0 1 0,1 0 1,0 1-1,24-15 1,-34 24 260,-1 0 1,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,-1 2-1,2 30 327,-2-26-261,2 1 90,-2 0 1,1 0-1,-1 0 1,0-1 0,0 1-1,-1 0 1,0 0-1,0-1 1,0 1 0,-7 10-1,20-31-128,0 1 0,1 1 0,0 0 0,1 1 0,0 0 0,0 1 0,28-16 0,-40 35-16,1-1 0,-1 1 0,0 0-1,-1-1 1,-1 15 0,1-18 13,0-2 16,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,0 0 0,1 0 0,2 5 1,-2-6-3,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 1,0-1-1,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0-1 0,3 1 0,-1 0-37,1-1-1,-1 1 0,0-1 1,0 0-1,0 0 0,0-1 0,-1 0 1,1 1-1,0-2 0,0 1 0,-1 0 1,0-1-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,2-5 0,0-1-264,0-1-1,-1 0 1,0 0 0,0-1-1,-2 1 1,0-1 0,0 1-1,0-23 1,-2 34 251,0 1 1,-1-1-1,1 1 0,0-1 1,0 1-1,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 1,-1 0-1,1-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,0-1 0,-1 1 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,-1 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,0 1 1,-23 14-299,20-10 382,1 1 1,-1 0-1,1 0 0,0 0 1,0 0-1,1 1 0,0-1 1,0 1-1,0-1 0,-1 13 1,-1 69 831,4-87-871,1-1 1,0 1-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 1-1,0 0 1,0-1 0,0 0-1,-1 1 1,1-1 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1-1 0,30-5 358,-25 3-376,0-1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0-1,0-1 1,-1 1 0,0-1 0,5-11 0,33-44-289,-40 67 171,-1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,0 0-1,0 6 1,0 90 1055,0-100-938,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,-1 0 0,3-1 0,32-9 207,-28 5-239,-1 0 0,1-1 0,-1-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,0-1 0,0 1 1,0-1-1,-1 0 0,0-1 0,0 1 0,-1 0 0,2-11 0,-4 19-6,-1 22-806,-13 24 817,11-42 51,1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 1,0-1-1,0 1 0,1 0 0,0 0 0,0 0 0,2 9 0,-1-13-34,0 0 0,0 0 0,0-1 0,1 1 0,-1 0-1,0 0 1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0-1,1 0 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,3-1 1,30-1-589,-31 1 229,1 0 0,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1-1 1,1 1-1,-1 0 0,0-1 0,4-3 0,-1-1-1139,-1 0-1,1-1 0,-1 1 0,0-1 0,3-10 0,4-15-4720</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2712.53">1763 184 8868,'0'0'10837,"0"-20"-11109,0 24-352,-4 6-881,1 2-256,3 3-2417,0-1-928</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3745.59">1776 197 9172,'83'69'2500,"-67"-57"1822,-38-4-2028,15-2-2082,1 1-1,-1 0 0,1 1 1,0-1-1,1 1 0,0 0 1,0 1-1,0-1 0,1 1 1,1 0-1,0 0 0,0 0 1,0 0-1,1 0 0,1 1 1,-1-1-1,2 1 0,-1 15 1,1-24-205,0 0 1,1-1 0,-1 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 1-1,0-1 1,1 0 0,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0 0,-1 0-1,1 0 1,0 1 0,25-2 340,22-16-59,37-39-914,-61 38-499,0 2 0,50-26 1,-69 41 1085,3 14 1406,-9-14-592,-4-3-841,2 1 57,0 0 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 1,0 0-1,0 1 0,0-1 0,-1 0 1,1 1-1,0 0 0,0 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,1 1 0,-1 0 1,0 0-1,0 0 0,-6 5 0,5-4 41,-1 2 1,1-1-1,1 1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,1 1 0,-1-1 1,1 1-1,0 0 0,0 0 0,1 1 1,0-1-1,0 0 0,0 1 0,1-1 0,0 1 1,0 9-1,1-15-8,1-1 1,0 1-1,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1-1-1,0 1 0,1-1 0,35-4 315,-30 1-300,1 0 0,-1-1 0,0 0-1,0 0 1,0-1 0,0 0-1,-1 0 1,0 0 0,6-9 0,-9 11-13,-2 4-27,-1 36-451,-1-34 473,1-1 1,0 0-1,0 1 1,0-1-1,0 1 0,1-1 1,-1 0-1,0 1 1,0-1-1,1 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 0,0-1 1,1 1-1,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 0 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,0 0-1,1-1 1,-1 1-1,2-1 1,3-1 8,-1 1 1,1-1 0,0-1 0,-1 1-1,1-1 1,-1 0 0,0 0 0,0-1-1,0 1 1,5-6 0,0-3-61,-1 0-1,0 0 1,0-1 0,-2-1-1,1 1 1,-2-1 0,0 0-1,0-1 1,-2 1 0,0-1-1,0 0 1,-1 0 0,-1 0-1,0-18 1,-2 32-17,-2 10-263,-12 26 450,-11 43 0,22-66-98,0 0 1,1 0 0,0 1 0,1-1-1,1 0 1,0 0 0,1 1-1,2 12 1,-3-23-88,0-1 1,1 1-1,-1 0 0,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,1 0 0,-1 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 1,4 2-1,0-1-1011,0 0 0,0 0 0,0 0 0,0-1 0,0 0-1,0 0 1,7-1 0,6-2-8568</inkml:trace>
@@ -8849,7 +8849,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">61 1 6835,'0'0'9791,"-1"7"-9399,-10 88 2414,-37 140-1,50-249-2086,-1 0-1,0 0 1,-3-26-1,1 24-818,0 0 0,0 0 0,2 1 0,0-1-1,1 0 1,0 1 0,10-30 0,-12 44 84,0 1 0,0 0 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,14 9-83,10 24 311,-22-32-231,18 29 191,-2 0-1,0 1 1,14 41-1,-32-70-71,1 1-1599</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="281.55">210 67 9380,'0'0'11115,"0"-4"-10478,-1 59-72,-1 82 837,1-92-5364,1-5-4050</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="637.86">323 224 10229,'0'0'8692,"-2"5"-8474,-2 12 208,0-1 0,1 0 0,1 1 0,-1 29-1,4-45-414,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1 0,24-11 821,-21 7-763,1 0-1,-1-1 0,0 1 1,0-1-1,0 0 1,-1 1-1,1-2 0,-1 1 1,0 0-1,-1-1 1,0 1-1,1-1 0,-2 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0-10 1,-1 15-57,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-2 1 0,-22 3-256,18-1-474,1 0 1,-1 1-1,1-1 1,0 1-1,1 0 1,-9 9-1,1-1-3880,4-5-2048</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="637.85">323 224 10229,'0'0'8692,"-2"5"-8474,-2 12 208,0-1 0,1 0 0,1 1 0,-1 29-1,4-45-414,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1-1 0,1 1 0,24-11 821,-21 7-763,1 0-1,-1-1 0,0 1 1,0-1-1,0 0 1,-1 1-1,1-2 0,-1 1 1,0 0-1,-1-1 1,0 1-1,1-1 0,-2 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0-10 1,-1 15-57,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-2 1 0,-22 3-256,18-1-474,1 0 1,-1 1-1,1-1 1,0 1-1,1 0 1,-9 9-1,1-1-3880,4-5-2048</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1489.58">453 209 10389,'0'0'7939,"5"3"-7389,-3-2-469,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 3 0,3 51 1400,-4-50-1400,1 10 492,4-13-50,11-24 31,-5 4-806,-1 4 95,1 1 0,0 0-1,1 1 1,0 1-1,1-1 1,26-15 0,-39 26 171,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,8 22 318,-6 31 157,-3-50-407,0-4-73,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,19-16 68,-18 16-87,17-18-279,1 1 1,0 1-1,44-29 0,-63 46 260,1 44 119,-1-42-70,0-1 0,0 1 0,0 0 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1-1 1,3 2 0,-1-2-8,0 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0-1 0,-1 0 0,1 1 1,0-1-1,4-3 0,0 1-15,0-1-1,1 0 0,-2-1 1,1 0-1,0 0 0,-1 0 0,0-1 1,0 0-1,9-12 0,-15 17 116,0 23-373,-1 9 597,0-22-249,0 1 0,1 0-1,0-1 1,1 1 0,2 12-1,-3-22-130,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1 0-1,1-1 1,-1 1 0,1-1 0,-1 0-1,1 1 1,0-1 0,-1 1 0,1-1-1,-1 0 1,1 1 0,0-1 0,0 0-1,-1 0 1,1 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,0 1-1,-1 0 1,1-1 0,-1 1 0,1 0-1,0-1 1,24-17-8014,-16 2-1290</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1664.12">1066 33 15015,'0'0'4674,"-3"14"-18056</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2588.46">1114 180 15591,'0'0'5539,"1"12"-4507,5 62 518,-6-73-1529,0-1-1,0 1 1,1 0-1,-1-1 1,0 1 0,0-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,0 1 1,1-1 0,0 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,-1 1 0,1-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,-1-1 1,1 1-1,0 0 1,-1 0-1,1-1 1,-1 1 0,1 0-1,0-1 1,-1 1-1,1 0 1,0-2-1,32-14 1,-7-3 125,-14 9-139,0 1-1,1 1 1,0 0-1,26-11 1,-39 19-8,1 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,1-1 0,-1 1-1,0 0 1,0-1 0,0 1 0,-1 0-1,5 34 171,-1-15-42,-3-19-128,0 1 1,1 0-1,-1-1 1,1 1-1,-1-1 0,1 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1-1 0,1 1 1,2 0-1,-1-1-32,1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,1-1 1,-1 1-1,5-3 1,-5 2-21,7-3-148,0 0-1,0-1 0,-1 0 1,0-1-1,13-12 0,-52 31 747,20-4-560,14-11-1101,21-21-1087,9 76 4015,-32-51-1777,1 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0-1,0-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0-1 0,0 1 0,0 0 0,-1-1-1,1 0 1,0 1 0,-1-1 0,1 0 0,0 0-1,-1-1 1,1 1 0,-1 0 0,4-3 0,7-5 44,-1 0 0,1-1 1,12-14-1,-23 23-85,6-8-105,-1-1-1,0 0 0,0 0 1,-1-1-1,-1 0 0,0 0 0,0 0 1,-1-1-1,0 1 0,-1-1 1,0 0-1,-1 0 0,-1 0 0,0-1 1,-1-21-1,0 34 110,0 0 0,0 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0-1 0,-12 15-142,3 7 169,1-1 1,1 2-1,1-1 0,0 1 1,2 0-1,1 0 0,1 0 1,0 44-1,2-64-55,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0-1 0,1 2-1,21-1-6115,-5-6-1966</inkml:trace>
@@ -8888,7 +8888,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5365.48">2709 826 2289,'0'0'12926,"49"-4"-9167,311 15-1070,-39 0-2435,586-28 26,-811 11-161,585-21 1245,-681 68-1423,-1 73 286,-1-4 80,18 167 0,-6-196-23,-1 106 0,-38-210 303,-193-142-1086,227 173 435,0 0-1,0 1 1,-1 0-1,-1-1 1,4 11-1,20 46 236,-22-56-150,1-1-1,0 1 0,0-1 1,0 0-1,1 0 1,0-1-1,14 11 1,-18-16-5,0 0 0,-1 0 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,3-4 0,34-27-93,67-74 0,-20 5-4732,-83 97 4311,-1 3 80,-1-1 0,1 0 0,-1 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,0-4 0,0-7-5526</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7418.96">4723 2040 12950,'0'0'7982,"4"-4"-7304,-1 2-542,0-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1-1 0,-1 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 1,-2 1-1,0-7 0,0 9-114,0 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 1 0,-1-1 0,-34 7-51,26-3 14,1 1 0,-1 0 0,1 1 0,0 0 1,1 1-1,-1-1 0,1 2 0,0-1 0,1 2 0,0-1 0,0 1 0,1 0 0,0 0 0,1 1 0,0 0 0,0 0 0,1 1 0,1-1 0,0 1 0,0 0 0,1 0 1,0 1-1,1-1 0,-2 19 0,5-28-97,-1 1 0,0-1 1,1 1-1,-1-1 0,1 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,0 0 0,1-1 1,4 1-1,10 1-746,0 0 1,0-1-1,26-2 0,-20 0-15,-12 1 499,-1 0-1,0-1 0,0 0 0,0-1 0,0 0 0,-1-1 0,1 0 0,-1 0 0,1-1 0,8-5 0,-13 6 460,-1 0 1,0 0-1,0 0 0,0-1 0,0 1 1,-1-1-1,1 0 0,-1 0 0,3-5 0,-3 5 571,-1-1-1,0 1 0,0-1 0,0 0 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 0,-1-8 1,-1 18-647,1 1 0,-2-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,-5 10 1,5-12 4,0 0 0,0 1 0,0 0 1,0-1-1,1 1 0,0 0 1,-1 0-1,1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 4 1,1-6-10,-1-1 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 0 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 0,2-1 1,38-10 477,-38 9-390,-1-1 1,1 1-1,0-1 0,-1 0 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,-1-1-1,0 0 0,1 0 1,-1 0-1,-1-1 0,1 1 1,-1 0-1,0 0 1,1-1-1,-1-7 0,0 10-82,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0-1,0-1 1,-1 2 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1-1,-1-1 1,-3 1 0,5 0-53,-55 0-292,32 10-2251,23-9 2218,0 0 0,0 0 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,0 3 0,0 3-7418</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8191.25">5099 2142 12998,'0'0'5861,"0"10"-4924,1 2-740,0-2-45,0 0-1,-1 0 1,0 0 0,-1 1-1,-1 10 1,109-97-1406,-115 116 2703,7-34-1373,0-1-12,0 1 0,0 0 0,0 0 0,0-1 0,1 1 0,0 0 0,1 9 0,0-13-47,0 0-1,0-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 1,0 0-1,1 0 0,-1 1 1,0-1-1,0 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,4-1 0,4 1-18,-1 0-1,1-1 0,0-1 0,-1 1 0,1-1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 0 1,-1-1-1,1 0 0,-1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0-1 0,-1 0 0,7-9 0,4-6-897,27-47 0,-38 59 850,0 1-1,-1-1 1,-1 0-1,0 0 1,0-1 0,-1 1-1,0-1 1,0-19-1,-20 52-290,12-11 428,0-1 0,0 2 0,1-1 0,1 0 0,0 1 0,1 0 0,0 0 0,1 0 0,0 0 0,1 0 1,0 1-1,1-1 0,2 21 0,-1-30-63,1-1-1,-1 0 1,0 1 0,1-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,1-1-1,-1 0 1,0 0 0,1 1 0,0-2-1,-1 1 1,1 0 0,0 0-1,-1-1 1,1 0 0,0 1-1,0-1 1,-1 0 0,5-1 0,3 2 20,1-1 0,-1-1 0,0 0 1,1 0-1,-1-1 0,13-4 1,-11 1-46,0-1 0,0 0 0,20-15 0,6-4 98,-37 62-118,-2-21-182,0 31 868,1-46-880,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 1 0,0-1-1,0 0 1,2 2 0,0-2-1275</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8365.38">5386 2074 6323,'0'0'8868</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8365.37">5386 2074 6323,'0'0'8868</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8504.19">5741 1993 13446,'0'0'2849,"14"-2"-16071</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10184.72">5922 2058 12758,'0'0'4821,"-3"12"-3247,-44 129 2161,135-189-3557,-7 6-1770,-80 42 1808,-1 22 696,0-10-662,-1-6-149,1 1 1,0-1-1,1 1 1,0-1-1,0 1 1,3 11-1,-3-16-113,0 0-1,0 0 1,0-1 0,0 1-1,1 0 1,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,1-1-1,3 0 1,3 0-449,0 0-1,0-1 1,1 0-1,-1 0 1,0-1-1,0-1 1,0 1-1,-1-1 1,1-1 0,-1 1-1,1-1 1,-1-1-1,10-7 1,-10 6 426,-1 1 0,-1-2 0,1 1 0,-1-1 1,0 1-1,0-2 0,-1 1 0,7-13 0,-13 22 2022,-11 15 955,8-11-2810,1 0 0,-1 1 0,1-1 0,0 1 0,1-1 0,0 1 0,0 0 0,0 0-1,-1 12 1,3-18-110,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 1 0,1-1-1,-1 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1 0,1 1-1,1 0 7,-1 0 1,1 0-1,0-1 0,0 1 1,-1-1-1,1 0 0,0 1 1,0-2-1,0 1 0,-1 0 1,5-1-1,-2 0-12,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,0-1 1,0 1-1,5-5 0,-7 3-41,1 1 1,-1-1-1,1 1 1,-1-1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1-10 1,-1 13 14,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 0,0-1 1,-1 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,0 1 1,0-1-1,-2 0 1,-50 0-95,53 1 96,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 1-1,-1-1 1,1 1 0,-1-1 0,0 2 0,8-1-214,1-1-1,-1 0 0,0 0 0,0-1 1,1 0-1,8-1 0,-8 1 62,80-8-578,-88 50 1833,0 25 37,42-68-915,-31-4-290,-1 1 0,0-1 0,-1-1 1,1 0-1,-1 0 0,0-1 0,0 0 0,-1 0 0,0-1 1,0 0-1,8-13 0,-20 28 143,0 1 1,0-1-1,0 1 1,1 0-1,0 0 0,1 0 1,0 0-1,0 1 0,1-1 1,-1 14-1,49-23 430,-37-3-483,0 1 0,-1-2 0,1 1-1,-1-1 1,1-1 0,-1 0 0,-1 0 0,1-1 0,-1 0 0,-1 0 0,1-1-1,-1 1 1,0-2 0,-1 1 0,0-1 0,0 0 0,-1-1 0,0 1 0,3-12-1,-7 21 24,-1-1 0,0 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,-1 1 0,1-1-1,0 0 1,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,-1 0-21,1 1-1,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 1 1,1-1-1,-3 2 0,-4 1-26,0 1-1,1 0 1,-1 1-1,1 0 0,-7 6 1,12-9-6,-1 1 1,1 0-1,0-1 0,0 1 1,0 0-1,1 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,1 1 1,-1-1-1,1 0 0,0 1 1,0-1-1,1 6 1,2-8 36,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,5-1-1,1-1-6,-1 0 0,0 0 0,0 0-1,0-1 1,0-1 0,0 1-1,-1-1 1,0 0 0,13-10 0,-16 11-64,0 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,1-1-1,-1 0 1,-1 0-1,1 0 1,0 0-1,-1-1 1,0 1 0,0-1-1,0 1 1,-1-1-1,0 0 1,1 1-1,-1-8 1,-1 11 43,0 1-1,0 0 1,0 0 0,0-1 0,0 1-1,-1 0 1,1-1 0,0 1 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0-1,1 1 1,-13 7-128,12-1 111,0 0 0,0 1 1,1-1-1,0 0 0,0 1 0,1-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,2-1 0,-1-1 0,1 1 1,0 0-1,0-1 0,1 1 0,6 8 0,4 9 125,-14-24-101,1 1-1,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0 0 0,-1 0 0,1-1 1,-1 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 1,-1-1-1,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,-6 2 39,-1-1 0,1 0-1,0 0 1,-15-1 0,5 0-20,-108 1-2618,72-2-657,-16 1-2102</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10647.46">5229 2053 7251,'0'0'12198,"121"0"-12182,-36 0 32,14 0-48,0 0-2417,-7 0-5859</inkml:trace>
@@ -8962,7 +8962,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4434.99">722 771 11189,'0'0'4946,"9"9"-4703,32 31 21,-39-38-216,0 0-1,0-1 0,0 1 1,0-1-1,0 0 1,1 0-1,-1 1 0,1-2 1,-1 1-1,0 0 1,1 0-1,0-1 0,-1 1 1,1-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1-1 1,-1 1-1,0 0 0,0-1 1,0 1-1,3-2 0,0-2 21,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,-1-1 0,6-10 0,-8 48 770,-2 54-1,-9-27-565,-16 58 0,20-97-201,0 0 0,-2-1 0,0 0 0,-1 0 0,-1-1 0,-20 30 0,26-44 43,-1 0-1,1 0 1,0-1 0,-1 1-1,0-1 1,0 0 0,0 0-1,0 0 1,-1-1 0,1 0 0,-1 0-1,-7 2 1,11-4-90,1 1 0,-1-1 1,0 1-1,1-1 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,0-1 0,0 1 1,1-1-1,-1 1 0,0-1 0,0 1 1,1-1-1,-1 1 0,1-1 0,0 1 1,-1-1-1,1 0 0,0 1 0,0-1 1,0 0-1,0-2 0,0-4-65,0 0 0,1 1 0,0-1 0,0 1 0,0-1 0,1 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,1 1 0,-1-1 0,1 1 0,0-1 0,1 1 0,0 0 0,0 0 0,7-6 0,86-80-3338,-67 66 2488,-1-2-1,-2 0 1,-1-2 0,29-42-1,-54 70 1014,-1 0 0,0 0 0,0 0 0,1 0-1,-1-1 1,-1 1 0,1 0 0,0 0 0,0-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 1-1,0 0 1,0-1 0,-1-3 0,1 5-1,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 1 0,0-1 1,0 1-1,0-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,-2 1 1,0 0-114,0-1 0,1 1 1,-1 0-1,1 0 1,0 0-1,-1 1 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 1,-1 3-1,0-2-11,1 1 0,0-1 0,0 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,1 0 0,-1 6 0,2-10-4,0 0-1,1-1 0,-1 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1-1 1,-1 1-1,3-1 0,-3 1 0,20 0 9,-18-1 8,0 1 0,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,1 1 0,-1 0 0,0-1 1,0 1-1,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,0-1 0,4 6 0,-2 0 82,1-1 0,0 1 0,0-1 0,1 0 0,0-1-1,0 1 1,9 6 0,-12-12-74,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,0-1-1,0 1 1,-1-1 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1-1,5-4 1,32-29-1516,-21 4-4571,-11 14-1594</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6345.52">61 1173 3474,'0'0'16314,"0"15"-16170,1 7 9,-5 120 693,3-127-758,-1 1 1,0 0-1,-1-1 0,-1 0 0,0 0 0,-1 0 0,-9 19 1,14-33-65,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 1,-6-25 416,6 16-451,1 1 0,-1-1-1,2 0 1,-1 1 0,3-12 0,4 8-91,0 0 1,0 1-1,1 0 1,1 0-1,0 1 1,0 0-1,1 0 1,0 1-1,13-8 1,19-20-205,20-28 1263,-63 80-1022,-5 42 116,-5 79 325,11-135-373,0 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,1 1 0,-1 0 0,0-1-1,1 1 1,-1 0 0,1-1 0,-1 0 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1 0,3 0-1,0 1 2,1-1-1,0 0 0,-1 0 0,1 0 1,0-1-1,-1 0 0,0 1 0,1-2 0,-1 1 1,0 0-1,7-7 0,43-68-81,-58 195-91,32-151-11806,-13 7 3482</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6475.07">448 1192 11861,'0'0'8340,"0"-16"-8788</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8460.95">448 1205 11717,'50'76'1148,"-47"-70"-598,0-1 0,-1 1 1,1 0-1,-1 0 0,0-1 1,-1 1-1,0 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,0 1 1,-2 9-1,1 4 704,17-38 960,18-27-2505,-32 42 267,0 1 1,0 0 0,-1 0 0,1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,6-2 0,-6 6-11,-1-1 0,0 0 0,1 1 0,-1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 5 0,-1-8 31,0 80 857,0-79-665,2-7 27,0 3-213,0 0-1,1-1 1,-1 1-1,1 1 1,-1-1 0,1 0-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 1 1,6-2-1,5 48 57,-13-43-56,0 0 1,-1 0 0,1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,4 1-1,-2-2-158,0 1-1,0-1 0,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,7-3 0,-2 0-296,-1-1-1,1 1 1,-1-2-1,0 1 1,0-1-1,0 0 1,-1-1-1,0 1 1,0-2-1,7-8 1,-13 14 556,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,0 0 1,-1-1 0,1 1-1,-1-1 1,0 0 0,1-3 1123,-20 13 898,14-3-2059,0 0 0,0 0 0,0 0 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 1 0,-2 6 0,6-13-72,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,2-2-1,17-14-102,28-19-274,-48 35 293,2 38-77,-3-29 279,1 16 567,-1-24-673,0 1 1,0-1 0,0 1-1,1-1 1,-1 0 0,0 1-1,0-1 1,1 0 0,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 0 0,1 0-1,-1 1 1,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,1-1-1,-1 0 1,21-12 72,-18 10-96,1 0 1,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,1-1 0,-1 1 0,0 0-1,0 1 1,1-1 0,-1 1 0,8 0 0,-10 1 12,-1 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 2 0,0-2 13,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 1,3 2-1,1-3 7,0 0 0,-1 0 1,1-1-1,0 1 0,-1-1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,0 0 0,0-1 1,0 1-1,0-1 0,0 0 1,0-1-1,-1 1 0,9-9 1,-5 5-18,-1-1 0,0-1 0,0 0 0,-1 0 0,0 0-1,-1 0 1,1-1 0,5-16 0,-11 22 10,0 4-64,8 54-271,-6-47 333,0 1-1,-1 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,-3 15 1,1-22 2,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0-1,-1 0 1,1 0 12,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 0 0,0 0 0,1-4-31,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1-1,0 0 1,1-1 0,-1 1 0,1 0 0,0 0 0,1 0 0,3-5 0,49-59-360,-18 25 61,-3-4 85,48-69 222,-69 98 973,-23 42-697,4-12-399,-7 15 255,2 0 0,1 1 0,1 0 0,1 0 0,2 1 0,0 0 0,-1 47 0,11-76-122,-1 0 0,1-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,6-4 0,81-51-17,-91 56-72,0 6-54,0 0 117,0 0 0,0 0 0,1 0 0,0 1 0,2 10-1,-2-16 22,-1 0 0,0-1-1,1 1 1,-1 0-1,0-1 1,1 1 0,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 1-1,1-1 1,1 1 0,0-1 1,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,1-2 0,5-2-11,-1 0-1,0-1 1,0 0 0,0-1 0,8-11 0,-14 16 0,-1 2-42,16 1-271,-14 0 307,0-1 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 1,-1 0-1,1-1 0,2-1 0,38-43-62,-42 45 124,0 36-221,0-30 263,0 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,3 8 1,9 1-2200,-12-13 1550,0-1 0,0 0 0,0 0 0,1 1 0,-1-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,2-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8460.94">448 1205 11717,'50'76'1148,"-47"-70"-598,0-1 0,-1 1 1,1 0-1,-1 0 0,0-1 1,-1 1-1,0 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,0 1 1,-2 9-1,1 4 704,17-38 960,18-27-2505,-32 42 267,0 1 1,0 0 0,-1 0 0,1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,6-2 0,-6 6-11,-1-1 0,0 0 0,1 1 0,-1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 5 0,-1-8 31,0 80 857,0-79-665,2-7 27,0 3-213,0 0-1,1-1 1,-1 1-1,1 1 1,-1-1 0,1 0-1,0 1 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 1 1,6-2-1,5 48 57,-13-43-56,0 0 1,-1 0 0,1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,4 1-1,-2-2-158,0 1-1,0-1 0,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,7-3 0,-2 0-296,-1-1-1,1 1 1,-1-2-1,0 1 1,0-1-1,0 0 1,-1-1-1,0 1 1,0-2-1,7-8 1,-13 14 556,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,0 0 1,-1-1 0,1 1-1,-1-1 1,0 0 0,1-3 1123,-20 13 898,14-3-2059,0 0 0,0 0 0,0 0 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 1 0,-2 6 0,6-13-72,-1-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,2-2-1,17-14-102,28-19-274,-48 35 293,2 38-77,-3-29 279,1 16 567,-1-24-673,0 1 1,0-1 0,0 1-1,1-1 1,-1 0 0,0 1-1,0-1 1,1 0 0,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 0 0,1 0-1,-1 1 1,0-1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,1-1-1,-1 0 1,21-12 72,-18 10-96,1 0 1,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,1-1 0,-1 1 0,0 0-1,0 1 1,1-1 0,-1 1 0,8 0 0,-10 1 12,-1 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 2 0,0-2 13,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 1,3 2-1,1-3 7,0 0 0,-1 0 1,1-1-1,0 1 0,-1-1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,0 0 0,0-1 1,0 1-1,0-1 0,0 0 1,0-1-1,-1 1 0,9-9 1,-5 5-18,-1-1 0,0-1 0,0 0 0,-1 0 0,0 0-1,-1 0 1,1-1 0,5-16 0,-11 22 10,0 4-64,8 54-271,-6-47 333,0 1-1,-1 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,-3 15 1,1-22 2,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0-1,-1 0 1,1 0 12,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 0 0,0 0 0,1-4-31,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1-1,0 0 1,1-1 0,-1 1 0,1 0 0,0 0 0,1 0 0,3-5 0,49-59-360,-18 25 61,-3-4 85,48-69 222,-69 98 973,-23 42-697,4-12-399,-7 15 255,2 0 0,1 1 0,1 0 0,1 0 0,2 1 0,0 0 0,-1 47 0,11-76-122,-1 0 0,1-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,6-4 0,81-51-17,-91 56-72,0 6-54,0 0 117,0 0 0,0 0 0,1 0 0,0 1 0,2 10-1,-2-16 22,-1 0 0,0-1-1,1 1 1,-1 0-1,0-1 1,1 1 0,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 1-1,1-1 1,1 1 0,0-1 1,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,1-2 0,5-2-11,-1 0-1,0-1 1,0 0 0,0-1 0,8-11 0,-14 16 0,-1 2-42,16 1-271,-14 0 307,0-1 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 1,-1 0-1,1-1 0,2-1 0,38-43-62,-42 45 124,0 36-221,0-30 263,0 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,3 8 1,9 1-2200,-12-13 1550,0-1 0,0 0 0,0 0 0,1 1 0,-1-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,2-2 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9018,7 +9018,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">99 61 15175,'0'0'7363,"0"-4"-7149,-11 91 165,-8 46 22,14-50-9895</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="276.22">3 126 14615,'0'0'7945,"-1"-5"-7321,1 5-627,0-1 0,-1 0 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 1,0 0-1,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1-1 0,2 1 1,27-4-253,-9 3 361,30-3 53,44-3-2508,-90 16-2068,-4-6 3018,3 9-4644</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="276.21">3 126 14615,'0'0'7945,"-1"-5"-7321,1 5-627,0-1 0,-1 0 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 1,0 0-1,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1-1 0,2 1 1,27-4-253,-9 3 361,30-3 53,44-3-2508,-90 16-2068,-4-6 3018,3 9-4644</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2211.39">311 222 8756,'0'0'13548,"0"-6"-12777,0 4-700,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1 0 0,0-1-1,0 1 1,0 0 0,-1 0-1,1 0 1,0 0 0,-2-2 0,1 3-66,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,-1 0 0,1 0 0,0 0 0,-2 2 1,-1 0-23,-1 0 1,0 1-1,1-1 1,0 1-1,0 0 1,0 0-1,0 1 1,1-1-1,0 1 1,0 0-1,0-1 1,0 2-1,1-1 1,-3 9-1,5-14-42,2-1 30,0-1 33,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,0 0 0,0-1 0,0 1-1,1-3 1,2-2-6,-3 6 4,-1 47-998,4-45 920,-1-1 1,1 0-1,0-1 0,-1 1 1,1 0-1,0-1 0,-1 0 1,1 0-1,-1 0 0,1-1 1,-1 1-1,0-1 0,0 1 1,6-5-1,-5 2-119,0-1 1,0 0-1,0 0 0,-1 0 1,0-1-1,0 1 1,0-1-1,2-6 0,4-12 78,-1 0 0,0 0-1,-2-1 1,3-30 0,-31 298 3576,22-242-2950,3-6-504,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-1,1 1 0,-1 0 1,1 0-1,0 0 0,0 0 1,1 0-1,-1 1 0,0 0 0,1 0 1,0 0-1,-1 0 0,1 1 1,0 0-1,8-1 0,-12 2-21,0 0 1,-1 1-1,1-1 0,0 0 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,-1-1 0,0 2 1,0 2 30,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,-5 5 0,-43 22 371,37-26 12,36-18-414,8-4-96,-1-1 1,-1-2-1,53-46 0,-74 59-39,-1-1 1,1-1 0,-1 0 0,-1 0 0,0 0-1,0 0 1,-1-1 0,0 0 0,-1 0 0,0-1-1,0 1 1,-1-1 0,-1 0 0,1 0 0,-2 0 0,1-20-1,-2 32 165,0-1-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,1 1-1,-14 15 189,-11 24 378,15-17-183,0 0-1,2 1 1,1-1-1,1 1 1,1 0-1,1 1 1,0-1-1,3 37 1,0-59-392,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 1,1 0-1,0 1 0,1 0 0,25 1 139,-21-3-124,1-1 1,-1 1-1,0-1 1,0 0-1,-1 0 1,1-1-1,5-2 1,-5 0-57,0 0 0,-1 0 0,1 0 0,-1 0 0,-1-1 0,1 0 0,-1 0-1,0 0 1,0 0 0,0-1 0,-1 1 0,0-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,0 0 0,0 0 0,0-11 0,-1 17-53,-2 2 15,0-1 63,0 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,-1 2 0,-15 39 41,17-40-26,-4 8 86,2 1 1,0 0 0,0 0 0,1 0-1,1 22 1,0-28-75,0-5-16,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,0 0 1,0-1-1,1 1 1,1 0-1,42-7 96,-37 3-77,-1 1 0,0-2 0,0 1-1,-1-1 1,1 0 0,-1 0 0,0-1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0-1-1,-1 0 1,0 0 0,0-1 0,-1 1 0,0-1 0,0 1 0,-1-1 0,0 0 0,0 0 0,-1 0-1,1-14 1,-2 21-64,0 44-278,1-41 323,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,4 2 0,45 16 13,-45-18-11,-1 1-1,1-1 1,0 1-1,-1 1 1,1-1-1,-1 1 1,9 5-1,-14-7-2,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 0 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 1-1,-27 11-56,26-12 65,-28 12-112,-51 17 100,28-18-3644,27-10-1692</inkml:trace>
 </inkml:ink>
 </file>
@@ -9235,16 +9235,16 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">188 627 13254,'0'0'5829,"-13"8"-4775,-41 29-91,51-35-900,1 0 0,-1 0 0,0 1 0,1-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,1 1 0,-1 1 0,0-1-1,1 0 1,-1 0 0,1 0 0,0 1 0,0-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,2 4 0,-1-7-52,0 1 0,0-1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,1-1 0,40-7 193,-39 6-178,0 1 0,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0 0,0-1-1,0 0 1,0 1-1,-1-1 1,1 0 0,0 0-1,-1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,-2-6 0,2 9-32,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 1 0,1-1-111,-1 0 0,1 0-1,0 0 1,-1 1-1,1-1 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,-1 0 0,1 0-1,0 1 1,0-1-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0 0,0 1-1,-1-1 1,1 0 0,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,0 1-1,0-1 1,1 0 0,-1 1-1,0-1 1,0 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,11 1-2373,0-1 1,0-1-1,1 0 1,16-3-1,4-6-18,2-8 5502,-7-6 8976,-27 24-11855,-1-1 0,1 1 1,-1 0-1,0 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,1 0 1,-1 1-1,0-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 0,0-1 1,0 0-1,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,7 20-579,-6-19 805,3 11-156,0-3-76,0 2-1,-1-1 0,0 0 0,0 1 0,-1-1 0,-1 1 1,0 0-1,-1-1 0,-1 16 0,0-26-75,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,0-1-1,0 1 1,-2-1-1,3 0-32,-1 1-1,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 1,0 1-1,1-1 0,-1 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 0,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 1-1,1-1 1,0 1-1,0-1 0,-1 1 1,2-1-1,10-9-480,0 0 0,1 1-1,1 0 1,-1 1 0,16-6 0,-12 5-65,-1 0 1,0 0 0,19-16-1,-35 25 553,0 0 1,0 0-1,1 0 0,-1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 1-1,-1-1 0,-2 25 1179,-12 39 1214,12-54-2152,2-6-175,0 0 1,0-1-1,1 1 0,-1 0 1,1 0-1,0 0 1,0-1-1,0 5 0,1-7-67,-1 0-1,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,-1-1 1,1 1-1,0 0 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,1-1 0,4-1 1,0 0 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1-1-1,6-5 1,-6 5-62,1 0 0,-1 0 0,1 0 0,-1 1 0,11-4-1,-15 7 22,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 1 1,0 0-1,0-1 1,2 3-1,19 3 73,-16-6-41,28-4 74,-34 4-74,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,0 1-14,-1 1 0,1-1 1,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1 0 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 1 0,0 0 1,2-1 4,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 1 0,1-1 0,-1 0 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 1 0,0-1-1,0 0 1,1 1 0,-1-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1-1,0 0 1,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0-1,1 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,0 1-1,-1-1 1,38 6 30,-32-6 16,0 0 1,0 1-1,-1-1 1,1 1-1,0 0 1,-1 0-1,1 1 1,0 0-1,-1-1 1,0 1-1,1 1 1,-1-1-1,0 1 1,0-1-1,0 1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,1 1-1,-2 0 1,4 4-1,-4-4 69,0-1 0,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1-1-1,1 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1-1 1,8 3 0,-6-3-69,1-1 0,-1 1 0,0-1 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1-1 0,0 0 1,0-1-1,10-3 0,12-6-15,-1-2 0,-1 0-1,35-24 1,-12-4-4133,-41 30-336,-5 3-5531</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1561.73">49 1105 16600,'0'0'6896,"1"37"-6709,-4-28-89,-1 1 0,0-1 0,-1 0 0,0-1 0,0 1 0,-1-1 0,-12 14 0,29-55 460,-4 23-564,0-1 0,0 2 0,1-1 0,0 1 0,0 0 1,1 0-1,1 1 0,-1 1 0,15-10 0,-23 17-5,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 1,0 1-1,0 0 0,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,0 2 0,0 32 70,0-27-44,-1 7-4,0 1 0,-1-1 1,-1 0-1,-7 24 0,20-49-3,0 1 0,1 0 0,0 1 0,1 0 0,23-14 0,-30 20-32,63-44-120,-68 46 195,-7 38 31,5-29-79,-1 0-1,2 0 0,-1 0 0,1 0 1,0 0-1,1 10 0,1-17-48,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,1-1-1,2 1 0,42-2-2356,-35 0 1371,-1 0 1,0 0-1,1-1 1,11-5-1,-19 7 692,0 0 1,1-1-1,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0-1 0,-1 1 0,1 0 0,-1-1 1,1 1-1,-1-1 0,0 0 0,0 1 0,3-7 0,-5 9 452,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-15 5 1020,-12 10-1393,27-15 264,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,21 0-9,26-9-189,-41 8 135,-4 0 78,0 0 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,5 1-1,-7 0 51,1 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1-1,0-1 1,1 1 0,-1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1 0,-1 2 0,1-3-60,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,1 0 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0-1 0,0 1 0,0-1 0,0 1 0,4-2 0,4-2-35,0 0-1,-1-1 0,1 0 0,13-10 0,-13 8 1,-1-1-1,0 0 1,0 0 0,-1-1-1,0 0 1,-1 0-1,0-1 1,0-1-1,-1 1 1,-1-1-1,0 0 1,9-22 0,-15 32 57,0 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 1,-15 5 165,9-2-168,0 0 0,1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1 1 1,0 0-1,0-1 1,0 1 0,1 1-1,-1-1 1,2 0-1,-1 1 1,1 0-1,0-1 1,0 1-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0-1,0 0 1,2 8-1,-2-13-27,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,1 1-1,1 0 1,1 1 9,1-1 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1-1 0,6 0 0,1 0 21,0-1 0,0 0 0,-1-1 0,1 0 0,17-7 0,-23 7-29,1 0 1,-1 0-1,1 0 1,-1-1-1,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 0-1,0 0 1,0 0-1,0-1 1,0 0-1,-1 1 1,0-1-1,0 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,-1 1-1,1-1 1,-1 0-1,1-7 1,-2 12 17,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,-28 11 169,24-7-175,1 0 1,-1 1-1,1-1 0,0 1 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,1 1-1,-3 6 0,4-10-13,0 0 1,0 0-1,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,3 1 0,5 1-116,0 0 0,-1-1 0,1-1 0,0 1-1,0-2 1,0 1 0,14-2 0,37-11-3570,-21-4-1790</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3043.32">110 166 7587,'0'0'12646,"0"81"-11400,0-67-1059,-1 0 1,-1 0-1,-5 23 0,6-33-155,0 1 0,0-1 0,0 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-2-1 0,1 0-1,-5 4 1,7-7-23,1 0 0,0-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1-1,0 1 1,0-1 0,-1 1-1,1 0 1,0-1 0,0 1-1,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,1-1 1,-2-26-13,1 23 13,1-15-2,0 0 1,1 0-1,1 1 0,0-1 0,2 1 1,0-1-1,1 1 0,1 1 0,1-1 1,13-22-1,-17 33-29,1 0-1,-1 0 1,2 0 0,-1 1 0,1-1-1,0 1 1,0 1 0,1-1 0,-1 1-1,1 0 1,0 1 0,1-1 0,-1 1-1,1 1 1,0 0 0,0 0 0,0 0-1,0 1 1,1 0 0,-1 1 0,0 0-1,1 0 1,-1 1 0,1 0 0,11 1-1,-18 0-180,-1-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 0,-1 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,-1 0 0,1 0 1,0 1-1,0-1 1,-1 0-1,0 2 0,-8 17-6793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2889.91">134 223 11733,'0'0'6836,"78"-10"-6788,-46 8-48,-4 2-1953,-3-2-1729,-8 2-3986</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2889.92">134 223 11733,'0'0'6836,"78"-10"-6788,-46 8-48,-4 2-1953,-3-2-1729,-8 2-3986</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1504.82">293 266 8516,'0'0'6099,"11"1"-5435,1 1-469,1-1-1,-1 0 1,1-1 0,12-1-1,-23 1-170,1 0 0,-1 0 0,1-1 1,-1 1-1,0 0 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-5 0,-2 7 48,0-1-1,0 0 1,0 0-1,1 1 1,-1-1 0,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,-2 1-1,-36 11 362,35-9-422,-1 1-1,1 0 1,0 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,1 1-1,0-1 1,0 0-1,1 1 1,0-1-1,0 1 1,0 0-1,1-1 1,-1 1 0,2 6-1,0-10-11,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,3-1-1,44-2-56,-36 1 32,0-2 1,0 0 0,-1 0 0,1-1-1,-1-1 1,0 0 0,16-11 0,-7 4 21,-21 13 26,0 4 23,0 1 0,0-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,3 8 0,1-11-25,-1-1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,5-5 0,1 2-10,15-8 27,-17 8-29,1-1 0,1 2 1,-1-1-1,0 1 1,1 0-1,0 0 0,-1 1 1,15-1-1,-22 4 40,0 0-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0-1 1,0 1-1,0 2 1,5 16 326,-4-19-354,0 0-1,0-1 1,0 1 0,0 0 0,1 0 0,-1-1 0,0 1-1,0 0 1,1-1 0,-1 1 0,0-1 0,1 0-1,-1 1 1,1-1 0,-1 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0-1 0,1 1-1,-1 0 1,3-1 0,37-18 138,-16 7-139,-23 12-26,0 0 0,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,1 2 0,0-1-2,-1 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,4 0 0,3 1-263,53-5-2252,-60 4 2455,-1 0 0,1 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1-1,1 1 1,-1-1 0,1 0 0,0-2 0,-2 3 194,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,-1 0 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-3 1 0,-38 2 398,29 4-721,32-4 40,34-5-153,-15-2 318,-28 4 7,0 0 0,0-1 0,-1-1 0,1 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,13-8 0,-11 5 4,0 0 0,0-1-1,-1 0 1,0-1 0,0 0 0,-1-1 0,0 0 0,-1-1 0,0 1 0,0-1 0,-1-1-1,0 0 1,-1 0 0,0 0 0,-1-1 0,6-18 0,-14 29 1918,-8 7-1612,-9 10-476,14-8 152,1 0 0,-1 0 1,1 1-1,1 0 1,0 0-1,0 0 0,-2 11 1,4-15 2,0 0 1,1 0 0,0 1 0,1-1-1,-1 0 1,1 1 0,0-1-1,0 1 1,0-1 0,1 0-1,0 1 1,0-1 0,0 0 0,4 9-1,-3-11-1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,1 0 1,-1-1-1,0 1 1,0-1 0,0 1-1,4-3 1,4 1-74,0-1 1,-1 0-1,0-1 1,0 0-1,0-1 1,17-11-1,-21 13 53,-1-1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,-1 0 0,1 0 1,-1-1-1,0 0 0,0 1 0,0-1 0,-1 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0-1 0,-1 0 1,2-11-1,-4 18 19,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,-3 1 0,1 1-6,-1 0 0,0 0 0,0 0 0,1 1 0,0 0 1,0-1-1,0 1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 1 0,0-1 1,1 1-1,-2 5 0,2-8-3,0 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,1 1 0,-1-1-1,1 1 1,0 0 0,-1-1 0,1 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,3 2 0,1-1-296,0 0 0,0 0 0,0-1 1,0 0-1,13 2 0,59 0-7682,-65-4 6395,47 0-3144</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38009.81">2317 31 9380,'0'0'4274,"29"-20"-3431,-8 16-674,0 1 0,39-1 0,-59 8-169,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,-1 0-1,0 0 1,0 0 0,-1 4-1,1-1 13,-2 11 73,0-1 0,-2 0-1,0 1 1,-1-1 0,0-1-1,-1 1 1,-1-1 0,-1 0-1,-18 27 1,17-27-49,0-1-1,0 1 1,1 1 0,1-1-1,1 1 1,1 1-1,0-1 1,1 1 0,-3 34-1,7-50-39,0-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 1 1,2-2-1,63 3-839,-52-3 373,13-1-186,-27 2 777,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,0-1-1,-20 19 454,4 9-548,1 1-1,1 0 1,2 0 0,0 2 0,2-1 0,-10 57-1,-8 186 85,16-112-88,10-153-26,1 1 0,-1 0 0,0 0 0,-1 0-1,0-1 1,0 1 0,-3 6 0,4-11 37,-1 0-1,1-1 1,0 1 0,-1 0-1,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,-3 0 0,0 0 88,-1 0 1,0-1 0,1 1 0,-1-1 0,0 0-1,1-1 1,-1 1 0,1-1 0,0 0-1,0 0 1,-10-7 0,12 7-172,0 0-1,0-1 1,0 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0 0,0 0-1,1-1 1,-1 1 0,0-1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0-7 1,1 11-11,-1-6-760,1 1-1,0 0 1,0-1-1,0 1 1,1 0 0,1-7-1,10-14-6229</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38427.67">2765 647 12902,'0'0'4479,"-4"0"-4372,46 3-64,0-3-1,0-1 1,51-8 0,-92 7 194</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39006.46">3343 449 11461,'0'0'6131,"-2"15"-5691,-20 59 155,17-61-490,0 1 0,1-1 0,0 1-1,1-1 1,1 1 0,-1 19 0,2-22-135,3 16 89,-2-27-184,0 1 0,1 0-1,-1-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1 0,1-1-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,-1 0 1,2 0 0,-1-1-201,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,-1-2 0,2-3-940,3-12-3571</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39225.34">3350 447 7812,'0'0'8561,"10"3"-8260,-6 3-275,0 1 0,0 0-1,-1-1 1,0 1 0,3 10 0,13 25 244,-7-22-290,-4-5-98,1-1 1,0 0-1,1 0 0,1-1 1,11 12-1,-15-23-6528</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39506.67">3523 394 7924,'0'0'8809,"0"10"-8126,-2 31 42,-2 0 0,-11 50 0,1-13-430,10-35-135,5-21-2653,-1-21 2198,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,9 0-3926</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39815.73">3573 609 4706,'0'0'10434,"0"-9"-10071,-4 40 112,2-23-351,1-1 1,0 1-1,0-1 1,1 1-1,0-1 0,0 1 1,3 12-1,-3-19-113,1 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,31-19 173,-27 12-150,-1 0-1,0 0 1,-1-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0-1,-1 0 1,0 0 0,-1 0 0,-1-16 0,0 24-99,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,1 0 1,-1 1-1,0 0 0,1-1 0,-1 1 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,1 0 1,-1 1-1,0-1 0,-2 2 0,-29 27-3523,21-14-998</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39815.72">3573 609 4706,'0'0'10434,"0"-9"-10071,-4 40 112,2-23-351,1-1 1,0 1-1,0-1 1,1 1-1,0-1 0,0 1 1,3 12-1,-3-19-113,1 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,31-19 173,-27 12-150,-1 0-1,0 0 1,-1-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,0 0-1,-1 0 1,0 0 0,-1 0 0,-1-16 0,0 24-99,-1 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,1 0 1,-1 1-1,0 0 0,1-1 0,-1 1 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,1 0 1,-1 1-1,0-1 0,-2 2 0,-29 27-3523,21-14-998</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40688.25">3774 617 11829,'0'0'5221,"0"28"-5303,-2 12-46,1-25 425,0-13 312,1-5 446,1-4-1029,1 1 0,-1-1 0,1 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,1 0 0,0 0 0,0 1 0,6-7 1,8-13-12,-18 25-16,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,3 21-243,-2 31-155,-1-49 395,-3 68 1533,7-86-1543,1 1-1,0 0 1,1 0 0,1 0-1,0 1 1,9-14-1,-7 12-108,-8 13 54,-1 4 51,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-2 0,0 1 0,2 0 1,0-1 21,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,-1 0 1,1 1-1,-1-1 1,1-1-1,-1 1 1,0 0-1,1-1 0,-1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,-1-1 0,0 1 1,2-6-1,-5 14-114,-4 14 184,1 0 0,-2 30 0,6-45-61,-1-1 0,2 1-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,1 1 0,-1-1-1,1 0 1,-1 0 0,4 5-1,-2-6-24,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-2 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,6 0 0,-3 0-402,18-3-4721,-15-10-2882</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40835.79">4133 428 6211,'0'0'9684,"-39"69"-16279</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40835.78">4133 428 6211,'0'0'9684,"-39"69"-16279</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41708.28">4144 600 1409,'0'0'15988,"-2"13"-15091,1-7-827,-4 32 791,-12 40 1,17-78-850,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,-1 0-1,1 0 0,1 0 1,-1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,13-6 214,10-10-164,8-6 1,-25 18-52,0 0-1,0 0 1,0 0 0,0-1 0,-1 0 0,1 0 0,6-10 0,11 67-211,-23-50 166,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,2 1 0,-1-2-93,-1 1 0,1-1 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1 0,-1-1-1,1 0 1,0 0 0,-1 0 0,5-2 0,-2 0-12,-1 1 0,0-1 0,0 1 1,-1-1-1,1-1 0,-1 1 0,1-1 1,-1 1-1,0-1 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 0 1,0 0-1,-1 0 0,5-10 0,-7 13 172,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,0-1 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,-1-1-1,2 2 19,-1 0-1,0 0 0,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,1 0 1,-3 1-1,1-1-16,-1 1-1,0-1 1,1 1-1,-1 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-4 5-1,5-7-46,-1 1 1,1-1-1,0 1 0,-1 0 1,1-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 1 1,1 0-1,0 0 0,0-1 1,0 1-1,1 0 0,-1 0 1,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 1,1 2-1,0-1-11,1-1-1,-1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,2 0 1,49-20-613,-49 19 588,-1 1 43,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,5 3-1,-4-1 40,1-1 0,0-1-1,0 1 1,0 0-1,0-1 1,0 0-1,0 0 1,5 0 0,-3 0 7,0-1 1,1 0 0,-1-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,0-1 0,0 0 0,0-1 0,0 1-1,-1-1 1,1 0 0,-1-1 0,1 1 0,-1-1 0,5-4-1,-3 0 79,0 0-1,0-1 0,-1 1 1,0-1-1,-1 0 0,0-1 1,0 1-1,-1-1 1,4-14-1,1-12 113,-1 0 1,-2-1 0,-2 1-1,0-67 1,-7 97 441,-4 15-563,-5 17-170,-1 6 274,2 0 0,2 1 0,1 1 0,1-1 0,-2 44 0,7-58-123,2-1 0,0 1 1,1 0-1,0 0 0,2-1 0,0 1 1,1-1-1,1 0 0,1 0 1,0 0-1,11 20 0,-14-32-179,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1-1,0 0 1,0 0-1,0 0 1,1 0 0,0-1-1,0 0 1,0 0-1,0-1 1,0 0-1,1 0 1,0 0-1,-1-1 1,10 2 0,10-3-4269</inkml:trace>
 </inkml:ink>
 </file>
@@ -9274,7 +9274,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">43 226 12630,'0'0'7907,"0"-5"-7048,0-17-280,0 17 929,-4 22-1482,-5 9 28,3-7-28,0 1 0,0 0 0,2 0 1,1 1-1,-2 27 0,6-47-28,-1 0-1,1 0 1,0 0-1,0-1 0,0 1 1,-1 0-1,1 0 1,0-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,2 0-1,35-7-118,-33 4 117,-1-1 1,0 1-1,0-1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,3-10 0,10-17 17,-17 38-28,0-1-1,0 0 1,1 1 0,0-1 0,0 1 0,0-1-1,0 0 1,1 1 0,-1-1 0,1 0-1,0 1 1,1-1 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,6 6 0,-6-9 13,-1 1 0,1-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,3 0 0,-2-1 4,0-1 0,0 1 0,0 0 0,-1-1 0,1 0 1,-1 0-1,1 1 0,-1-1 0,0-1 0,0 1 0,0 0 0,2-6 0,1-3 24,-1-1 1,0 0-1,-1 0 1,0 0-1,-1 0 1,1-21-1,-1 13 76,-2 16-20,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,-1-8 1,2 13-116,-1-1 1,1 1-1,0-1 1,0 1 0,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,0 0-1,-1 1 1,1-1 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 1,-14 21-5073,14 4-5009,3-15 5141</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1414.18">290 266 2769,'0'0'8367,"3"3"-6876,-1-1-1251,0 0 1,0 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 0 1,0 0-1,5 0 0,-4-1-78,1 0-1,-1 0 0,0 0 0,1-1 0,-1 0 1,0 0-1,0 0 0,0 0 0,0-1 1,0 1-1,5-6 0,-2 2-109,-1-1 0,0 1-1,0-1 1,-1 0 0,1-1 0,-2 1 0,1-1 0,-1 0-1,0 0 1,-1 0 0,0-1 0,0 1 0,1-11 0,0-86 76,-4 78-91,-3 12 53,-5 19-123,-5 25-64,9 13 92,1 1 1,4 69 0,1-33 28,-2-78-23,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1 1,0 1-1,1-1 0,16-9 53,-6-2-19,1 1 0,0 1 0,1 0 1,16-9-1,-28 18-67,16 52-280,-16-48 315,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,3 2 0,-3-2-22,1-1 0,-1 1-1,0-1 1,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 0-1,0 1 1,-1-1 0,1 0-1,-1 0 1,3-3-1,0 1 17,-1-1-1,1 1 0,-1-1 1,0 0-1,0 0 0,0-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 0 1,-2 0-1,1-1 0,1-8 1,-3 14 339,0 32-347,0-24 14,2 28 46,-2-35-48,1 1-1,-1-1 1,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1-1,0 1 1,0-1 0,0-1-2,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,1-1 0,-2 1 0,1 0 0,-1-5 0,1 5 2,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 1 0,-2-1 0,1 0 0,0 0 0,0 1 0,0-1-1,-1 1 1,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 1 0,-2-2 0,-2 1 33,1 0 0,-1 1 0,1 0 1,-1-1-1,1 2 0,-1-1 1,1 1-1,-11 2 0,14-2-45,0-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0-1,1 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,1 0 0,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 2 1,1-3-47,1 0 1,0 0-1,0 0 1,-1-1-1,1 1 0,0-1 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,1 1-1,1-1-14,5 0 47,0 0-1,0 0 1,-1-2 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0-1-1,-1 1 1,1-1 0,-1 0 0,0-1 0,0 1 0,-1-2 0,12-12-1,-11 10 160,-1 1-1,0-1 1,0-1-1,-1 1 1,0-1-1,0 0 0,-1 0 1,0 0-1,-1 0 1,-1-1-1,1 1 1,-2-1-1,2-17 0,-4 32-122,1-1 0,-1 1 0,-1-1-1,1 1 1,0-1 0,-1 1 0,1-1-1,-5 6 1,-6 17 26,7-6-40,1 0 0,1 1 0,-1 29 0,4-42 2,0 0 0,0 0 0,1-1 1,0 1-1,0 0 0,1 0 0,0-1 1,0 1-1,1 0 0,0-1 0,7 12 0,-8-16 3,0-1-1,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,1-1 0,-1 0 0,0 1 1,4-3-1,2 0 11,0 0 1,-1 0-1,1-1 0,-1 0 1,0-1-1,-1 0 0,1 0 1,10-10-1,-13 11 10,-1 0-1,0-1 1,0 1 0,-1-1-1,1 0 1,-1 0 0,0-1-1,0 1 1,-1-1 0,1 1-1,-1-1 1,-1 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,-1-10 0,0 15-2,-1 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,-1 0-1,-25 6 422,20-3-460,-1 0-1,1 1 1,0 0 0,1 0-1,-1 1 1,1 0 0,0 0-1,1 0 1,-7 10 0,9-12-13,0 0 0,0 1 1,0-1-1,0 1 0,1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,1 1 1,0-1-1,0 11 0,1-16-26,-1 1-1,0 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,0-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,2 0 1,27 0-971,-23-1 549,1 1-470,0-1 1,1 1-1,-1-2 0,0 1 0,0-1 0,0 0 1,13-6-1,15-12-7711</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1414.17">290 266 2769,'0'0'8367,"3"3"-6876,-1-1-1251,0 0 1,0 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 0 1,0 0-1,5 0 0,-4-1-78,1 0-1,-1 0 0,0 0 0,1-1 0,-1 0 1,0 0-1,0 0 0,0 0 0,0-1 1,0 1-1,5-6 0,-2 2-109,-1-1 0,0 1-1,0-1 1,-1 0 0,1-1 0,-2 1 0,1-1 0,-1 0-1,0 0 1,-1 0 0,0-1 0,0 1 0,1-11 0,0-86 76,-4 78-91,-3 12 53,-5 19-123,-5 25-64,9 13 92,1 1 1,4 69 0,1-33 28,-2-78-23,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1 1,0 1-1,1-1 0,16-9 53,-6-2-19,1 1 0,0 1 0,1 0 1,16-9-1,-28 18-67,16 52-280,-16-48 315,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,3 2 0,-3-2-22,1-1 0,-1 1-1,0-1 1,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1-1 1,1 0-1,0 1 1,-1-1 0,1 0-1,-1 0 1,3-3-1,0 1 17,-1-1-1,1 1 0,-1-1 1,0 0-1,0 0 0,0-1 1,-1 1-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 0 1,-2 0-1,1-1 0,1-8 1,-3 14 339,0 32-347,0-24 14,2 28 46,-2-35-48,1 1-1,-1-1 1,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1-1,0 1 1,0-1 0,0-1-2,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,1-1 0,-2 1 0,1 0 0,-1-5 0,1 5 2,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 1 0,-2-1 0,1 0 0,0 0 0,0 1 0,0-1-1,-1 1 1,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 1 0,-2-2 0,-2 1 33,1 0 0,-1 1 0,1 0 1,-1-1-1,1 2 0,-1-1 1,1 1-1,-11 2 0,14-2-45,0-1-1,1 1 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0-1,1 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 1,1 0 0,0 0-1,-1 0 1,1-1-1,0 1 1,0 0-1,0 2 1,1-3-47,1 0 1,0 0-1,0 0 1,-1-1-1,1 1 0,0-1 1,0 0-1,0 1 1,-1-1-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,1 1-1,1-1-14,5 0 47,0 0-1,0 0 1,-1-2 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0-1-1,-1 1 1,1-1 0,-1 0 0,0-1 0,0 1 0,-1-2 0,12-12-1,-11 10 160,-1 1-1,0-1 1,0-1-1,-1 1 1,0-1-1,0 0 0,-1 0 1,0 0-1,-1 0 1,-1-1-1,1 1 1,-2-1-1,2-17 0,-4 32-122,1-1 0,-1 1 0,-1-1-1,1 1 1,0-1 0,-1 1 0,1-1-1,-5 6 1,-6 17 26,7-6-40,1 0 0,1 1 0,-1 29 0,4-42 2,0 0 0,0 0 0,1-1 1,0 1-1,0 0 0,1 0 0,0-1 1,0 1-1,1 0 0,0-1 0,7 12 0,-8-16 3,0-1-1,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,1-1 0,-1 0 0,0 1 1,4-3-1,2 0 11,0 0 1,-1 0-1,1-1 0,-1 0 1,0-1-1,-1 0 0,1 0 1,10-10-1,-13 11 10,-1 0-1,0-1 1,0 1 0,-1-1-1,1 0 1,-1 0 0,0-1-1,0 1 1,-1-1 0,1 1-1,-1-1 1,-1 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,-1-10 0,0 15-2,-1 1 1,0-1-1,0 1 0,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,-1 0-1,-25 6 422,20-3-460,-1 0-1,1 1 1,0 0 0,1 0-1,-1 1 1,1 0 0,0 0-1,1 0 1,-7 10 0,9-12-13,0 0 0,0 1 1,0-1-1,0 1 0,1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,1 1 1,0-1-1,0 11 0,1-16-26,-1 1-1,0 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,0-1 0,0 0 1,-1 1-1,1-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,2 0 1,27 0-971,-23-1 549,1 1-470,0-1 1,1 1-1,-1-2 0,0 1 0,0-1 0,0 0 1,13-6-1,15-12-7711</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9305,7 +9305,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">32 64 11733,'0'0'6777,"0"-7"-4999,0 3-538,0 7-745,-1 11-328,0 0 0,-2 0 0,1 0 0,-6 16-1,3-16-49,2 1 0,0-1 1,0 1-1,0 19 0,3-33-112,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,1 0 0,-1 1 0,0-1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,0 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,0 0 0,0 0 0,0 0 0,2 0 1,-1 0-5,0 0 1,0-1-1,0 1 1,1-1-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1-1 1,1 0 0,3-1-36,0 0 1,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0-1-1,6-6 1,-5 2 7,-1-1-1,-1 0 0,1-1 0,-1 1 1,-1-1-1,0 0 0,5-18 0,-8 24-204,-3 27 250,-1 1 1,-1-1-1,0-1 1,-11 29-1,-10 55 484,23-93-33,2-3-2331,13-21-2519,7-6-1476</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="627">631 278 7027,'0'0'11459,"-11"-5"-10920,-35-18-16,43 21-445,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,1 0 1,0 0 0,-1 1-1,1-1 1,0 0-1,1 0 1,-2-4 0,0-53 106,3 42-66,-1 17-114,0-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 1-1,1 0 1,-1-1 0,1 1 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,1-1 0,1-1 0,1 1-36,0-1 1,0 1 0,0 0 0,0 0-1,0 1 1,0-1 0,8 1-1,-12 2 22,0 0 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,-3 3 0,-47 35 153,42-35-144,1 1 0,-1 0 1,1 1-1,0-1 0,1 2 1,-1-1-1,2 1 0,-1 0 0,-7 13 1,13-21-6,0 1-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,-1-1 0,2 3 0,0-2 4,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,2 0 0,5-1 20,0 0 1,0-1-1,0 0 0,-1 0 0,1-1 0,12-6 0,-2 5-1460,7 7-6400,-11 2-578</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1045.83">954 102 10997,'0'0'7289,"-9"-4"-6945,-29-12-208,37 15-134,0 1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 1 1,0-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 1 1,0-1-1,-1 2 1,-3 46 39,4-47-29,0 1-8,0 1-1,0-1 1,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0 0-1,0-1 1,1 0 0,-1 1 0,5 2 0,3 3-2,2-1 0,-1-1 0,23 10 0,22 13 58,-55-29-23,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1 0 0,-22 12 922,-32-1-579,36-10-1218,0-3-3553,15-1 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1284.68">973 76 11701,'0'0'5283,"85"-39"-4515,-57 31-208,-3 0 113,0 2-145,-8 0-304,-2 2-64,-8 2-48,-4 0 32,-6 2-3169,-15 0-2802</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1284.67">973 76 11701,'0'0'5283,"85"-39"-4515,-57 31-208,-3 0 113,0 2-145,-8 0-304,-2 2-64,-8 2-48,-4 0 32,-6 2-3169,-15 0-2802</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9345,7 +9345,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1470.68">1091 1312 8308,'0'0'12806,"7"-18"-12886,14 12 32,18-1-337,4 3-1247,6 0 911,8 0-1232,-7 0-2913,-4-4-1761</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1120.11">1679 1219 6659,'0'0'13676,"-4"0"-13073,63-7 4,1 2-2611,-10 2-3480,-38 3 135</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-903.91">1708 1315 7652,'0'0'11557,"-8"2"-11557,16 0-256,6-2 256,14 2 112,4-2-112,7 0-785,0-4-895,0-6-657,-7-3-3074,-7-1-2449</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-585.29">1826 1122 14038,'0'0'4242,"-1"0"-4262,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 1,3 8 33,1-1 0,1-1 0,-1 1 0,1-1 0,0 0 0,1 0 1,8 6-1,32 33 177,-42-38-13,-1-1 0,0 1 0,0-1 0,-1 1 1,0 0-1,0 1 0,0-1 0,2 11 0,-5-15-111,1 0-1,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 1,0 0-1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 1,0-1-1,-4 4 0,-4 1-44,0 0-1,0-1 1,-1 0 0,1-1 0,-1-1 0,0 1-1,0-2 1,-17 3 0,-9-2-2191,-46-1 1,67-2 933,-36 0-3815</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-585.3">1826 1122 14038,'0'0'4242,"-1"0"-4262,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 1,3 8 33,1-1 0,1-1 0,-1 1 0,1-1 0,0 0 0,1 0 1,8 6-1,32 33 177,-42-38-13,-1-1 0,0 1 0,0-1 0,-1 1 1,0 0-1,0 1 0,0-1 0,2 11 0,-5-15-111,1 0-1,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 1,0 0-1,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 1,0-1-1,-4 4 0,-4 1-44,0 0-1,0-1 1,-1 0 0,1-1 0,-1-1 0,0 1-1,0-2 1,-17 3 0,-9-2-2191,-46-1 1,67-2 933,-36 0-3815</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2506.13">2877 1065 7443,'0'0'9621,"1"-8"-8154,2-37 1913,-13 46-2889,-1 3-483,1 0 0,0 0-1,1 1 1,-1 0-1,1 1 1,0 0 0,0 0-1,0 1 1,1 0 0,0 0-1,1 1 1,-12 14 0,9-8-24,1-1 0,0 1 0,1 0 1,0 1-1,2 0 0,-1 0 0,-7 30 1,12-35 9,0-1 0,0 1 0,1 0 0,0 0 0,1-1 1,0 1-1,0 0 0,1 0 0,0 0 0,5 15 0,-4-20-1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 0 0,8 1 0,-3 0-4,1 0-1,0-2 0,0 1 0,0-1 0,16-2 0,-26 2 20,1 0 0,0 0 1,-1 0-1,1-1 0,0 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1 0 1,1 1-1,-1-1 0,0-2 0,-1 2-2,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1 0-1,-4-1 1,-51-4-204,52 5 151,-51-1-2602,34 1-4365</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3134.71">2971 895 9188,'0'0'5365,"-16"-10"-4482,-54-27-336,64 34-508,-1 1 0,-1-1-1,1 1 1,0 0 0,-1 1 0,1-1-1,-1 2 1,1-1 0,-1 1-1,1 0 1,-13 2 0,-11 0 91,16-2-85,0 1 0,1 0 1,-1 1-1,0 1 0,1 0 0,0 1 0,0 1 0,0 0 0,0 1 0,1 0 0,0 1 0,0 1 0,1 0 0,0 0 1,0 2-1,1-1 0,0 1 0,-12 16 0,9-8 12,1 0 0,0 2 0,2-1-1,0 1 1,1 1 0,1 0 0,1 1 0,1-1 0,1 1 0,1 1 0,-3 27 0,5-28 2,0 1 0,2 0 1,1 0-1,0-1 0,2 1 1,5 29-1,-4-43-49,-1 0 0,2 0 1,-1 0-1,1-1 0,0 1 1,1-1-1,0 0 0,0 0 0,1-1 1,0 0-1,0 1 0,1-2 1,0 1-1,0-1 0,1 0 0,-1-1 1,17 9-1,-6-6 6,0 0 0,0-2 0,0 0 0,1-1 0,0-1 0,0 0 0,0-2 0,0 0-1,0-1 1,1-1 0,-1-1 0,29-5 0,-18 1-24,-1-1-1,0-2 1,0 0-1,-1-2 0,0-1 1,-1-2-1,37-21 1,-49 23 13,0 0 0,0-1 0,-1-1 0,0 0 0,-2-1 0,1 0 0,-2-1 1,0 0-1,0-1 0,-2 0 0,0 0 0,9-24 0,-10 19 5,-1 0 0,-1-1 0,-1 0 0,0-1 0,-2 1-1,-1-1 1,-1 1 0,0-1 0,-6-43 0,4 59 19,0-1 1,0 1-1,-1-1 0,0 1 0,0 0 1,-1 0-1,0 0 0,0 0 0,-1 0 1,0 1-1,0-1 0,0 1 1,-1 0-1,0 1 0,0-1 0,-1 1 1,1 0-1,-1 0 0,0 0 0,0 1 1,-1 0-1,1 0 0,-1 1 0,0 0 1,0 0-1,0 1 0,0-1 1,-1 1-1,1 1 0,-1 0 0,1 0 1,-1 0-1,-7 1 0,-3-1-175,0 2 0,0-1 1,0 2-1,-23 5 0,-33 18-4199,31-7-2818</inkml:trace>
 </inkml:ink>
@@ -9463,7 +9463,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">60 3 11957,'0'0'3509,"-19"51"-2263,-16 139 1059,30-168-2831,4-35-3074,4-39-806,-3 0 1978,1-7 559,8 25 3970,-8 33-1962,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,1-1 0,0 2-1,37 23 1073,3 9-1097,65 72-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212.71">240 1 6771,'0'0'9012,"0"105"-8235,-10-31-438,6-53-1555,0 0-1,1 25 0,4-42-2561</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212.7">240 1 6771,'0'0'9012,"0"105"-8235,-10-31-438,6-53-1555,0 0-1,1 25 0,4-42-2561</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="548.04">289 130 9780,'0'0'3613,"-3"12"-3272,1-5-305,-2 8 89,0 0-1,1 0 1,-1 27-1,4-38-100,0-1 0,0 1 0,0 0 0,1-1 1,-1 1-1,1-1 0,0 1 0,0-1 0,1 0 0,1 5 0,-2-6-18,0-1 0,0 0 0,0 1 0,1-1 0,-1 0-1,0 0 1,0 1 0,1-1 0,-1 0 0,1-1 0,-1 1 0,1 0-1,-1 0 1,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,3 0 0,-2-1 37,1 1 0,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,2-4 0,-1 2 99,-1 1 0,0-1 1,0 0-1,0-1 0,0 1 1,-1 0-1,0 0 1,0-1-1,-1 1 0,1 0 1,-1-1-1,0 1 0,0-1 1,-1 1-1,-1-6 1,2 11-124,0-1 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 1 0,0-1-1,-1 0 1,1 1-1,-22 19-855,14 6-1721,9-8-2468,2-9-663</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="892.55">573 108 6707,'0'0'12067,"-14"-4"-11744,-44-12-251,58 16-76,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 1-1,0-1 1,0 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0-1,0 1 1,-2 25-162,3-21 169,-1-1-23,0 1 1,1-1-1,-1 0 0,1 1 1,0-1-1,1 0 1,-1 1-1,1-1 1,0 0-1,1 0 1,-1-1-1,6 9 0,1-2 1,0-1 0,1 0-1,16 13 1,5 5 55,-30-28-14,-1 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,1 1 0,-1-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,1 0 1,-1 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0-1,0 1 1,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,0 0 0,-1 1 0,1-1-1,-29 7 728,21-6-1178,0-1 1,0 0-1,-1 0 1,1-1-1,-15-3 1,15-3-3799,1-7-4648</inkml:trace>
 </inkml:ink>
@@ -9624,7 +9624,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">53 56 4914,'0'0'9853,"0"-6"-2738,-19 83-7126,12-49 88,0 0-1,-3 31 1,0 34 115,10-93-144,0-22-16770</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="395">50 183 12838,'0'0'8977,"5"0"-15473</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="746.96">4 311 9204,'0'0'6947,"0"2"-6883,0 0 465,0 0-321,3 2-80,1-4-80,3 4-48,-3-4-176,-1 2-945,1-2-1376,-1 0-1681,1 0 1473</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="746.95">4 311 9204,'0'0'6947,"0"2"-6883,0 0 465,0 0-321,3 2-80,1-4-80,3 4-48,-3-4-176,-1 2-945,1-2-1376,-1 0-1681,1 0 1473</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1595.47">4 311 8260,'29'-54'4212,"-28"52"-3689,0 1-1,0-1 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 0,0 0 1,1-1-1,0 1 1,-1 0-1,3-1 0,31-6-928,-19 6 846,11-5-359,-6 2-33,0 0-1,-1-1 0,1-2 1,-2 0-1,38-20 0,-55 25-38,1 1 0,0 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,0 1 0,-1-1 0,0-3 0,1 6 151,-2 3-183,0 1 0,-1-1 1,1 0-1,0 1 0,1-1 1,-1 1-1,0 0 0,1 0 1,-2 3-1,-6 13 8,1 0 0,1 1 0,1 0 0,1 0-1,1 0 1,1 1 0,0-1 0,1 37 0,55-55 127,-50-2-89,1-1-1,-1 1 1,0-1 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 0-1,-1 0 1,1 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,0 0-1,-1-7 1,-4 33-128,-2 15-36,7-37 130,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,-1-1 0,1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 1,1-1-1,7 1-38,0-1-1,1 0 1,-1 0 0,0-1 0,0 0 0,0-1-1,0 0 1,12-4 0,-16 5-54,0-1 1,-1 0-1,1 0 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,4-7 0,-16 29 2486,7-12-2438,1 0-1,0 0 0,0 0 0,0 1 1,1-1-1,-1 9 0,2-15-76,0 1-1,0 0 1,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0 0,0-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1-1,0 0 1,1 0-249,18 0-4763</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1731.12">645 190 7155,'0'0'13174,"0"-59"-13174,4 59-688,3 6-1265,7 8 592,4 0-3153,7-2-1568</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2533.97">854 179 13750,'0'0'4648,"-13"3"-4083,-43 14-394,55-16-165,-1 0-1,0 0 1,0 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 2-1,-2 40-66,3-31 34,0-2 19,0 0-1,1 0 0,0-1 1,0 1-1,8 16 1,-7-17 42,1 1 0,-1-1 0,-1 1 0,0 0 0,1 17 0,-2-22-14,-2 1 0,1-1 0,0 1 0,-1-1 0,0 1 0,-1-1 0,1 0 1,-1 1-1,-1-1 0,1 0 0,-6 9 0,6-12 72,-1 0-1,0 0 0,1-1 1,-1 1-1,0-1 0,0 1 1,-1-1-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1-1-1,0 1 0,1-1 1,-1 0-1,0 0 0,0-1 1,1 1-1,-1-1 0,0 0 1,-5 0-1,8-1-61,-1 0-1,1 1 1,0-1 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,0 0 1,-1-1-1,1 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,1-1 0,-1-5-129,0 0 0,1 0 0,0 0 0,3-15 0,4 7-473,0 0 0,1 0 0,0 1 0,1 1 0,1-1 1,13-13-1,11-15-393,-2-3 674,31-39 2906,-64 85-2564,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0-1,2 28 375,0 28-602,-3-39 165,1-12 24,-1-1 0,1 0-1,0 0 1,1 0 0,-1 1 0,1-1 0,2 8-1,-2-11-30,-1 0 0,1 1 0,0-1-1,0 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1 0,1-1 0,-1 0-1,1 1 1,-1-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,1 0-1,5-1 11,0 0 0,0 0 0,-1 0 0,1-1 1,-1 0-1,1-1 0,-1 0 0,0 0 0,11-6 0,1-1 53,-16 10-49,1-1 0,0 0 0,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,0 0 0,-1 0 0,1 0 0,6 3 0,25 4 109,-30-8-99,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0-1-1,0 1 0,0-1 1,0 0-1,-1 0 1,1 0-1,-1-1 1,8-5-1,-6 3-43,0 0-1,-1-1 1,0 0-1,0 0 1,0-1 0,-1 1-1,0-1 1,4-11-1,-6 15 37,6-12 22,-1 0 0,0 0 0,-1 0 0,-1-1 0,0 0 0,-1-1 0,3-28 0,-7 43 487,-2 29-283,-14 43-423,-7 35-38,18-33-5797,5-56-604</inkml:trace>
@@ -9632,7 +9632,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3361.84">1800 245 6099,'0'0'15193,"-9"11"-15030,-24 33-163,33-44-2,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1-1-1,0 1 1,-1 0 0,1-1-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1 0,0-1-1,0 0 1,-1 0-1,1 1 1,0-1 0,1 0-1,38 5 5,-40-5-1,6 0-59,-1 0-1,1-1 0,-1 1 1,0-1-1,1 0 1,-1 0-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,9-6-1,-12 6 12,0 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,0 1 0,-1 0-1,0-1 1,1 1 0,-1-1-1,0 0 1,0 1 0,0-1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 1 0,-1-1-1,1 0 1,-1 0 0,1 1-1,-1-1 1,-1-3 0,1 5 58,0-1 0,0 1 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-2 2 0,1 1-733,9 0-317,9-2-185,-9-1 1220,0 0 0,0-1 0,0 0 0,-1 0 1,1-1-1,0 1 0,-1-1 0,1-1 1,-1 0-1,0 0 0,0 0 0,0 0 0,0-1 1,-1 0-1,1 0 0,-1-1 0,0 1 0,0-1 1,4-6-1,5-8 540,-1-1 0,-1 0 0,-1-1 0,10-25 0,1 0 635,-20 46 127,-1 7-1193,-3 12-436,-38 112 405,26-93-87,2 1 1,2 1 0,-6 43-1,11-49 8,2-1 0,2 1 0,1 0 1,1-1-1,10 57 0,-11-88 0,1 1 1,-1-1-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1-1-1,1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 0-1,0-1 1,4 2-1,-4-2-2,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 0,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1-4-1,1-5-287,-1 0 1,0-1-1,0 1 0,-1-1 0,0 1 1,-1-1-1,-1 1 0,0 0 1,0-1-1,-7-18 0,5 22 213,1 1 0,-1-1 0,-1 1 0,1 0 0,-1 0 0,-7-7 0,5 6 592,-1 1 1,0 0 0,0 0-1,-1 1 1,-11-6 0,69 6-2683,3 4-1315,13 0-4834</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3919.51">2740 155 6227,'0'0'14740,"-13"-4"-14041,-44-9-438,55 13-257,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 1-1,0 0 0,0 0 0,0-1 1,0 1-1,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,1 0 0,-1 1 1,1-1-1,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0 3 0,-2 3-26,0 1 1,1 0-1,0 0 0,-1 13 0,1-4 33,1-1-1,2 1 1,-1-1 0,2 1-1,0-1 1,2 0 0,5 20-1,-8-32-7,0 0 0,0-1-1,-1 1 1,1 0 0,-1 0-1,-1 0 1,1-1-1,-1 6 1,1-9-4,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1-1 0,-1 1 1,0-1-1,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 0,0-1 1,0 1-1,0-2 0,0 2-18,1-1 0,-1 0 0,1 1 0,0-1 1,-1 1-1,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,16-21-1807,1 7 347,2 0 1,25-14-1,-26 18 800,-1-1-1,0 0 1,27-26 0,3-22 1991,-25 14 2420,-19 40 1965,-5 21-4940,-6 27-1397,-4-3 751,-12 70 0,18-45-7011</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4267.15">2800 276 2113,'0'0'12598,"14"-7"-11659,-1 1-924,1 1-1,0 0 1,0 0 0,0 2-1,1-1 1,-1 2 0,26-2-1,-39 4-5,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,1 0 1,-1 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,2 1 1,3 32 499,-5-31-476,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1-1,1 0 1,0 1 0,1-1 0,-1 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,2 3 0,-2-5 137,-1 1 0,0-1 0,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1-1 1,-1 0-1,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,2-1 1,27-49 114,-24 42-284,-4 5-403,-1 3-1133</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5236.27">3349 300 16680,'0'0'2481,"-15"-1"-1022,-45-3-512,56 5-940,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 1,0 0-1,1-1 1,0 1-1,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,1 0-1,0 0 0,0 0 1,1 5-1,0-7-35,0-1 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 0,1-1 0,48-8 238,-44 5-217,1 0 0,-1 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-2 0,-1 1 0,1 0 0,-2-1 0,1 0 0,-1 0 0,4-9 0,3-10-149,-2 0 0,0-1-1,5-32 1,2-7 42,-20 83 81,1 0 0,0 0 0,1 0 1,1 0-1,1 19 0,0-30 35,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,1-1 0,-1 1 0,1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,5 5 0,-5-7-6,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0-1-1,0 0 1,1 1-1,-1-2 1,0 1-1,0 0 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0-1-1,0 1 1,3-8-1,0-1 396,-4 11 183,-9 38-373,12-36-229,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,6-2 0,12-4-63,13-3-451,-32 9 527,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 2 0,-1 0 43,1-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 0,-1 1 0,1-1 0,4-3 0,0 2 8,0-1-1,0 0 1,-1-1 0,1 0 0,-1 0-1,0 0 1,0-1 0,0 0 0,-1 0-1,0 0 1,8-10 0,1-11 7,-1-1 0,0-1 0,-2 0 0,8-32 0,-1 3 295,-25 77 324,-15 42-606,-26 116 0,44-162-1527,1-2-1517,3-5-2045</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5236.26">3349 300 16680,'0'0'2481,"-15"-1"-1022,-45-3-512,56 5-940,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 1,0 0-1,1-1 1,0 1-1,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,1 0-1,0 0 0,0 0 1,1 5-1,0-7-35,0-1 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 1,1-1-1,0 1 0,0 0 0,1-1 0,48-8 238,-44 5-217,1 0 0,-1 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-2 0,-1 1 0,1 0 0,-2-1 0,1 0 0,-1 0 0,4-9 0,3-10-149,-2 0 0,0-1-1,5-32 1,2-7 42,-20 83 81,1 0 0,0 0 0,1 0 1,1 0-1,1 19 0,0-30 35,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,1-1 0,-1 1 0,1-1-1,0 0 1,1 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,5 5 0,-5-7-6,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 0 1,1 0 0,-1 0-1,0 0 1,0-1-1,0 0 1,1 1-1,-1-2 1,0 1-1,0 0 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0-1-1,0 1 1,3-8-1,0-1 396,-4 11 183,-9 38-373,12-36-229,-1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,6-2 0,12-4-63,13-3-451,-32 9 527,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 2 0,-1 0 43,1-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 0,-1 1 0,1-1 0,4-3 0,0 2 8,0-1-1,0 0 1,-1-1 0,1 0 0,-1 0-1,0 0 1,0-1 0,0 0 0,-1 0-1,0 0 1,8-10 0,1-11 7,-1-1 0,0-1 0,-2 0 0,8-32 0,-1 3 295,-25 77 324,-15 42-606,-26 116 0,44-162-1527,1-2-1517,3-5-2045</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5409.12">3877 163 10837,'0'0'10869,"92"-4"-10677,-39 4-128,-3 0-64,-1 0-896,-10 0-3090,-17-6-5154</inkml:trace>
 </inkml:ink>
 </file>
@@ -9702,14 +9702,14 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1692.37">209 402 11541,'0'0'3642,"7"1"-3471,7 0-89,-7 1-50,1-1 1,0-1-1,0 0 0,0 0 1,14-2-1,-20 2-23,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 1,1 1-1,-1-1 0,0 0 0,0 0 0,0-3 0,0 4 20,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,0 1 1,0 0-1,1 0 1,-1-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 0-1,-1 1 1,1-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,-3 1-1,2-1 8,0 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 1 0,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 3-1,-3 42 215,4-42-221,1-4-42,-1 1 1,0-1 0,1 0-1,-1 1 1,1-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 1-1,0-1 1,1 1 0,-1-1-1,1 0 1,-1 0 0,1 0-1,-1 1 1,3-2-1,56 3-1143,-53-3 937,1 1-72,0-1 0,-1 0-1,1 0 1,0-1 0,-1 0-1,0 0 1,1-1 0,-1 0-1,0 0 1,0-1 0,6-4-1,-9 5 160,-1 1 0,1-1-1,-1 0 1,0 0 0,0-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1-1,0 1 1,-1 0 0,1-8-1,-1 11 333,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 0,-1-1 1,0 1-159,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,0 1 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0 0 0,0 0 1,-1 0-1,-1 3-55,0-1-1,0 1 1,1 0 0,-1 0 0,1 0 0,0 0-1,0 1 1,0-1 0,1 0 0,-1 1 0,1-1 0,0 1-1,1-1 1,-1 1 0,1 0 0,0-1 0,0 1-1,0 5 1,3-9-71,0 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,-1 0 0,1 1 0,0-1-1,0 0 1,2-2 0,10-8 705,-10 18 482,4 16-1183,-7-20 72,0 0-1,1 0 1,-1-1 0,0 1 0,1-1-1,-1 1 1,1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1-1 0,-1 1-1,1-1 1,-1 0 0,5 0 0,-6-1-1,1 1 1,-1 0-1,0-1 1,1 1-1,-1-1 0,0 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,0-4 1,0-1-43,1 6 117,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 0,0 0 1,0 1-1,1-1 0,-1 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0 0 0,-1-1 1,31 11-2365,100-8 1254,-128-2 1054,-1 30 1105,0-16-906,0-11-151,0 0 0,-1 0 1,1 1-1,1-1 0,-1 0 0,0 1 1,1-1-1,0 0 0,0 0 1,0 0-1,1 4 0,0-6-47,0 1 0,-1-1 0,1 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 1,0-1-1,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,4-1 0,3 1-55,0-1 0,0 0 0,-1-1 0,1 1 0,0-2 0,-1 1-1,0-1 1,1 0 0,-1-1 0,0 0 0,-1 0 0,1-1 0,-1 0-1,0 0 1,0-1 0,0 0 0,-1 0 0,0-1 0,0 1 0,-1-1-1,1-1 1,-2 1 0,1-1 0,-1 1 0,0-1 0,-1-1 0,1 1-1,-2 0 1,1-1 0,-1 1 0,-1-1 0,1 0 0,-1-10 0,-1 18 132,0 0 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1-1,-1-1 1,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-2-2 0,1 3-45,1-1 0,-1 1 0,0-1 1,1 1-1,-1 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 0 0,-1 0 0,0 0 1,0 1-1,-2 0-13,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 1,-4 6-1,-25 63 113,29-66-134,1-1 1,-1 1 0,1 0 0,0 0-1,1 0 1,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,1 0-1,0 0 1,2 8 0,-1-12-34,-1 1 1,1 0-1,0-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,0-1 1,3 1-1,54-9-791,-48 6 594,0-1 0,0 0 0,-1 0 0,0-2 0,0 1 0,0-1 0,-1-1 0,0 1 0,0-2-1,-1 1 1,0-1 0,0 0 0,0-1 0,11-17 0,-12 14 127,-1 0 0,1-1 0,-2 0 0,0 0 0,-1 0-1,4-17 1,-5 14 1124,-1 0-1,1-30 526,-3 49-1402,-2 55-61,0-39-41,1-1-1,0 1 0,1 0 1,1-1-1,1 1 1,1-1-1,1 1 0,6 21 1,-9-38-60,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,2 0 0,5-1-49,1-1 0,-1 0 0,0 0 0,11-4 0,-5 1 485,-12 5-399,-1 0 0,0 0-1,0 0 1,0 0-1,0 1 1,1-1 0,-1 1-1,0 0 1,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1 0-1,-1 0 1,2 3-1,22 20-1699,-3-16-1627,0-1-3698</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2856.72">1692 310 13078,'0'0'3009,"-2"8"-2771,2-4-178,-1-1 1,1 1-1,-1 0 1,1-1 0,0 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,1 5-1,-1-7 23,0 1 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0-1 1,1 1 0,-1-1 0,0 0-1,0 0 1,5 0 0,-1 0-27,1 1-1,-1-2 1,1 1-1,-1-1 0,1 0 1,-1 0-1,0 0 1,1-1-1,-1 0 1,0 0-1,0-1 1,0 0-1,0 0 1,-1 0-1,1-1 1,-1 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 0 1,-1 0-1,0 0 1,4-8-1,-2 0-72,0 0 0,0 0 0,-1-1-1,-1 1 1,0-1 0,-1 0 0,-1-1 0,0 1-1,-1 0 1,-1-16 0,0-7-39,0 37-8,-4 5 10,1 0 0,-1 0 1,1 0-1,0 1 0,0 0 0,0-1 0,1 1 1,0 0-1,0 0 0,1 1 0,0-1 0,-1 12 1,-1 85 122,4-70-93,-2-4 74,0-10-11,1 0 0,4 35 0,-4-50-30,1-1 1,0 1 0,-1-1-1,1 1 1,1-1-1,-1 1 1,0-1 0,1 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,5 3-1,-7-4 3,0-1-1,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0-1-3,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,-1 0-1,0-1 1,1-2 0,-1 0-20,0-1 1,0 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,-1 0-1,0 0 1,-2-6 0,0 7-8,0-1 1,0 1 0,0 0 0,-1 0 0,0 1-1,1-1 1,-1 1 0,-1 0 0,1 0 0,0 1-1,-1-1 1,1 1 0,-1 1 0,1-1 0,-1 1-1,0 0 1,-11-1 0,17 2-36,33-7-1473,-26 4 1386,150-71-819,-163 85 4058,-12 38-2642,16-43-392,0 0 0,1 0 0,0 1 0,0-1 0,0 1 0,1-1 1,0 1-1,0-1 0,2 11 0,-2-16-57,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 1-1,1-1 0,-1 1 6,1 0-1,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,3-1 0,-2-4 13,0 0-1,-1 0 1,1 0-1,-1 0 1,-1 0-1,1 0 1,-1 0-1,-1-10 1,0-3 45,2 19-75,-1 0 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,1 1 0,31 9-191,-28-8 181,0 1-1,1 1 1,-1-1-1,-1 1 0,1-1 1,0 2-1,-1-1 0,0 0 1,0 1-1,0 0 1,-1-1-1,1 1 0,-1 1 1,-1-1-1,1 0 1,-1 1-1,1 0 0,-2-1 1,1 1-1,1 9 1,-3-14 34,0-1 1,-1 0-1,1 0 1,0 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0-1,0-1 1,0 1 0,0-1-1,-1-4 35,0 0 0,1-1 0,0 1-1,0 0 1,0 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,1 0-1,0 0 1,0 0 0,1 1 0,-1-1-1,1 0 1,0 1 0,4-6-1,-4 7-217,0 0 0,0 0-1,0 1 1,1-1 0,-1 1-1,1-1 1,-1 1 0,1 0-1,0 0 1,6-1-1,-7 1-359,1 1-1,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,1 1 0,-1-1 1,0 1-1,-1 0 0,6 1 0,12 8-5492</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4908.03">2680 363 14247,'0'0'6080,"-11"-8"-5592,-38-21-243,47 28-234,1 0-1,-1 0 0,0 1 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 1,0 1-1,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,1 0 1,-1-1-1,0 1 0,1 0 0,-1 0 1,1 0-1,-2 1 0,-27 32 77,21-22-83,8-11 7,-1 1-1,1-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,2 0 0,-1 2 0,1-2-4,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,3 0 0,0 0-18,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 1,1 0-1,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,4-4 0,-5 3 4,-1-1 0,1 0 0,0 0 0,-1 0 1,0-1-1,0 1 0,0 0 0,-1-1 0,0 1 0,1-1 0,-2 0 0,2-8 1,12-162-2184,-7 82 1946,-14 156 806,4 126 1,4-183-522,0 1 0,0-1 0,0 0-1,1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,1-1-1,-1 0 1,10 9 0,-11-11-24,1 0 0,0-1 0,0 0 0,-1 0 1,2 1-1,-1-2 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 0 0,0 0 0,-1-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 0 0,7-2 0,-7 1-5,0 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1-1 0,0 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1-7 1,0 2 88,-1 0-1,0-1 1,0 1-1,0-1 1,-1 1-1,-2-15 1,1 22-80,1 0 1,-1-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0-1-1,-3 1 1,4 0-28,-1 0-1,0-1 1,0 1 0,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 1 0,1-1-1,-1 0 1,0 1-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1 1 0,4-2-561,-1 0 437,0 0 1,0-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 1 1,-1-1 0,0-1-1,0 1 1,0 0-1,0 0 1,-1-1-1,1 1 1,0-1-1,2-2 1,16-13 67,-9 75 1696,-10-55-1610,0 1 0,0-1 0,1 0 0,-1 0 0,1 1-1,0-1 1,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1-1,1-1 1,-1 0 0,4 3 0,-4-4-17,-1-1-1,0 1 1,0 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,1-3 1,10-15-105,-1-1-1,-1 0 1,-1-1 0,-1 1 0,-1-2-1,0 1 1,-2-1 0,0 0-1,-2 0 1,0-1 0,-1-31 0,-17 72-199,7 7 365,0-1 0,2 1 0,1 1 0,1-1 0,2 1 0,0-1 0,2 30 0,0-53-55,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 1,0-1-1,0-1 0,0 1 0,3 0 0,1-1 2,1 1 1,-1-1-1,1-1 1,-1 1-1,0-1 1,0 0-1,1 0 1,-1-1-1,-1 0 1,1 0-1,8-5 1,-10 4-19,0 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-2-1 0,1 1 1,0-1-1,-1 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 0,-1 0 1,1-1-1,-1 1 1,0 0-1,0-1 0,0 1 1,-2-6-1,2 10 2,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 1-1,-1-1 1,0 0-1,1 0 1,-1 1-1,1-1 1,-1 1-1,-22 14-11,21-11 11,-1 0 0,1-1-1,0 1 1,0 0 0,0 0-1,0 1 1,-1 6 0,3-11-32,-1 1 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0-1,0 0 1,0-1 0,-1 1 0,1 0 0,0-1-1,0 1 1,0-1 0,0 1 0,-1-1 0,1 1 0,0-1-1,0 0 1,2 1 0,-1 0 64,1 1-1,0-1 1,-1 1-1,0-1 1,1 1 0,-1 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,-1 1 1,3 3 0,20 21 620,-23-27-640,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1-1 1,1 1 0,0 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 1,0 1 0,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1 0,1 1-1,0-2 1,15-23 397,-13 19-349,-1 3-75,-1 1 1,0-1-1,0 1 1,1 0-1,0 0 1,-1 0-1,1-1 1,0 2-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0 0,0 1-1,-1-1 1,1 1-1,0-1 1,5 1-1,-7 1 14,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,-1 4 0,1-1 1,0 0-1,0 0 0,-1 0 1,1 0-1,-1 0 0,0 1 1,0-2-1,-1 1 0,-1 5 1,1-7 9,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 0,-4 1 0,7-1-13,2-9-1214,6 0 501,1 0-1,-1 0 1,19-14 0,25-26-102,-49 46 898,0 0 0,-1-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1-6 1468,-3 12-1490,0-1 0,0 1 0,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 1,0 1-1,-1 3 0,1-4-45,-1-1 1,1 1-1,0-1 0,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1 0 1,0-1-1,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 1,1-1-1,-1 0 1,0 0-1,3 2 0,0-3 3,0 1 1,0-1-1,1 0 0,-1 0 0,0 0 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,-1-1 0,1 1 0,0-1 0,0 0 0,5-5 0,-2 2-2,-1-1 1,1 0-1,-1-1 0,0 1 0,-1-1 0,0-1 0,7-11 0,1-5-184,-2-1-1,-1-1 1,0 0-1,5-29 1,-5 19 558,-10 36-358,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,-2 21 236,-12 47-110,8-45-128,2 1-1,-3 24 1,8-28-383,-2 16-1268,-3-18-7718</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5032.23">3439 203 6339,'0'0'8420,"106"-55"-8756,-74 49-1217,4 0-2033,-8-2-1280</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5032.22">3439 203 6339,'0'0'8420,"106"-55"-8756,-74 49-1217,4 0-2033,-8-2-1280</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5262.1">2783 181 9316,'0'0'4098,"82"-2"-4098,-29-7-1344,0 1-3987</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5982.56">4026 187 12678,'0'0'8014,"-12"2"-7758,-36 12-72,47-13-168,-1 0-1,1 0 0,0 1 1,-1-1-1,1 0 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 0,0 1 1,1 0-1,-1 0 0,1 2 1,-1-2 13,0 0 0,1 1 1,-1-1-1,1 0 0,-1 0 1,1 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,1 1 0,3-2 11,-1 1-1,1-1 1,-1 0-1,1 0 0,-1-1 1,1 0-1,7 0 0,-11 0-27,-1 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-2 0,1 0 6,-2 1 1,1 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,1 1 1,-1-1 0,0 0-1,1 1 1,-1-1 0,0 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 1-1,0-1 1,0 1 0,-1 0-1,1 0 1,0-1 0,-1 2-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1 0,-2 2 0,3-2-79,0 0 1,0 0-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1 0,0-1-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1 1 0,-3 22-6291,3-13 99</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6069.21">4026 187 6563</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6369.34">4026 187 6563,'89'45'5619,"-72"-36"-3205,-18 0 1241,2 15-2748,-1-18-171,0 126 1738,23-132-2293,-16-2-197,1 0-1,-1-1 1,1 0 0,-1-1-1,0 1 1,-1-1 0,1-1-1,-1 1 1,9-8-1,52-53-234,-58 55 226,-3 4-69,19-16 339,-24 22-237,0 0-1,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 1,-1-1-1,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 1,0-1-1,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 1,0-1-1,0 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1 1 0,5 13-394,13 48 1314,-1-35-2773,9-6-4401,-5-13-3363</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8538.46">4612 363 3650,'0'0'10687,"17"-9"-9361,3-1-1122,-2 0 0,1-2 0,-1 0-1,-1 0 1,0-2 0,-1 0 0,-1-1 0,0-1 0,14-18-1,-21 20-80,-1 1 0,0-1 1,-1 0-1,-1-1 0,0 0 0,-1 1 0,4-28 0,-4-21 3668,-18 84-3610,1 13-69,1-1-1,2 2 1,1 0-1,2 0 1,1 0-1,2 1 1,2-1-1,1 38 0,3-77-69,0 0-1,0-1 1,0 1-1,0 1 1,1-1-1,-1 0 1,1 0-1,0 1 1,0 0-1,0-1 1,1 1-1,6-4 1,-1-2 13,-4 3-70,0 1 1,1-1-1,0 1 0,0 0 0,0 0 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 1 0,1 0 0,-1 1 0,1 0 0,10-3 0,-17 5-78,-4 23-171,1-20 229,-1 0 0,0 0-1,1-1 1,-1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1-1 0,0 1 0,-5 0 0,-2 1-460,0-1-1,-1 0 1,-21 0 0,33-2 526,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,1 1 0,-1-1 1,0 1-1,0 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,1 1 0,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1 0 1,0 0-1,1 0 0,0 0 0,3 2 4,-1-1 1,1 1-1,-1 0 0,0-1 0,0 1 0,1 1 0,-1-1 0,-1 0 0,1 1 0,0 0 0,4 5 0,22 17 153,-21-20-328,1-2 0,0 1 1,0-1-1,0-1 0,0 0 1,1 0-1,10 1 0,-7-2-603,0 0-1,0-1 0,1-1 0,-1 0 0,0 0 0,0-1 1,0-1-1,13-4 0,-20 4 321,0 0 0,0 0 0,0 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,4-9 0,-5 9 1225,0-1 0,-1 1 0,1-1-1,-1 0 1,0 0 0,-1-7 0,0 14-673,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 0-1,-1 1 1,0 0 0,-26 9 758,22-8-822,0 1 0,0 0-1,1 0 1,-1 0 0,1 1 0,0-1-1,0 1 1,0 0 0,1 1 0,-1-1-1,1 1 1,0-1 0,0 1-1,1 0 1,0 0 0,-1 0 0,1 0-1,1 0 1,-1 1 0,1-1 0,0 1-1,0 8 1,26-15-1073,-21-1 1082,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,0-1 0,3-8 1,-4 10 1581,-1 33-1205,-1-28-483,0 1 1,1-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,1 0-1,0 0 1,-1-1 0,1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,0 1-1,1 0 1,-1-1 0,0 0-1,1 0 1,-1 1 0,0-1-1,1-1 1,-1 1-1,0 0 1,4-1 0,1 0-23,-1-1 1,0 1 0,1-1 0,-1 0 0,0 0-1,0-1 1,0 0 0,-1 0 0,1 0 0,-1-1-1,1 0 1,-1 0 0,5-5 0,39-49 1488,-50 64-1304,0 1 0,1-1 1,-1 0-1,1 1 0,1-1 0,0 8 0,0 17-158,-1 18 46,1-24-20,-2-1 0,-5 42 1,6-61-88,-1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 0,1-1 1,-1 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 0-1,0 0 0,-5 4 1,7-6 55,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-2 0-1,3 1 34,0-1-1,-1 1 0,1-1 0,0 0 0,0 1 1,0-1-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1-2-14,-1 1 0,1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,3-2 0,16-14-1092,1 1-1,1 2 0,27-16 0,-26 18 370,-1-2-1,0 0 1,21-21 0,-17-1 1440,-25 36-419,-1 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,0-4 0,0 6-220,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,-1 1 0,1-1-1,0 1 1,0-1 0,-1 1 0,1-1-1,0 1 1,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,-1 1 0,-1-1-1,-29 3 303,30-3-366,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,0 0 0,-1 1 0,2 1 0,3 6-191,0 0 0,0 0 0,1-1 0,14 15 0,-17-19 105,2 1 93,-1 0 0,-1 0-1,1 0 1,-1 0-1,0 1 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,-1-1 1,0 0 0,0 1-1,0-1 1,-3 12-1,2-16 40,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,1 0 0,0 0 0,0 1 0,-1-1-1,1-1 1,-1 1 0,1 0 0,-1 0 0,1-1-1,-6 1 1,-53 3 779,60-4-806,0 0-13,1 0 1,-1-1-1,1 1 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 1,0-1-1,1 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 1,14-21-445,38-27-2549,51-62-1,-84 86 1183,-1-2 0,-1 0 0,-1 0 0,-2-2 0,13-30 0,-14 9 5112,-13 46-2681,-1 0-1,0-1 0,1 1 1,-1 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,-1 0 1,0 0-1,0 0 0,0 0 0,-2-4 1,3 6-577,-1 0 1,1 0-1,-1 1 1,0-1 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1 0 1,0-1 0,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 1 0,-23 43 60,15-21 140,2 0 0,1 0 0,1 0-1,1 1 1,1-1 0,1 1 0,2 37 0,0-60-226,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,4-2 0,0 1 41,0-1 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0-1 0,-1 1 0,0-1 1,1 0-1,-1 0 0,6-8 0,-7 6 20,-1 1-1,-1-1 1,1 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,0-10 0,-1 17-87,1-1 1,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1-1,-1 1 1,-15 12-9,11-6 14,0 0 0,1 0 1,0 0-1,0 1 0,1 0 1,0-1-1,0 1 0,1 0 1,0 0-1,0 0 0,1 1 1,0-1-1,0 0 0,1 1 1,1 12-1,0-19-61,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,1 0 1,46-7-2885,-23-5-1534,-3-3-5027</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8538.45">4612 363 3650,'0'0'10687,"17"-9"-9361,3-1-1122,-2 0 0,1-2 0,-1 0-1,-1 0 1,0-2 0,-1 0 0,-1-1 0,0-1 0,14-18-1,-21 20-80,-1 1 0,0-1 1,-1 0-1,-1-1 0,0 0 0,-1 1 0,4-28 0,-4-21 3668,-18 84-3610,1 13-69,1-1-1,2 2 1,1 0-1,2 0 1,1 0-1,2 1 1,2-1-1,1 38 0,3-77-69,0 0-1,0-1 1,0 1-1,0 1 1,1-1-1,-1 0 1,1 0-1,0 1 1,0 0-1,0-1 1,1 1-1,6-4 1,-1-2 13,-4 3-70,0 1 1,1-1-1,0 1 0,0 0 0,0 0 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 1 0,1 0 0,-1 1 0,1 0 0,10-3 0,-17 5-78,-4 23-171,1-20 229,-1 0 0,0 0-1,1-1 1,-1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1-1 0,0 1 0,-5 0 0,-2 1-460,0-1-1,-1 0 1,-21 0 0,33-2 526,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,1 1 0,-1-1 1,0 1-1,0 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,1 1 0,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1 0 1,0 0-1,1 0 0,0 0 0,3 2 4,-1-1 1,1 1-1,-1 0 0,0-1 0,0 1 0,1 1 0,-1-1 0,-1 0 0,1 1 0,0 0 0,4 5 0,22 17 153,-21-20-328,1-2 0,0 1 1,0-1-1,0-1 0,0 0 1,1 0-1,10 1 0,-7-2-603,0 0-1,0-1 0,1-1 0,-1 0 0,0 0 0,0-1 1,0-1-1,13-4 0,-20 4 321,0 0 0,0 0 0,0 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,4-9 0,-5 9 1225,0-1 0,-1 1 0,1-1-1,-1 0 1,0 0 0,-1-7 0,0 14-673,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1 0 1,1-1 0,-1 1-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 0-1,-1 1 1,0 0 0,-26 9 758,22-8-822,0 1 0,0 0-1,1 0 1,-1 0 0,1 1 0,0-1-1,0 1 1,0 0 0,1 1 0,-1-1-1,1 1 1,0-1 0,0 1-1,1 0 1,0 0 0,-1 0 0,1 0-1,1 0 1,-1 1 0,1-1 0,0 1-1,0 8 1,26-15-1073,-21-1 1082,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,0-1 0,3-8 1,-4 10 1581,-1 33-1205,-1-28-483,0 1 1,1-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,1 0-1,0 0 1,-1-1 0,1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,0 1-1,1 0 1,-1-1 0,0 0-1,1 0 1,-1 1 0,0-1-1,1-1 1,-1 1-1,0 0 1,4-1 0,1 0-23,-1-1 1,0 1 0,1-1 0,-1 0 0,0 0-1,0-1 1,0 0 0,-1 0 0,1 0 0,-1-1-1,1 0 1,-1 0 0,5-5 0,39-49 1488,-50 64-1304,0 1 0,1-1 1,-1 0-1,1 1 0,1-1 0,0 8 0,0 17-158,-1 18 46,1-24-20,-2-1 0,-5 42 1,6-61-88,-1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 0,1-1 1,-1 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 0-1,0 0 0,-5 4 1,7-6 55,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-2 0-1,3 1 34,0-1-1,-1 1 0,1-1 0,0 0 0,0 1 1,0-1-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1-2-14,-1 1 0,1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,3-2 0,16-14-1092,1 1-1,1 2 0,27-16 0,-26 18 370,-1-2-1,0 0 1,21-21 0,-17-1 1440,-25 36-419,-1 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,0-4 0,0 6-220,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,-1 1 0,1-1-1,0 1 1,0-1 0,-1 1 0,1-1-1,0 1 1,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,-1 1 0,-1-1-1,-29 3 303,30-3-366,1 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,0 0 0,-1 1 0,2 1 0,3 6-191,0 0 0,0 0 0,1-1 0,14 15 0,-17-19 105,2 1 93,-1 0 0,-1 0-1,1 0 1,-1 0-1,0 1 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,-1-1 1,0 0 0,0 1-1,0-1 1,-3 12-1,2-16 40,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,1 0 0,0 0 0,0 1 0,-1-1-1,1-1 1,-1 1 0,1 0 0,-1 0 0,1-1-1,-6 1 1,-53 3 779,60-4-806,0 0-13,1 0 1,-1-1-1,1 1 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 1,0-1-1,1 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 1,14-21-445,38-27-2549,51-62-1,-84 86 1183,-1-2 0,-1 0 0,-1 0 0,-2-2 0,13-30 0,-14 9 5112,-13 46-2681,-1 0-1,0-1 0,1 1 1,-1 0-1,0 0 0,-1 0 1,1-1-1,0 1 0,-1 0 1,0 0-1,0 0 0,0 0 0,-2-4 1,3 6-577,-1 0 1,1 0-1,-1 1 1,0-1 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0 0,0 1-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1 0 1,0-1 0,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 1 0,-23 43 60,15-21 140,2 0 0,1 0 0,1 0-1,1 1 1,1-1 0,1 1 0,2 37 0,0-60-226,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,4-2 0,0 1 41,0-1 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 0 0,0-1 0,-1 1 0,0-1 1,1 0-1,-1 0 0,6-8 0,-7 6 20,-1 1-1,-1-1 1,1 0-1,-1 0 1,0 0 0,0 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,0-10 0,-1 17-87,1-1 1,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1-1,-1 1 1,-15 12-9,11-6 14,0 0 0,1 0 1,0 0-1,0 1 0,1 0 1,0-1-1,0 1 0,1 0 1,0 0-1,0 0 0,1 1 1,0-1-1,0 0 0,1 1 1,1 12-1,0-19-61,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,1 0 1,46-7-2885,-23-5-1534,-3-3-5027</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8847.72">6238 321 6739,'0'0'15111,"-7"0"-14407,17 0-512,8 0 33,10 0-225,4 0-193,-3 0-863,-1 0-1281,-7 0-1201,-6-2-4914</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9065.8">6284 400 9012,'0'0'12006,"-4"10"-11526,19-8 80,6-2-448,4 0-112,-1 0-608,1-4-1489,0-6-848,-7-2-2578,-8 0-4466</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9065.79">6284 400 9012,'0'0'12006,"-4"10"-11526,19-8 80,6-2-448,4 0-112,-1 0-608,1-4-1489,0-6-848,-7-2-2578,-8 0-4466</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9477.76">6409 157 12182,'0'0'9644,"-5"0"-9311,4 0-326,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-2 2 0,1 3 35,0 0 0,0 0 1,0 0-1,0-1 0,1 13 1,1-11-51,-1 0 0,1 0 1,1 0-1,0 0 1,0-1-1,0 1 0,0 0 1,1-1-1,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,1-1 1,-1 1-1,1-1 0,0 0 1,1-1-1,-1 1 0,1-1 1,0 0-1,0-1 1,0 1-1,0-1 0,1 0 1,-1-1-1,1 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0-2 1,12 1-1,-19-3 201,0 2-187,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,-1-1-1,1 1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1-1,-1 1 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,-6 3-6,-1 0 0,1 1 1,-1 0-1,1 0 0,0 0 1,1 1-1,-1 0 0,1 0 0,-5 6 1,-45 60 14,35-44 2,2-3 31,1 1 1,-14 29-1,12-8-4523</inkml:trace>
 </inkml:ink>
 </file>
@@ -9776,37 +9776,37 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">7216 57 10341,'0'0'9636,"0"-7"-8462,-4-42 1659,3 55-2868,0 1-1,-1-1 0,0 0 0,0 1 1,-5 8-1,-2 9 45,-19 54 77,12-36-60,2 0 1,-9 48-1,23-89-23,0-1 0,-1 1 0,1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,2-1 0,31 7-20,-20-7-81,-1-1 0,1 0 0,18-3 0,-26 3 4,1-1-1,0 1 1,-1-1-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 1,0 0-1,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,0 0-1,0-1 0,-1 1 1,0-1-1,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,-1 0-1,1 1 1,-1-1-1,0-8 1,-1 13 168,-15 27 0,-14 32 190,27-55-255,1 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,0 0 0,-1 1 1,1-1-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,2 5 0,-2-7-158,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1 0,-1 0-1,1-1 1,0 1 0,-1-1-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,4-1 1,1 0-724,-1 0-1,0 0 1,0 0 0,0-1 0,0 1-1,7-5 1,7-9-5340</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="118.7">7455 49 9764,'0'0'2770</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="682.01">7490 197 7619,'0'0'8100,"-6"14"-6851,-52 111 2427,58-124-3681,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,15-8-343,28-26-369,-33 25 486,-10 8 240,-1 0 1,1 0-1,0 1 0,0-1 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 1-1,16 22 231,-16-22-246,1 0 0,-1 0 0,1-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 0 1,0-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1-1 0,0 1 0,1 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0 0,3-2-1,-3 1-37,1-1-1,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0-1-1,-1 1 1,0 0-1,1-5 1,12-122-917,-13 119 3047,-2 47-1652,-8 43-1,1-21-1163,5 1-4145,3-49-1181</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1505.71">7752 278 9236,'0'0'7556,"-16"3"-7031,-5 2-416,0 1 0,1 1 0,-1 0 0,-31 17 0,51-24-111,1 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,11 7 80,21 3 172,-28-10-218,16 4-14,0 0 0,1-2 0,-1 0 0,1-2 0,0 0 0,-1-1 0,1-1 0,22-4 0,-41 4-22,0 1 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,1-1-1,-1 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1-3 0,-1 5 102,-1 0-95,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 2 0,-1 27 60,1-25-59,6-3-86,0 1 0,0-1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,6-1 1,-7-1 35,0 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1-1 0,0 0 1,0-1-1,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 0,-1-1 1,1 1-1,-1-1 0,3-7 1,1-3-123,0 0 0,-1-1 0,0 0 0,-2 0 0,4-26 0,-7-11 508,0 52 22,-17 10-294,15-6-71,1-1 0,-1 1 1,1-1-1,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2 3 0,3 7-7,0-1-1,1 1 0,12 17 0,-12-21 90,-1 1 1,1 1-1,6 17 0,-12-25-77,6 33 1585,-7-36-1556,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-2 0-1,-60 0-2145,59-1-472,1-6-3079</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1806.95">7993 263 13158,'0'0'5704,"6"1"-5477,48 4 191,98-1 0,-105-4-814,-47 0 236</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3400.41">8014 253 11333,'0'0'5779,"5"0"-5272,3 1-470,0 0 0,-1-1 1,1 0-1,0 0 0,0-1 1,0 0-1,0 0 1,-1-1-1,1 0 0,0 0 1,-1-1-1,0 0 0,10-5 1,-16 7-20,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1-1,1 0 1,-2-1 0,-2-1 20,1 0 0,0 0-1,0 1 1,-1 0 0,1-1-1,-1 1 1,0 1 0,1-1-1,-7 0 1,8 1-3,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 1,-3 6-1,1-2-15,1 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,1 1 1,1-1-1,-1 1 1,1 0-1,1 7 1,0-12-57,0 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1-1-1,0 1 0,3-1 1,13 2-575,-1 0 1,30-2-1,-32 0 298,13 0-374,-18 1 5,0 0 0,0-1-1,0 0 1,0-1 0,0 0 0,0 0-1,0-1 1,0 0 0,-1-1-1,18-7 1,-14-4-886,-13 13 1693,1 1 0,-1-1 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,-1 0 0,0-1 1,0 1 143,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,-1 0 0,-3 0-28,0 0 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 1 0,1-1 0,-1 1 0,1 1 0,-10 4-1,13-5-222,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,1 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,1 6-1,0-9-36,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,25-6-354,21-25 229,-40 23 127,0 0-1,-1-1 1,-1 0 0,1-1-1,-1 1 1,0-1-1,-1 0 1,0 0 0,-1 0-1,0-1 1,0 1 0,-1-1-1,2-10 1,0-18 389,0-77 0,-4 92 148,0 22 116,-7 39-191,0-11-284,1 0 0,2 0 0,0 1-1,1 29 1,3-49-137,0 1-1,1-1 0,0 0 1,0 0-1,1 1 1,0-1-1,0 0 0,1 0 1,0-1-1,0 1 0,1-1 1,0 1-1,0-1 1,1 0-1,0-1 0,0 1 1,1-1-1,6 6 1,-8-9-28,0-1 1,0 1-1,0-1 1,0 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,1 0 0,-1 0 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 0 1,6-3-1,-4 1-16,-1 1 1,1-1-1,-1 0 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,3-7 0,-5 8 53,-1 0 0,1-1-1,-1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1 0,0-1-1,-1 0 1,1-6-1,-1 10 167,-1 2-187,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0-1,0 1 1,0-1 0,0 0 0,0 3-1,-3 26 107,3-29-129,0 0 1,1 0-1,-1 1 1,1-1-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,2-1 1,46 0-787,-43 0 626,-1 1 139,0-1-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,0-1-1,-1 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,8-8 1304,9 41-1230,16-26-301,-33-4 261,1 0 1,0 0 0,0 1-1,0-1 1,-1 1-1,1 0 1,6 3-1,45 20-571,-55-22-175,-15-2-13998</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3552.43">8627 80 13846,'0'0'881,"92"31"-13495</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3852.79">9191 25 15719,'0'0'6881,"0"3"-6775,-10 39 85,-2 0 0,-21 49 0,-9 29 125,31-83-280,2 1 0,1 0 1,2 0-1,-1 51 0,15-89-3934,2-3-181</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5180.77">9737 240 10485,'0'0'9007,"1"-10"-8132,4-27-384,-6 35-472,1 1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,-2 1 0,-2-1-4,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1-1,1 0 1,-7 3 0,9-3-24,0 1 0,0-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,0 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 1 1,0-1 0,0 0-1,0 1 1,1-1 0,-1 0-1,1 1 1,-1-1 0,1 1-1,0-1 1,0 1 0,0-1-1,1 5 1,2-6-52,0-1 1,1 1-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,5-2-1,11-22 206,-19 22-34,1 1 0,0-1 0,-1 1 0,1 0-1,0-1 1,0 1 0,0 0 0,0 0 0,4-3-1,-5 5-109,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 2-1,4 18-91,7 53 230,-3-1 0,-4 2 0,-5 85 0,0-156-138,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,0-1 0,-4 3 0,5-3 4,0-1 0,0 1 0,0 0 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1-2-1,-1-1-32,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,0 1 0,0-1 0,0 0-1,0 1 1,1-1 0,0 0 0,0 1 0,0 0 0,0-1 0,1 1 0,4-6 0,4 0-406,0-1 1,1 2 0,0 0-1,1 0 1,0 1-1,15-7 1,-16 10 227,-1-1 1,0-1 0,0 0-1,0 0 1,-1-1 0,0 0-1,-1-1 1,0 0 0,15-18-1,-19 14 2499,-5 15-2236,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,0 3 1,0-3-36,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,1-1 1,-1 1-1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,4-1 0,-2 0-1,0 1 0,0-1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,5-5 0,1-5-98,-1-1 0,-1 0 0,0-1 0,-1 0 0,0 0-1,-2-1 1,6-23 0,-5 12 176,-1 0 0,-1-1 0,0-33 0,-8 165-211,0-68-265,3 1 0,1-1 1,1 1-1,7 37 0,-4-60-1988,-1-5-3340</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5309.03">10117 275 11509,'0'0'4178,"88"-63"-4706,-63 53-2049,-4 0-3506</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5460.85">10005 55 12102,'0'0'2080</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6755.2">10322 342 5651,'0'0'7782,"13"-12"-6635,1 0-941,-1 0 0,0-1 0,0 0 0,-2-1 0,0-1 0,0 0 0,-2 0 0,0-1 0,9-19 0,-13 19 246,-1-1 1,0 1 0,-1-1 0,0 1 0,-2-1-1,0-18 455,-19 44-622,12-2-270,0 0 1,1 0-1,0 0 1,1 1-1,-1 0 1,1 0-1,1 0 0,0 1 1,0-1-1,0 1 1,-1 12-1,-1 5 262,2 0 0,-1 44 1,3-68-258,1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,2 2 1,0-2-10,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,0-1 1,-1 0-1,1 0 0,3-1 1,5 1-59,-7 0 8,0-1 0,1 1 0,-1-1 0,0 0 0,0-1 0,1 1 0,-1-1 0,5-2 0,-5 1 8,1 1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1 0 0,1 0 0,7 0 0,-11 1-38,-1 5 83,0 0 35,0 0 0,0 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1-1-1,0 1 1,4 5 0,-5-9-36,1 1 1,-1-1-1,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 0 0,1 0 1,-1 1-1,0-1 1,0-1-1,0 1 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 0,0 0 1,0 0-1,0 1 1,2-3-1,3 0-18,0-1 0,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0 0,5-5 0,-8 7-4,0 0 1,0 0 0,-1-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,0-1 1,0 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0-7 0,-1 11-70,6 6-678,-5-6 719,-1 1-1,0-1 1,0 1-1,1-1 0,-1 1 1,0-1-1,0 0 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 0,2 0-17,1 1 0,-1-1-1,0 0 1,0 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,1-1-1,-1 0 1,0 0 0,0-1-1,0 1 1,0-1-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 0-1,5-4 882,-8 8-776,1 0 0,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,2 2-1,-1-2-36,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1-1,0 0 1,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,2-3-1,5-5-22,0-1-1,-1 0 0,1 0 0,7-13 0,-16 22 9,14-20-7,-1 0-1,-1-1 0,-1 0 0,-1-1 1,-1 0-1,7-28 0,-83 143 1308,61-80-1239,0 0 0,0 0 0,2 0 0,-1 1 0,2 0 0,-1 0 1,-1 21-1,31-34 92,47-15-703,-60 11 286,0 1 1,0 0 0,0 1-1,1 1 1,26 0 0,-39 0 258,0 1 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 1,0 1-1,0-1 14,0 1 1,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0 0,-1 0-1,-22 6 355,0-1 0,-1-1 0,-39 3 1,3-6-4866,50-2-2096</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9157.69">1 946 15799,'0'0'3869,"29"-4"-2439,111-2 1129,-83 2-2461,0 3-1,74 6 1,-107 2-686,-37-9-38,5-1 621,-1-1 0,1-1 0,0 1 1,0-1-1,1 0 0,-1-1 0,1 0 1,0 0-1,-10-13 0,8 10 63,0 0-1,0 1 1,0 0-1,-13-7 1,22 15 171,2 3-233,0 0-1,1 0 0,0 0 1,-1 0-1,1-1 0,0 1 1,1-1-1,-1 1 0,0-1 1,0 0-1,6 1 0,1 4 0,11 6-23,-9-6 42,0 1 0,0 0 1,-1 1-1,19 19 0,-28-26-24,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,-1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,-1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,-1 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,-1 0 0,-2 4-1,-11 11-1041,-1 0 0,0-1-1,-2 0 1,-31 22-1,4-4-4097,19-13-765</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12855.02">907 854 6963,'0'0'10189,"0"-3"-9547,0 1 1,0-1-1,0 0 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 1,0-1 0,2-2-1,258 21-1725,-265-15-3706,-2 1 2629,-2 1-287,-13 3-6910</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13877.48">932 760 320,'0'0'13014,"-1"-8"-11664,-1-13-837,-2-27 3673,1 34-1981,2 19-788,-8 64-1425,3-21 96,0 50 0,6-97 251,20-1-297,2 1-151,0-1-1,1-1 0,-1-1 0,0-1 1,42-11-1,-63 13 101,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,0-1 0,0-44 118,-1 25-143,0 21 45,-1 0-3,2 0 8,-5 32-256,0 11 448,1-1 0,3 42 1,1-74-111,0-8 3,0-1-85,0 1-173,0-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,-2 0-1590,-7 5-3090</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14384.03">1298 1022 11941,'0'0'6155,"9"-5"-5869,7-3-223,50-29 197,-63 34-249,0 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1-9 1,-1-68 356,-2 50 804,1 40-790,-2 54 263,1 47 422,2-106-950,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,5 7-1,8 5-1646,3-10-7679</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16049.5">1358 927 8900,'0'0'8799,"4"-2"-8322,16-2-415,0 0-1,-1 1 1,1 1-1,0 0 0,0 2 1,33 3-1,5-1-93,-12 0-427,-32 0 222,0-1 0,-1-1 0,1 0 0,0-1 0,0 0 0,23-6 0,-38 4 505,-11 1 335,-17 2 372,22 2-879,1 0 1,0 0-1,-1 1 1,1 0-1,0 0 1,1 0 0,-1 1-1,-9 8 1,12-10-54,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 6 0,1-9-36,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,-1-1 1,2 1-1,34-12-251,-31 9 284,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,2-10 1140,10 53-851,-13-36-320,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,2 0-1,-1 0 3,-1-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1-2 1,4-4-35,-1 0 0,-1-1 0,0 0 0,0 0 1,0 0-1,-1 0 0,4-15 0,-4 3-80,0 0 0,-1 0 1,0-43-1,-4 73 142,0 0 1,-1 0-1,0-1 1,0 1-1,-5 10 1,-7 33 209,11 69 335,3-120-564,3-2 47,1 0-1,-1 0 1,0 0-1,0-1 1,1 1-1,-1-1 1,0 0-1,0 0 0,-1 0 1,6-4-1,-6 4-67,1 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,0 2-1,1-1 0,-1 0 0,4 0 0,-6 1 0,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 3 0,0 0 5,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-3 2 1,-1-1 16,0 1-1,0-1 0,0 0 0,-1-1 1,1 1-1,0-1 0,-1 0 1,0-1-1,-6 2 0,55-27-205,20-3-14,-47 22 94,0-1 1,-1-1-1,0 0 1,0 0-1,-1-2 0,0 0 1,0-1-1,-1 0 1,16-16-1,-26 21 88,0 1-1,-1-1 1,1 0 0,-1 1 0,0-1-1,-1 0 1,1 0 0,-1 0-1,0-1 1,0 1 0,-1 0 0,0 0-1,0 0 1,0-1 0,0 1-1,-2-9 1,1 12 24,1 0 0,0 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,-1 0 1,1 0 0,0 1 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 1 0,-3 1 0,2 0 6,0-1 0,1 1 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,1 1 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,1-1 1,-1 5-1,-5 63 392,5-63-347,1 0 1,1 0-1,-1 0 0,1 0 0,1 0 0,-1 0 1,1-1-1,0 1 0,1 0 0,6 11 1,-6-14-40,0 0 1,0-1 0,0 1 0,0-1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1-1 0,6 1 0,-1 0-1,0-1-1,1 0 1,-1 0 0,1-1 0,-1-1 0,1 0 0,-1 0 0,0-1-1,0 0 1,0 0 0,15-7 0,-21 7-20,1 0 1,-1 0-1,0-1 0,1 1 1,-2-1-1,1 0 1,0 0-1,0-1 0,-1 1 1,0-1-1,0 0 0,0 1 1,0-2-1,0 1 1,-1 0-1,0 0 0,0-1 1,0 1-1,0-1 0,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 0,-1 0 1,0-5-1,-3-8-43,-4 20-47,5 1 84,1-1 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,1 1 0,0-1 0,-1 4 0,1-2 12,0 0 0,0 0 1,0 1-1,0-1 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,3 6 1,-4-8-2,1 0 1,0-1 0,0 1 0,0 0-1,0-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 0 1,1 0 0,4 0 0,-3 0-44,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,6-6 1,-6 4-11,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,0-8 1,-1 13 24,1-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1 0,-1 0-1,0-1 1,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,0 0-1,18 14-713,-15-9 689,0 0 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0 0 0,2 6-1,-5-10 86,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,-2 0 0,-11 2-268,0-1-1,0 0 1,-23-2-1,13 0-2693,10 1-3051</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19133.73">3935 849 12198,'0'0'6365,"2"6"-5551,6 25-122,-2 1 1,-1 0 0,-1 0-1,-1 50 1,3-62-3204,-5-19 2115,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,1 0 1,-1 1-1,0-1 0,1 0 0,1 0 1,11 0-6080</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19528.86">4091 977 6963,'0'0'10202,"-7"13"-9260,3-5-687,1 0-1,1 1 1,-1-1-1,1 0 1,1 1 0,0 0-1,0-1 1,0 15 0,2-22-244,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,1 0-1,1 0 0,40-4 144,-40 3-146,-1 0-1,1 0 1,0 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0-4 0,0 5 0,0 0 1,0-1 0,0 1-1,-1-1 1,0 1 0,1 0-1,-1-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 0 0,1 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-5 0 0,5-1-19,0 1 0,0 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 0,-1 2 0,-4 13-2102,5 7-3605,2-15 482</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20202.37">4416 946 5250,'0'0'13468,"-9"-3"-12633,-28-8-392,35 11-432,1 0 1,0-1-1,-1 1 0,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 1 0,1-1 1,-1 0-1,1 1 1,-1 1-1,-6 45 196,7-46-193,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0-1 0,0 1-1,1 0 1,-1-1-1,1 1 1,0-1 0,-1 1-1,4 1 1,-2-2-7,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1-1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 1 1,3-2-1,-5 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-2-3 0,2 2 3,-1 0-1,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 1 0,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,-3 0 0,5 1-51,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,-1 0-1,-1 18-5594,3-12-42</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20701.13">4623 952 8852,'0'0'9258,"-10"2"-8613,-32 3 28,40-4-628,0-1 1,0 1 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,-1 1 1,1-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0 0-1,1 3 1,-2-3-24,1 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,1 0-1,-1 0 1,0-1 0,1 1-1,0 0 1,-1-1 0,1 0-1,2 2 1,-1-2-4,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,3-2 0,-4 1-5,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,-1 1 0,0-1 0,0 0 0,0-5 0,0 7-12,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,0 0-1,-1-1 1,1 1-1,0 0 1,-1 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1 0,0-1-1,0 1 1,-2-1-1,0 0-173,-1 0 1,0 1-1,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-5 1 1,-14 11-5034,11-3 80</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21030.51">4267 1123 10149,'0'0'8452,"0"13"-8244,-3 1-32,-5 0-80,5-2-16,-8 0-80,4-2 32,-3-1-32,2-1-432,8-4-1297</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21430.03">4750 997 3666,'0'0'16306,"-4"10"-15567,2-6-681,-1 3 61,-1 1-1,1-1 0,0 1 1,1 0-1,0 0 0,0 0 1,1 0-1,0 1 1,0-1-1,2 16 0,-1-23-104,1 0 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,2-1 0,37-7 73,-37 6-82,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,-1-4-1,0 4-4,1 0 0,-1 1 1,1-1-1,-1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 1 0,1 0 1,-1-1-1,-2 1 0,3 0-56,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-4 3 0,-2 11-2955,8 8-3699,3-12-2221</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21812.54">5030 1040 13494,'0'0'9461,"-10"0"-9429,31 0 160,7 0-192,11 0 0,-3-4-609,-4-3-991,-8 3-1170,-6-2-207,-14-4-8852</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22019.29">5135 926 9540,'0'0'12502,"-39"29"-11766,36-5-399,3 6-193,0 5-128,0-5 128,7 2-144,4 1-16,-4-3-833,0-1-831,-7-7-2034,0-4-944</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24181.12">6606 990 6755,'0'0'13436,"-6"20"-11990,-3 1-1354,2-1 1,0 1 0,1 0-1,2 1 1,0-1 0,1 1 0,0 22-1,3-43-358,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 1,2 0-1,14 4-9743</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24546.83">6753 1083 11541,'0'0'7604,"-5"4"-6841,2-2-667,1 0 0,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 6 0,1-8-81,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,1 1-1,-1 0 1,1-1 0,40-10 151,-40 10-159,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 1-1,0-1 0,-2-2 0,-1 1 5,1-1 0,-1 1 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,-1 1 0,0-1 0,1 1 0,-1 0-1,0 0 1,-6 0 0,8 2-48,0-1 0,0 0-1,0 1 1,1 0 0,-1 0 0,0-1 0,1 2-1,-1-1 1,0 0 0,1 0 0,-1 1 0,-2 2-1,-5 12-2670,10-15 2359,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1 0-1,1 1 1,13 8-6218</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24754.06">6976 1117 13990,'0'0'7972,"50"-4"-7940,-25 4 16,-1 0-48,5 0-256,-4 0-1009,-4 0-880,-3 0-432,-4 0-3121</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25004.42">7092 1019 2161,'0'0'17389,"0"0"-17353,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 1,-2 8 251,1 1 0,0-1 0,0 0 0,1 1 1,0 0-1,1 13 0,-1-3-94,-3 90-762,3-109 393,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,2 0-1,11 2-8029</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26335.44">7476 1063 11749,'0'0'8978,"-10"6"-8423,-31 22 34,39-26-567,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,2-1 0,-1 1 1,0 0-1,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,1 1-1,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 1,0-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,4 1 1,7 1-93,-1-2 0,1 0 0,-1 0 0,1-1 0,-1 0 0,15-4 0,-23 4 42,0 0 0,-1 0 0,1-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,1-5 0,-3 9 42,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1 0,-14 6 248,-14 14 17,27-18-273,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,-1 1 0,0-1 1,1 0-1,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1-1 0,1 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,0-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,2 0 0,-1 0-28,0 0-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 0 1,1 0-1,0 0 0,6-4 1,-9 4 2,1 0 0,0 0 1,-1 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 0,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,-1 0-1,-1-4 1,1 5 14,1-1 0,-1 1 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1 0 1,-3-1-1,-35-2-117,35 3 105,4 0-10,19 13-176,-11-12 90,1 0-1,0-1 0,-1 0 1,1 0-1,0-1 0,-1 0 1,1 0-1,-1-1 1,1 0-1,-1-1 0,0 0 1,0 0-1,0-1 1,11-6-1,-14 6 93,0 0 0,0 1 0,-1-2 0,1 1 0,-1 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,0-8 0,1-2-51,0 13 68,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 1 1,-1-1-1,-3-3 0,4 6 7,0-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0 0,0-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 1 1,1-1-1,-1 0 1,0 0 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0 0,-9 33 464,9-27-246,-3 12 167,1 0 0,1 0-1,1 0 1,0 0 0,3 23-1,-1 3-79,-1-41-296,0-1 1,1 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,1 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1 0,0 0-1,0 1 1,1-2-1,-1 1 1,4-1 0,-5 1-13,-1 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,1-2-1,11-33-13,-4 8 34,-10 31-18,1-1 0,-1 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,-1 1 0,1-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,0 1 1,0-1 0,0 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,1-1-1,4 2 1,-5-2 3,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1-1,1-2 1,-1 0 16,-1 0-1,1 0 1,-1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-2-7-1,1 11-39,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 1-1,1-1 0,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 0,-10 2-7711</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26961.16">8125 1115 12694,'0'0'9212,"6"4"-8494,21 14-291,-26-18-402,0 1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 0 0,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 1 0,0-1-1,0 2 1,2 11 101,-1-14-133,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,2 1-1,25-11-272,-25 9 249,1 1-1,0-1 0,0 1 1,-1 0-1,1-1 0,0 2 1,8-2-1,17 44 222,-26-40-187,0 0-1,-1 0 0,1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,0-1 1,1 1-1,3-2 1,-3 0-6,1 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0 0,0 0 0,0 0-1,0-1 1,-1 1 0,5-7 0,-1 2-4,-2 0 1,1 0 0,-1 0-1,-1-1 1,0 0-1,0 0 1,0 0 0,-1-1-1,-1 1 1,1-1-1,-2 1 1,2-12 0,-3 21 5,-1-1 1,1 1-1,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1 0 1,-22 17 10,22-16-45,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,2 2 0,3 2-330,1 0 0,0-1 1,0 0-1,1 0 0,0-1 0,9 4 1,-4-2 256,-15-6 132,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-17 5 598,-21 1-525,35-6-28,-68 13-426,17-3-5165,17-2-3812</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">7180 57 10341,'0'0'9636,"0"-7"-8462,-4-42 1659,3 55-2868,0 1-1,-1-1 0,0 0 0,0 1 1,-5 8-1,-2 9 45,-18 54 77,11-36-60,2 0 1,-9 47-1,23-88-23,0-1 0,-1 1 0,1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,2-1 0,31 7-20,-20-7-81,-1-1 0,0 0 0,19-3 0,-26 3 4,1-1-1,0 1 1,-1-1-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 0 1,0 0-1,0-1 0,-1 1 1,0-1-1,1 0 1,-1 0-1,-1 0 1,1-1-1,-1 1 1,0 0-1,0-1 1,-1 0-1,1 1 1,-1-1-1,0-8 1,-1 13 168,-15 27 0,-14 32 190,27-55-255,1 0 0,0 0 1,1 0-1,-1-1 0,0 1 1,1 0-1,0 0 0,-1 1 1,1-1-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,2 5 0,-2-7-158,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1 0,-1 0-1,1-1 1,0 1 0,-1-1-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,4-1 1,1 0-724,-1 0-1,0 0 1,0 0 0,0-1 0,0 1-1,7-5 1,6-9-5340</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="118.7">7418 49 9764,'0'0'2770</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="682.01">7453 197 7619,'0'0'8100,"-6"14"-6851,-52 110 2427,58-123-3681,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,15-8-343,28-25-369,-33 24 486,-10 8 240,-1 0 1,1 0-1,0 1 0,0-1 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 1-1,16 21 231,-16-21-246,1 0 0,-1 0 0,1-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 0 1,0-1 0,1 1-1,-1 0 1,-1-1 0,2 1 0,-1-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1-1 0,0 1 0,1 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0 0,3-2-1,-3 1-37,1-1-1,-1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0-1-1,-1 1 1,1 0-1,-1-1 1,0 0-1,0 0 1,0-1-1,-1 1 1,0 0-1,1-5 1,12-122-917,-13 119 3047,-2 47-1652,-8 43-1,1-21-1163,5 0-4145,3-48-1181</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1505.71">7714 278 9236,'0'0'7556,"-16"3"-7031,-5 2-416,0 1 0,1 1 0,-1 0 0,-31 16 0,51-23-111,1 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,11 7 80,21 3 172,-28-10-218,16 4-14,0 0 0,1-2 0,-1 0 0,1-2 0,0 0 0,-1-1 0,0-1 0,23-4 0,-41 4-22,0 1 1,0 0-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,1-1-1,-1 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1-3 0,-1 5 102,-1 0-95,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 2 0,-1 27 60,1-25-59,6-3-86,0 1 0,0-1 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,6-1 1,-7-1 35,0 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1-1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,-1-1 1,1 1-1,-1-1 0,3-6 1,1-4-123,0 0 0,-1-1 0,0 0 0,-2 0 0,4-26 0,-7-11 508,0 52 22,-17 10-294,15-6-71,1-1 0,-1 1 1,1-1-1,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2 3 0,3 7-7,0-1-1,1 1 0,12 17 0,-12-21 90,-1 1 1,1 1-1,6 16 0,-12-24-77,6 33 1585,-7-36-1556,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-2 0-1,-60 0-2145,59-1-472,1-6-3079</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1806.95">7954 263 13158,'0'0'5704,"5"1"-5477,49 4 191,97-1 0,-104-4-814,-47 0 236</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3400.41">7974 253 11333,'0'0'5779,"5"0"-5272,3 1-470,0 0 0,-1-1 1,1 0-1,0 0 0,0-1 1,0 0-1,0 0 1,-1-1-1,1 0 0,0 0 1,-1-1-1,0 0 0,10-5 1,-16 7-20,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1-1,1 0 1,-2-1 0,-2-1 20,1 0 0,0 0-1,0 1 1,-1 0 0,1-1-1,-1 1 1,0 1 0,1-1-1,-7 0 1,8 1-3,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 1,-3 6-1,1-2-15,1 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,1 1 1,1-1-1,-1 1 1,1 0-1,1 7 1,0-12-57,0 0 0,-1 1 1,1-2-1,0 1 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1-1-1,0 1 0,3-1 1,13 2-575,-1 0 1,30-2-1,-32 0 298,13 0-374,-19 1 5,1 0 0,0-1-1,0 0 1,0-1 0,0 0 0,0 0-1,0-1 1,0 0 0,-1-1-1,18-7 1,-14-4-886,-13 13 1693,1 1 0,-1-1 0,0 0 1,0 0-1,1 1 0,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,-1 0 0,0-1 1,0 1 143,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,-1 0 0,-3 0-28,0 0 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 1 0,1-1 0,-1 1 0,1 1 0,-10 4-1,13-5-222,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 2 1,0-1-1,0 0 1,0 1-1,1 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,0 0 1,0 6-1,0-9-36,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,25-6-354,21-25 229,-40 23 127,0 0-1,-1-1 1,-1 0 0,1 0-1,-1 0 1,0-1-1,-1 0 1,0 0 0,-1 0-1,0-1 1,0 1 0,-1-1-1,2-10 1,0-18 389,0-77 0,-4 92 148,0 22 116,-7 39-191,0-11-284,1 0 0,2 0 0,0 1-1,1 29 1,3-49-137,0 1-1,1-1 0,0 0 1,0 0-1,1 1 1,0-1-1,0 0 0,1-1 1,0 0-1,0 1 0,1-1 1,0 1-1,0-1 1,1 0-1,0-1 0,0 1 1,1-1-1,6 6 1,-8-9-28,0-1 1,0 1-1,-1-1 1,1 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,1 0 0,-1 0 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 0-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 0 1,6-3-1,-4 1-16,-1 1 1,1-1-1,-1 0 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,3-7 0,-5 8 53,-1 0 0,1-1-1,-1 1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1 0,0-1-1,-1 0 1,1-6-1,-1 10 167,-1 2-187,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0-1,0 1 1,0-1 0,0 0 0,0 3-1,-3 25 107,3-28-129,0 0 1,1 0-1,-1 1 1,1-1-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,2-1 1,46 0-787,-43 0 626,-1 1 139,0-1-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,0-1-1,-1 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,8-7 1304,9 39-1230,16-25-301,-33-4 261,0 0 1,1 0 0,0 1-1,0-1 1,-1 1-1,1 0 1,6 3-1,45 20-571,-55-22-175,-15-2-13998</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3552.43">8584 80 13846,'0'0'881,"92"31"-13495</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3852.79">9146 25 15719,'0'0'6881,"0"3"-6775,-10 39 85,-2 0 0,-21 49 0,-9 28 125,31-82-280,2 1 0,1 0 1,2 0-1,-1 51 0,15-89-3934,2-3-181</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5180.76">9689 240 10485,'0'0'9007,"1"-10"-8132,4-27-384,-6 35-472,1 1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0-1,0 0 1,-2 1 0,-2-1-4,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1-1,1 0 1,-7 3 0,9-3-24,0 1 0,0-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,0 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 1 1,0-1 0,0 0-1,0 1 1,1-1 0,-1 0-1,1 1 1,-1-1 0,1 1-1,0-1 1,0 1 0,0-1-1,1 5 1,2-6-52,0-1 1,1 1-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 1,5-2-1,11-22 206,-19 22-34,1 1 0,0-1 0,-1 1 0,1 0-1,0-1 1,0 1 0,0 0 0,0 0 0,4-3-1,-5 5-109,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 2-1,4 18-91,7 53 230,-3-2 0,-4 3 0,-5 85 0,0-156-138,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,0-1 0,-4 3 0,5-3 4,0-1 0,0 1 0,0 0 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 1-1,-1-1 1,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1-2-1,-1-1-32,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,0 1 0,0-1 0,0 0-1,0 1 1,1-1 0,0 0 0,0 1 0,0 0 0,0-1 0,1 1 0,4-6 0,4 0-406,0-1 1,1 2 0,0 0-1,1 0 1,0 1-1,15-7 1,-17 10 227,0-1 1,0-1 0,0 0-1,0 0 1,-1-1 0,0 0-1,-1-1 1,0 0 0,15-18-1,-19 14 2499,-5 15-2236,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,0 3 1,0-3-36,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,1-1 1,-1 1-1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,4-1 0,-2 0-1,0 1 0,0-1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,5-5 0,1-5-98,-1-1 0,-1 1 0,0-2 0,-1 0 0,0 0-1,-2-1 1,6-23 0,-5 12 176,-1 0 0,-1-1 0,0-33 0,-8 165-211,0-68-265,3 1 0,1-1 1,1 1-1,7 36 0,-4-59-1988,-1-5-3340</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5309.03">10067 275 11509,'0'0'4178,"88"-63"-4706,-64 53-2049,-3 0-3506</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5460.85">9956 55 12102,'0'0'2080</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6755.2">10271 341 5651,'0'0'7782,"13"-12"-6635,1 0-941,-1 1 0,0-2 0,0 0 0,-2-1 0,0-1 0,0 0 0,-3 0 0,1-1 0,9-19 0,-13 19 246,-1-1 1,0 1 0,-1-1 0,0 1 0,-2-1-1,0-18 455,-19 44-622,12-2-270,0 0 1,1 0-1,0 0 1,1 1-1,-1 0 1,2 0-1,0 0 0,0 1 1,0-1-1,0 1 1,-1 12-1,-1 5 262,2 0 0,-1 44 1,3-68-258,1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,2 2 1,0-2-10,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 1,0 0-1,1 0 0,3-1 1,5 1-59,-7 0 8,0-1 0,1 1 0,-1-1 0,0 0 0,0-1 0,1 1 0,-1-1 0,5-2 0,-5 1 8,1 1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1 0 0,1 0 0,7 0 0,-11 1-38,-1 5 83,0 0 35,0 0 0,0 0-1,1 0 1,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,1-1-1,0 1 1,4 5 0,-5-9-36,1 1 1,-1-1-1,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0-1-1,0 0 0,1 0 1,-1 1-1,0-1 1,0-1-1,0 1 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 0,0 0 1,0 0-1,0 1 1,2-3-1,2 0-18,1-1 0,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0 0,5-5 0,-8 7-4,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0-1 0,0 1-1,0-1 1,0 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0-7 0,-1 11-70,6 6-678,-5-6 719,-1 1-1,0-1 1,0 1-1,1-1 0,-1 1 1,0-1-1,0 0 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 0,2 0-17,1 1 0,-1-1-1,0 0 1,0 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,1-1-1,-1 0 1,0 0 0,0-1-1,0 1 1,0-1-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 0-1,5-4 882,-8 8-776,1 0 0,0 0 1,0 0-1,1 0 0,-1 1 1,0-1-1,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,2 2-1,-1-2-36,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1-1,0 0 1,-1 1 0,2-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,2-3-1,5-5-22,0-1-1,-1 0 0,1 0 0,7-13 0,-16 22 9,14-20-7,-1 0-1,-1-1 0,-1 0 0,-1-1 1,-1 0-1,7-28 0,-83 143 1308,61-80-1239,0 0 0,0 0 0,2 0 0,-1 1 0,2 0 0,-1 0 1,-1 21-1,31-34 92,47-15-703,-60 11 286,0 1 1,-1 0 0,1 1-1,1 1 1,26 0 0,-39 0 258,0 1 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 1,-1-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 1,0 1-1,0-1 14,0 1 1,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,0 0 1,1 0 0,-1 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0 0,-1 0-1,-22 6 355,0-1 0,-1-1 0,-38 3 1,2-6-4866,50-2-2096</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9157.69">1 944 15799,'0'0'3869,"29"-4"-2439,110-1 1129,-82 1-2461,0 3-1,73 6 1,-106 1-686,-37-8-38,5 0 621,-1-2 0,1-1 0,0 1 1,0-1-1,1 0 0,-1-1 0,1 0 1,0 0-1,-10-13 0,8 10 63,0 0-1,0 1 1,1 0-1,-14-7 1,22 15 171,2 3-233,0 0-1,1 0 0,0 0 1,-1 0-1,1-1 0,0 1 1,1-1-1,-2 1 0,1-1 1,0 0-1,6 1 0,1 4 0,11 6-23,-9-6 42,0 1 0,0 0 1,-1 1-1,19 18 0,-28-25-24,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,-1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,-1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,-1 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,-1 0 0,-2 4-1,-11 11-1041,-1 0 0,0-1-1,-2 0 1,-31 22-1,5-4-4097,18-13-765</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12855.02">903 853 6963,'0'0'10189,"0"-3"-9547,0 1 1,0-1-1,0 0 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 1 1,-1-1 0,3-2-1,257 21-1725,-264-15-3706,-2 1 2629,-2 1-287,-13 3-6910</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13877.48">927 759 320,'0'0'13014,"-1"-8"-11664,-1-13-837,-2-27 3673,1 34-1981,2 19-788,-8 64-1425,4-21 96,-1 50 0,6-97 251,19-1-297,3 1-151,0-1-1,1-1 0,-1-1 0,0-1 1,42-11-1,-63 13 101,1 0-1,-1 1 1,0-1 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,0-1 0,0-44 118,-1 25-143,0 21 45,0 0-3,1 0 8,-5 32-256,0 11 448,1-1 0,3 41 1,1-73-111,0-8 3,0-1-85,0 1-173,0-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,-2 0-1590,-7 5-3090</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14384.03">1292 1020 11941,'0'0'6155,"9"-5"-5869,6-3-223,51-29 197,-63 34-249,0 0 0,0 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,0 0-1,0 1 1,0 0-1,-1-1 1,1 0-1,-1 0 1,0 0-1,0 0 0,1-9 1,-1-68 356,-2 50 804,1 40-790,-2 54 263,1 46 422,2-105-950,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,5 7-1,8 5-1646,3-10-7679</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16049.5">1351 926 8900,'0'0'8799,"4"-2"-8322,16-2-415,0 0-1,-1 1 1,1 1-1,0 0 0,0 2 1,32 3-1,6-1-93,-12 0-427,-32 0 222,0-1 0,-1-1 0,1 0 0,0-1 0,0 0 0,22-6 0,-37 4 505,-11 1 335,-16 2 372,21 2-879,1 0 1,0 0-1,-1 1 1,1 0-1,0 0 1,1 0 0,-1 1-1,-9 8 1,12-11-54,0 2 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 6 0,1-9-36,1 1-1,-1 0 1,1 0-1,-1-1 1,1 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,-1-1 1,2 1-1,34-12-251,-31 9 284,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-2 1 0,2-1 0,-1 0 0,0 1 0,2-11 1140,10 52-851,-13-35-320,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,2 0-1,-1 0 3,-1-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1-2 1,4-4-35,-1 0 0,-1 0 0,0-1 0,0 0 1,0 0-1,-1 0 0,4-15 0,-4 3-80,0 0 0,-1 0 1,0-43-1,-4 73 142,0 0 1,-1 0-1,0-1 1,0 1-1,-5 10 1,-7 33 209,11 68 335,3-119-564,3-2 47,1 0-1,-1 0 1,0 0-1,0-1 1,1 1-1,-1-1 1,0 0-1,0 0 0,-1 0 1,6-4-1,-6 4-67,1 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,-1 2-1,2-1 0,-1 0 0,4 0 0,-6 1 0,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 3 0,0 0 5,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-3 2 1,-1-1 16,0 1-1,0-1 0,1 0 0,-2-1 1,1 1-1,0-1 0,-1 0 1,0-1-1,-6 2 0,54-27-205,21-3-14,-47 22 94,0-1 1,-1-1-1,0 0 1,0 0-1,-1-2 0,0 1 1,0-2-1,-1 0 1,15-16-1,-25 21 88,0 1-1,-1-1 1,1 0 0,-1 1 0,0-1-1,-1 0 1,1 0 0,-1 0-1,0-1 1,0 1 0,-1 0 0,0 0-1,0 0 1,0-1 0,0 1-1,-2-9 1,1 12 24,1 0 0,0 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0-1-1,-1 0 1,1 0 0,0 1 0,-1-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1-1,1 1 1,-1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 1 0,-3 1 0,2 0 6,0-1 0,1 1 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,1 1 0,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 0,1-1 1,-1 5-1,-5 63 392,5-63-347,1 0 1,1 0-1,-1 0 0,1 0 0,1 0 0,-1 0 1,1-1-1,0 0 0,1 1 0,6 11 1,-6-14-40,0 0 1,0-1 0,0 1 0,0-1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0-1 0,1 0 0,-2 0 0,2-1-1,-1 1 1,1-1 0,6 1 0,-1 0-1,0-1-1,1 0 1,-1 0 0,1-1 0,-1-1 0,1 0 0,-1 0 0,0-1-1,0 0 1,0 0 0,15-7 0,-21 7-20,1 0 1,-1 0-1,0-1 0,1 1 1,-2-1-1,1 0 1,0 0-1,0-1 0,-2 1 1,1-1-1,0 0 0,0 1 1,0-2-1,0 1 1,-1 0-1,0 0 0,0-1 1,0 2-1,0-2 0,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 0,-1 0 1,0-5-1,-3-8-43,-4 20-47,5 1 84,1-1 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,1 1 0,0-1 0,-1 4 0,1-2 12,0 0 0,0 0 1,0 1-1,0-1 0,1 0 1,0 0-1,0-1 0,0 1 1,0 0-1,1 0 0,3 6 1,-4-8-2,1 0 1,0-1 0,0 1 0,0 0-1,0-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 0 1,1 0 0,4 0 0,-3 0-44,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,6-6 1,-6 4-11,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,0-8 1,-1 13 24,1-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 0-1,1 1 1,-1-1 0,0 1-1,0-1 1,1 1 0,-1 0-1,0-1 1,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,0 0-1,18 14-713,-15-9 689,-1 0 1,0 1-1,1-1 1,-1 1-1,0 0 1,0 0 0,2 6-1,-5-10 86,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,-2 0 0,-11 2-268,0-1-1,0 0 1,-23-2-1,13 0-2693,10 1-3051</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19133.73">3916 848 12198,'0'0'6365,"2"6"-5551,6 25-122,-3 1 1,0-1 0,-1 1-1,-1 50 1,3-62-3204,-5-19 2115,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,1 0 1,-1 1-1,0-1 0,1 0 0,1 0 1,11 0-6080</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19528.86">4071 975 6963,'0'0'10202,"-7"13"-9260,3-5-687,1 0-1,1 1 1,-1-1-1,1 0 1,1 1 0,0 0-1,0-1 1,0 15 0,2-22-244,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,1 0-1,1 0 0,40-4 144,-40 3-146,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,0-4 0,0 5 0,0 0 1,0-1 0,0 1-1,-1-1 1,0 1 0,1 0-1,-1-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-5 0 0,5-1-19,0 1 0,0 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 0,-1 2 0,-4 13-2102,5 7-3605,2-15 482</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20202.37">4394 944 5250,'0'0'13468,"-9"-3"-12633,-28-7-392,35 10-432,1 0 1,0-1-1,-1 1 0,1 0 1,-1 0-1,1 1 0,-1-1 1,1 0-1,0 0 1,-1 1-1,2-1 0,-2 1 1,1-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 1 0,1-1 1,-1 0-1,1 1 1,-1 1-1,-6 45 196,7-46-193,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,1 0 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0-1 0,0 1-1,1 0 1,-1-1-1,1 1 1,0-1 0,-1 1-1,4 1 1,-2-2-7,-1 0 1,1 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1-1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 1 1,3-2-1,-5 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 1 0,-1-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,-2-3 0,2 2 3,-1 0-1,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 1 0,-1-1 1,1 1-1,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 1,0 0-1,-3 0 0,5 1-51,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,-1-1-1,-1 19-5594,3-12-42</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20701.12">4600 950 8852,'0'0'9258,"-10"2"-8613,-32 3 28,40-4-628,0-1 1,0 1 0,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,0 0 0,0 0-1,-1 1 1,1-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,0 0 0,0 0-1,1 3 1,-2-3-24,1 0-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,1 0-1,-1 0 1,0-1 0,1 1-1,0 0 1,-2-1 0,2 0-1,2 2 1,-1-2-4,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,3-2 0,-4 1-5,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,-1 1 0,0-1 0,0 0 0,0-5 0,0 7-12,0 0-1,0 0 1,0-1-1,0 1 1,0 0 0,0 0-1,-1-1 1,1 1-1,0 0 1,-1 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1 0,0-1-1,0 1 1,-2-1-1,0 0-173,-1 0 1,0 1-1,1-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-5 1 1,-14 11-5034,12-3 80</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21030.51">4246 1121 10149,'0'0'8452,"0"13"-8244,-3 1-32,-5 0-80,5-2-16,-8 0-80,4-2 32,-3-1-32,2-1-432,8-4-1297</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21430.03">4727 995 3666,'0'0'16306,"-4"10"-15567,2-6-681,-1 3 61,-1 1-1,1-1 0,0 1 1,1 0-1,0 0 0,0 0 1,1 0-1,0 1 1,0-1-1,2 16 0,-1-23-104,1 0 0,0 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,2-1 0,36-7 73,-36 6-82,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,-1-4-1,0 4-4,1 0 0,-1 1 1,1-1-1,-1 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 1 0,1 0 1,-1-1-1,-2 1 0,3 0-56,-1 0 0,1 0 0,0 0 0,-1 0-1,1 0 1,1 1 0,-2-1 0,1 1 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,-4 3 0,-2 11-2955,8 8-3699,3-12-2221</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21812.54">5005 1038 13494,'0'0'9461,"-10"0"-9429,31 0 160,7 0-192,11 0 0,-3-4-609,-5-3-991,-7 3-1170,-6-2-207,-14-4-8852</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22019.29">5110 925 9540,'0'0'12502,"-39"28"-11766,36-4-399,3 6-193,0 5-128,0-5 128,7 2-144,4 1-16,-4-3-833,0-1-831,-7-7-2034,0-4-944</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24181.12">6573 988 6755,'0'0'13436,"-6"20"-11990,-3 1-1354,2-1 1,1 1 0,0 0-1,2 1 1,0-1 0,1 1 0,0 22-1,3-43-358,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,0 1 1,2 0-1,13 4-9743</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24546.83">6720 1081 11541,'0'0'7604,"-5"4"-6841,2-2-667,1 0 0,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 6 0,1-8-81,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,1 1-1,-1 0 1,1-1 0,39-10 151,-39 10-159,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 1-1,0-1 0,-2-2 0,-1 1 5,1-1 0,-1 1 0,1 0 0,-1 0-1,0 1 1,0-1 0,1 1 0,-2 0 0,1 0-1,0 0 1,-1 1 0,0-1 0,1 1 0,-1 0-1,0 0 1,-6 0 0,8 2-48,0-1 0,0 0-1,0 1 1,1 0 0,-1 0 0,0-1 0,1 2-1,-1-1 1,0 0 0,1 0 0,-1 1 0,-2 2-1,-5 12-2670,10-15 2359,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1 0-1,1 1 1,13 8-6218</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24754.06">6942 1115 13990,'0'0'7972,"49"-4"-7940,-24 4 16,-1 0-48,5 0-256,-4 0-1009,-4 0-880,-3 0-432,-4 0-3121</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25004.42">7057 1017 2161,'0'0'17389,"0"0"-17353,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 1,-2 8 251,1 1 0,0-1 0,0 0 0,1 1 1,0 0-1,1 13 0,-1-3-94,-3 90-762,3-109 393,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,2 0-1,11 2-8029</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26335.44">7439 1061 11749,'0'0'8978,"-10"6"-8423,-31 22 34,39-26-567,0-1 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,2-1 0,-1 1 1,0 0-1,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,1 1-1,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 1,0-1-1,0 0 0,-1 0 0,1 1 0,0-1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,4 1 1,7 1-93,-1-2 0,1 0 0,-1 0 0,1-1 0,-1 0 0,15-4 0,-23 4 42,0 0 0,-1 0 0,1-1 0,0 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,1-5 0,-3 9 42,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1 0,-14 6 248,-13 14 17,26-18-273,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,-1 1 0,0-1 1,1 0-1,-1 1 0,1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1-1 0,1 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,0-1 0,-1 1 1,2 0-1,-1-1 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,2 0 0,-1 0-28,0 0-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 0 1,1 0-1,0 0 0,6-4 1,-9 4 2,1 0 0,0 0 1,-1 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 0,-1 0 1,1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,-1 0-1,-1-4 1,1 5 14,1-1 0,-1 1 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1 0 1,-3-1-1,-35-2-117,35 3 105,4 0-10,19 13-176,-11-12 90,1 0-1,0-1 0,-1 0 1,1 0-1,0-1 0,-1 0 1,1 0-1,-1-1 1,1 0-1,-1-1 0,0 0 1,0 0-1,0-1 1,11-6-1,-14 6 93,0 0 0,0 1 0,-1-2 0,0 1 0,0 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,0-8 0,1-2-51,0 13 68,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 1 0,-1-1 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,1 1 1,-1-1-1,-3-3 0,4 6 7,0-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0 0,0-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 1 1,1-1-1,-1 0 1,0 0 0,1 1-1,-1-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1 0 0,-8 32 464,8-26-246,-3 12 167,1 0 0,1 0-1,1 0 1,0 0 0,3 23-1,-1 3-79,-1-41-296,0-1 1,1 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,1 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1 0,0 0-1,0 1 1,1-2-1,-1 1 1,4-1 0,-5 1-13,-1 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1-1-1,1 1 1,1-2-1,11-33-13,-4 8 34,-10 31-18,1-1 0,-1 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,-1 1 0,1-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,0 1 1,0-1 0,0 1 0,1-1 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,1-1-1,4 2 1,-5-2 3,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 0 1,0 1 0,-1-1-1,1 0 1,0 0-1,-1 0 1,1-1 0,-1 1-1,0 0 1,1-1-1,1-2 1,-1 0 16,-1 0-1,1 0 1,-1-1-1,0 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-2-7-1,1 11-39,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 1-1,1-1 0,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 0,-9 2-7711</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26961.16">8085 1113 12694,'0'0'9212,"6"4"-8494,21 14-291,-26-18-402,0 1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 0 0,-1 1-1,0-1 1,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 1 0,0-1-1,0 2 1,2 11 101,-1-14-133,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,2 1-1,24-11-272,-24 9 249,1 1-1,0-1 0,0 1 1,-1 0-1,1-1 0,0 2 1,8-2-1,17 44 222,-26-40-187,0 0-1,-1 0 0,1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,0-1 1,1 1-1,3-2 1,-3 0-6,1 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0 0,0 0 0,0 0-1,0-1 1,-1 1 0,4-7 0,0 2-4,-2 0 1,1 0 0,-1 0-1,-1-1 1,0 0-1,0 0 1,0 0 0,-1-1-1,-1 1 1,1-1-1,-2 1 1,2-12 0,-3 21 5,-1-1 1,1 1-1,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,-1 0 1,-22 17 10,22-16-45,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,2 2 0,3 2-330,1 0 0,0-1 1,0 0-1,1 0 0,0-1 0,9 4 1,-4-2 256,-15-6 132,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-17 5 598,-21 1-525,35-6-28,-67 13-426,16-3-5165,17-2-3812</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -9842,7 +9842,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2935.29">2451 71 10085,'0'0'6339,"-14"31"-7636,21-13-3537,7-4-2994</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3561.09">2618 167 10309,'0'0'8822,"-14"6"-7429,-44 23-446,56-28-915,0 0-1,0 0 1,0 1 0,0-1-1,1 0 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 1-1,0-1 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 1 1,0-1 0,0 0-1,0 0 1,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,1 1 0,0-1-1,0 0 1,-1 0-1,1 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1 0-1,-1-1 1,1 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,0 0-1,0 0 1,3 1 0,18 1-211,-1-1 1,1-1-1,24-1 0,-39-1-108,0 1 0,1-2 0,-1 1-1,0-1 1,0 0 0,0 0-1,0-1 1,0 0 0,0-1-1,-1 0 1,11-6 0,-14 6 96,0-1-1,0 1 1,-1 0 0,1-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0-1 0,0 1 0,0-1-1,-1 1 1,2-11 0,0-7 785,-2 0 0,-1-31 0,0 26 2970,-10 71-2913,8-34-586,0-1-1,1 1 1,0 0 0,1 0-1,0 0 1,0 0 0,1 0-1,0 0 1,4 16 0,-4-22-54,0 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1-1 1,7 1-1,-1 0-114,0-1 1,1 0-1,-1 0 1,0-1-1,0 0 1,0-1-1,0 0 1,12-4-1,-18 5 90,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,-1 0 1,0 0 0,1-6 0,-1 103 243,0-94-329,0 1 1,0-1-1,0 1 1,1-1 0,-1 0-1,0 1 1,0-1-1,0 0 1,0 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,1 0 1,-1 1 0,0-1-1,1 0 1,-1 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,0-1 1,7-6-6054,-8-4-1161</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3867.95">2699 119 11749,'0'0'1340,"15"0"-1028,1 0-32,104-3-2149,-105 2 1870,1 0 1,-1-1-1,0-1 0,0 0 1,0-2-1,15-5 0,-12-3 3097,-12 9 390,0 16-6461,-3-3-2745</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4220.9">3184 186 11221,'0'0'9271,"-4"13"-8972,-13 43-30,17-56-246,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0-1-1,1 1 1,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,0 0 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,40-11 460,-38 8-470,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-8 0,-2 11-17,-1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1 0-1,-1 0 1,-3 1 0,0-2-419,-19 1-277,15 5-2746,5 5-4776</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4220.89">3184 186 11221,'0'0'9271,"-4"13"-8972,-13 43-30,17-56-246,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0 0,0-1-1,1 1 1,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0-1 1,0 0 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,40-11 460,-38 8-470,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-8 0,-2 11-17,-1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1 0-1,-1 0 1,-3 1 0,0-2-419,-19 1-277,15 5-2746,5 5-4776</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5322.5">3288 159 1889,'37'-1'11007,"-12"10"-5510,-23-6-5303,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 6 0,1-8-175,0-1 0,1 1-1,-1 0 1,0-1-1,0 1 1,1 0 0,-1-1-1,0 1 1,1 0-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 0-1,35 2 162,6 3-146,-35-3-59,0 1 1,0-1 0,0-1-1,1 1 1,-1-1-1,1 0 1,-1-1-1,1 0 1,8-1 0,-14 1 4,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1-1 1,0 1 0,-1-1-1,1 1 1,0-1-1,-1 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,0 0 1,1 0 0,-1-4-1,0 5 19,0-1-1,1 1 0,-1-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,-2 0 1,-1-1 3,-1 1 0,1 0 0,0 1 0,0-1 1,-1 1-1,1 0 0,-8 0 0,-2 1-39,10 0-459,9 1-783,11 1 39,125-7-1647,-141 4 2917,0 0 0,1 0-1,-1 0 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0 0,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,1 1-1,-1-1 1,0 0 0,0 1-1,1-1 1,-1 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 1-1,0-1 1,1 0 0,-1 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,1 25 1387,0-25-1330,-1 1 0,1 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1 1 0,3-2-182,1 0-1,0 0 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 1,-1 1-1,1-1 0,-1-1 1,1 1-1,9-5 0,-13 5 88,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1-1,1 0 1,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0-1,0-3 1,1 7 9,-1 1 0,0-1 0,1 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,-1 0 0,1 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1-1 0,-1 1 0,0 0 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,1 0 0,6 1 5,-1-1 0,0 0 0,0-1 0,0 0-1,11-2 1,-5-9 271,-5 4 1762,-6 19-1204,0 22-495,1 1 0,2-1 0,1 1 0,1-2-1,26 64 1,10 41 742,-43-133-1046,1 0 0,-1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,-1 0 0,0 6 0,1-8-30,-1-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-3-1 0,-4 2 33,0-1 0,0 0 0,0 0 0,-1-1 0,1 0 0,0-1 0,0 0 0,0 0 0,1-1 0,-14-5-1,18 6-8,0-1 0,0 1-1,0 0 1,1-1-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,0-1-1,-1 1 1,2-1 0,-1 1-1,0-1 1,0 1-1,1-1 1,0 0 0,0 1-1,0-1 1,0 0-1,1 1 1,1-7 0,-1 5-60,0 1 0,1-1 0,0 1 1,0 0-1,0-1 0,0 1 0,1 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,1 1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 1,0-1-1,1 2 0,7-4 0,47-14-2105,-5 7-3426,-51 12 5018,29-5-6062</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5479.11">4298 423 6643,'0'0'18889,"3"-2"-18889</inkml:trace>
 </inkml:ink>
@@ -9874,7 +9874,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">17 187 6995,'0'0'7292,"-4"0"-6938,-8 0 3234,41 2-2291,47 1-883,115 6-9,-191-9-341,11-8 30,-12 6-130,0 1 1,1-1 0,-1 0-1,0 0 1,-1 1 0,1-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1 0-1,-1 0 1,0 0 0,-2-2-1,-35-20-270,30 19 332,-33-27 689,44 30-717,1 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1-1,1 1 1,0-1 0,4 3-1,39 16 15,-35-14-47,38 14-446,33 15-1055,-82-33 1539,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,1 1-1,-1-1 1,0 1-1,0-1 1,0 1 0,0-1-1,1 1 1,-1 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,1 1 0,0-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 1-1,-23 20 14,19-17-2,-10 9-337,-9 7 494,0 1 1,-21 27-1,37-39-1170,1 0 0,1 1 0,0 0 0,0 0 0,-5 15 0,4-8-4385</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1638.37">1094 174 3618,'0'0'9801,"0"-4"-9024,0 4-739,0-1 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 0 0,1 1 1,0-1-1,0 0 0,-1 1 1,1-1-1,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1 0-1,0-1 0,-1 0 1,-31 0 334,24 3-280,0 0 1,0 0-1,1 1 0,-1 0 0,1 1 0,-1 0 1,-10 7-1,13-8-26,0 0 0,0 1 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,-5 10 1,10-14-72,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,2 0 0,25 7-220,-18-8 14,1 0-1,0 0 1,0-1 0,11-2-1,-16 1-57,1-1 0,-1 1 0,0-1 0,0 1 0,0-2 0,0 1-1,0 0 1,-1-1 0,0 0 0,1 0 0,-1 0 0,-1-1 0,1 1 0,-1-1-1,0 0 1,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,1-7-1,1-1-338,-1 0 0,-1-1 0,0 1 0,0-19 0,-5-21 1704,-4 40 3752,0 22-1920,-3 28-1212,9-29-1573,-1 13 251,0 1 0,2 0 0,0 0-1,1 0 1,4 21 0,-4-38-483,0 1 0,0-1 0,0 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,0 1-1,0-1 1,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,1 0 0,8 1 0,0 0-926,0-1 0,0-1-1,0 0 1,0-1 0,0 0 0,23-6-1,-32 6 826,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-7 0,0 9 444,0-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 1-1,-1-1 1,1 1 0,0 0 0,0-1 0,-1 1 0,1 0-1,0 0 1,0 0 0,-1-1 0,1 1 0,0 1-1,-1-1 1,-1 0 0,1 0-165,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,0 1 1,1-1 0,-1 0-1,1 1 1,-1-1-1,-1 3 1,3-3-85,-1 0-1,1 0 1,-1 0 0,0 1 0,1-1 0,0 0-1,-1 0 1,1 1 0,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,1-1 0,-1 0 0,1 0-1,-1 1 1,1 0 0,0-1-35,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,2-1 0,3-1-84,1 0-1,0-1 1,0 0-1,-1 0 1,0 0-1,12-9 1,23 62 3272,-38-48-3159,0 1 0,1-1 0,-1 1 0,1-1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,1 0 0,-1-1 0,0 1 0,0-1-1,0 0 1,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1-4 0,5-19-433,-2 0 1,-2 0-1,0-1 1,-2-52-1,-1 62 857,-14 65 1661,9-6-1510,3 1-1,3 42 1,0-66-943,1 0-1,1 0 1,1 0 0,6 18-1,3-12-2022,2-15-4268,-8-9 1663</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2150.22">1502 173 6931,'0'0'8943,"6"-2"-8796,14-3-252,0 1 0,1 1 0,-1 1 0,0 1 0,1 0 0,-1 2 0,27 4 1,34-1-2056,-62-3 1542,-14 0 318,1 0-1,-1-1 1,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1-1 1,8-3-1,-12 0 3218,-11 1-1789,-12 4-221,17 0-821,1 0 1,-1 1 0,0-1 0,1 1 0,-1 0-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1-1,0 1 1,1-1 0,-1 0 0,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,1 0 0,-2 8 0,3-13-104,1 1 1,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1 0,1 1-1,1 0 1,0 0-35,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 1,-1-1-1,1 0 0,2-2 0,-2 0 31,1 0 0,-1 1 0,0-1 0,0 0 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0-6 0,24 77 1362,-23-63-1423,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,6 4 0,-6-5-521,0 0 0,1 0 0,-1-1 0,0 1-1,1-1 1,-1 0 0,1 0 0,5 0 0,18 0-4862</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2150.21">1502 173 6931,'0'0'8943,"6"-2"-8796,14-3-252,0 1 0,1 1 0,-1 1 0,0 1 0,1 0 0,-1 2 0,27 4 1,34-1-2056,-62-3 1542,-14 0 318,1 0-1,-1-1 1,1 0-1,-1 0 1,1 0-1,-1-1 1,1 1-1,-1-1 1,8-3-1,-12 0 3218,-11 1-1789,-12 4-221,17 0-821,1 0 1,-1 1 0,0-1 0,1 1 0,-1 0-1,1 1 1,0-1 0,0 1 0,0-1 0,0 1-1,0 1 1,1-1 0,-1 0 0,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,1 0 0,-2 8 0,3-13-104,1 1 1,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1 0,1 1-1,1 0 1,0 0-35,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 1,-1-1-1,1 0 0,2-2 0,-2 0 31,1 0 0,-1 1 0,0-1 0,0 0 0,-1 0 1,1 0-1,-1-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0-6 0,24 77 1362,-23-63-1423,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,6 4 0,-6-5-521,0 0 0,1 0 0,-1-1 0,0 1-1,1-1 1,-1 0 0,1 0 0,5 0 0,18 0-4862</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3565.23">2150 65 12230,'0'0'4599,"-2"12"-3609,-1 9-769,1-1 1,1 1-1,1 0 1,1 0-1,1 0 0,6 32 1,-1-34-254,4 30-1598,-12-71-1545,-11-14 2424,9 30 1244,0 0-1,1 0 1,0 0-1,1-1 1,-1 1 0,0-11-1,30 15 309,79-4-1009,-97 5 47,0-1-1,1 0 1,-1-1 0,0 0 0,0-1 0,0 0 0,17-9 0,-28 13 192,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 0 0,-1 1-1,1-1 1,0 0 0,-1 1 0,1-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,1-1 0,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 1 0,1-1-1,-3 1-22,0 1-1,1-1 1,-1 1-1,0 0 1,1-1-1,-1 1 1,1 0-1,0-1 0,-1 1 1,1 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,2 2 0,-1-1-26,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,0 1-1,-1-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,3 0-1,-2 1 12,0-1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1-1 1,1 0-1,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 1,0 1-1,1-4 0,1 2 24,-3 3-12,0-1 1,1 0-1,-1 1 1,0-1-1,1 0 0,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 0,0 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 1,-1 1-1,1-1 0,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,0 0 0,1-1 1,-1 2-1,18 39 27,-16-36-14,9 26 32,-1 0 0,-1 0-1,-2 1 1,-1 0-1,3 55 1,-9-84-47,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1-1-1,0 1 1,0 0-1,0 0 1,-1-1-1,1 0 1,0 1-1,-1-1 0,0 0 1,1 0-1,-5 2 1,3-2 29,-1 0 1,1 0 0,0 0-1,-1 0 1,1-1-1,-1 0 1,1 0 0,-1 0-1,1-1 1,-1 1-1,0-1 1,1 0-1,-1-1 1,0 1 0,1-1-1,-6-1 1,9 1-7,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,1-1-1,-1 1 0,0 0 1,1-1-1,-1 1 0,1-1 0,0 1 1,-1-1-1,1 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-2-1,3-42-51,2 30-390,1 0 0,0 1 0,0-1 0,2 1-1,0 1 1,0 0 0,1 0 0,1 0 0,14-14 0,19-28-3744,-23 26 861,23-44 0,-22 18 4539,-13-5 8645,-8 78-9012,-4 15-412,2 0 0,2 0 0,0 0 0,3 0 1,0 0-1,15 58 0,-14-75-394,9 21 173,-12-36-158,-1-40 617,0 29-694,0 0 0,1 0-1,0 0 1,1 1-1,0-1 1,5-16-1,-6 24-6,0-1-1,1 0 1,-1 1-1,0-1 0,1 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 1,-1 0-1,4 0 0,-4 0-1,-1-1 0,1 2 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,1 0 0,-1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-2 3 0,-2 0 10,1-1 0,0 0 0,-1 0 0,0 0 0,1-1 1,-1 1-1,0-1 0,0 0 0,0 0 0,-1-1 1,1 1-1,0-1 0,-1 0 0,1 0 0,-6 1 0,28-21-1700,36-13-432,-44 28 1868,-1-1 0,0 0-1,-1 0 1,1-1 0,-1 0-1,0 0 1,-1-1 0,1 0-1,-1 0 1,9-14 0,-14 19 256,-1 0 1,0 0-1,0-1 1,-1 1-1,1 0 1,0-1 0,-1 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,-1-1-1,1 1 1,-1 0-1,0-3 1,0 4 51,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 1 1,0-1-1,-3 1 0,2 1-14,0-1 1,1 1-1,-1-1 0,0 1 0,1 0 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 0 0,0 1 0,-1-1 1,1 0-1,0 1 0,0 2 0,0 2 54,-1 0-1,1 1 1,1-1-1,-1 0 1,1 1-1,2 7 0,-1-11-54,0-1-1,0 0 0,0 1 0,0-1 0,0 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,1-1 0,-1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,0-1 0,-1 1 0,6 0 1,36 5-1435,-3-8-4607,-27-3-1468</inkml:trace>
 </inkml:ink>
 </file>
@@ -9966,7 +9966,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="342.74">240 2 8820,'0'0'7163,"0"-1"-7147,1 1 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 1,1-1-1,-1 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,5 4 17,-1-1 0,-1 1 0,1 0 0,-1 1 0,1-1 0,-2 1 0,1 0 0,-1 0 0,1 0 0,-2 1 0,1-1 0,-1 1 0,2 7 0,-6-12 35,-1 0 0,1 0 0,-1 0 1,0-1-1,1 1 0,-1-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 1,-5 1-1,0 1 11,4-1-568,-34 11 1667,20-3-2998,10 1-5720</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.21">591 47 2513,'0'0'12574,"-1"7"-11435,-7 29 2,3-9-348,0 0-1,-1 31 1,6-57-996</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="883.93">586 50 8516,'0'0'8916,"2"13"-8228,-2-8-987,2 6 632,-1-1-1,1 1 1,1-1-1,0 0 0,7 17 1,-8-24-410,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,4 2 0,-3-3-474,-1 0 0,0 0 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,7-1 0,-6-1-3723</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1123.39">706 22 2961,'0'0'13233,"0"12"-12166,-6 33 304,1-10-1833,-1 45-1,21-78-8987,-2-2 3978</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1123.38">706 22 2961,'0'0'13233,"0"12"-12166,-6 33 304,1-10-1833,-1 45-1,21-78-8987,-2-2 3978</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2462.97">849 112 944,'0'0'6307,"-4"-31"2006,2 29-8205,-1 1-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,0 0 0,-4 3 0,5-3-57,0 1 0,0 0 0,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,1 1 0,-1-1 0,1 0 0,0 1-1,-1-1 1,1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,1 0 0,0 3 0,0-4-40,0 0 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 1,0-1-1,0-1 0,0 1 0,3-1 1,-1 2-51,-1-1 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,3-3 0,3-9-7,-1 0 110,-11 31-15,2-16-50,0 1-1,1-1 1,-1 1 0,1-1-1,0 1 1,-1 0 0,1-1-1,0 1 1,0 0-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,1 2-1,0-3-35,-1-1-1,0 1 1,1-1 0,-1 1-1,1-1 1,-1 0-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1 0,0 0-1,-1 0 1,1 0-1,0 1 1,-1-1 0,1 0-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0-1-1,3 1-64,-1-1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,0-1 0,-1 1 0,5-5 0,-6 6 125,-1 1 0,0-1-1,1 1 1,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,0-1 0,1 1 0,4 11 719,-5 29 567,-1-32-1182,1-7-116,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0 0,1 0-1,0 0 1,-1 1 0,1-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,-1 0-1,1 0 1,-1-1 0,2 0 0,18-8 8,-15 7-35,2-3-66,0 0-1,1 0 1,-1 1 0,1 0 0,0 1 0,1 0 0,-1 0 0,0 1 0,1 0 0,13-2 0,-21 5 87,-1-1 1,1 0-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,1 1 0,4-1-212,-1 1 0,0-1 0,1-1 1,-1 1-1,0-1 0,1 1 0,-1-2 1,0 1-1,0 0 0,0-1 0,0 0 1,0 0-1,0-1 0,-1 0 0,7-4 1,-10 7 277,0 0 1,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0-1,0 0 1,1 1 0,4 7 16,-3-7-94,1-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,-1 1 0,1-1 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-5 0,-1 6 19,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,1-1-1,-1 0 1,-2-1-1,2 2 36,0 0 0,-1-1 0,1 1 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 1,-1 1-1,1 0 0,0-1 0,-1 1 0,1 0 0,-2 1 0,-1 1 73,0 1-1,0-1 1,0 1-1,0 0 1,1 0 0,-1 0-1,-4 9 1,6-11-114,1 1 1,0-1-1,-1 0 1,1 1-1,0-1 1,1 1-1,-1-1 0,0 1 1,1-1-1,-1 1 1,1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,1-1-1,-1 1 0,1 2 1,0-4-88,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 1,-1 0-1,1 1 0,2-1 0,35 1-3255,-34-1 2384,23 0-5711</inkml:trace>
 </inkml:ink>
 </file>
@@ -10328,7 +10328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18BF21D-57E0-4D00-AE55-6E595DDCBE16}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -10381,28 +10381,28 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
@@ -10435,10 +10435,10 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -10457,8 +10457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D2DFA3-BBAA-4C10-A752-A9713912B3F4}">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B21"/>
+    <sheetView topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10530,349 +10530,349 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A48436-A956-4B55-81B5-4A697FFE44EE}">
   <dimension ref="O7:X39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36:O39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="7" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="8" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="3" t="s">
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="6"/>
     </row>
     <row r="9" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O9" s="6"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="9"/>
     </row>
     <row r="10" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O10" s="6"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="8"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="9"/>
     </row>
     <row r="11" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O11" s="6"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="8"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="9"/>
     </row>
     <row r="12" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O12" s="6"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="8"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="9"/>
     </row>
     <row r="13" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O13" s="6"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="8"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="9"/>
     </row>
     <row r="14" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O14" s="6"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="8"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="9"/>
     </row>
     <row r="15" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O15" s="6"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="8"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="9"/>
     </row>
     <row r="16" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="O16" s="9"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="11"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="12"/>
     </row>
     <row r="17" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="18" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O18" s="12" t="s">
+      <c r="O18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="3" t="s">
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="6"/>
     </row>
     <row r="19" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O19" s="15"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="8"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="9"/>
     </row>
     <row r="20" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O20" s="15"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="8"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="9"/>
     </row>
     <row r="21" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O21" s="15"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="8"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="9"/>
     </row>
     <row r="22" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="O22" s="18"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="11"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="12"/>
     </row>
     <row r="23" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="3" t="s">
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="6"/>
     </row>
     <row r="24" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O24" s="6"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="8"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="9"/>
     </row>
     <row r="25" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O25" s="6"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="8"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="9"/>
     </row>
     <row r="26" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O26" s="6"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="8"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="9"/>
     </row>
     <row r="27" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="O27" s="9"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="11"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="12"/>
     </row>
     <row r="28" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O28" s="3" t="s">
+      <c r="O28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="3" t="s">
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="6"/>
     </row>
     <row r="29" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O29" s="6"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="8"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="9"/>
     </row>
     <row r="30" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O30" s="6"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="8"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="9"/>
     </row>
     <row r="31" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O31" s="6"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="8"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="9"/>
     </row>
     <row r="32" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O32" s="6"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="8"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="9"/>
     </row>
     <row r="33" spans="15:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="O33" s="9"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="9" t="s">
+      <c r="O33" s="10"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="12"/>
     </row>
     <row r="36" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O36" s="21" t="s">
+      <c r="O36" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O37" s="21" t="s">
+      <c r="O37" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O38" s="21" t="s">
+      <c r="O38" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" spans="15:24" x14ac:dyDescent="0.45">
-      <c r="O39" s="21" t="s">
+      <c r="O39" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -10897,8 +10897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23ECABD-6903-4E21-A69C-B1641E9D1A3E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>